<commit_message>
Neues Excel-Tool nach Anpassung MoVe- und DVAG-Provisionen
</commit_message>
<xml_diff>
--- a/ExcelBlanko.xlsx
+++ b/ExcelBlanko.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\oneLine_Backoffice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\V\DATEN\BN_BSS11\T_PRO_PKG\Performance\DB Verprobung\Vertriebstool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F2EDC7A-DA90-4029-9294-CD5030BA7518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="QV38z4XmEvP8epS8iL+DBd/fDI6DPwUt6dqz4ds4POUcSf+ob5trf1LoOzg+RQYpyxLPCmIPlrdkm3z9IgO1Dg==" workbookSaltValue="l5I7Gq32r5XB3f3EfH79gQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{07A89781-C5D2-4FF0-9952-8938F62F6B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="wJFlHBhF99Wnc1g+0/u0ACNiHmTzjlFIDlICnHtkYn+yyomZ0UkjA+fw9BBXroFt6P8XaPp63Hl6G4XiQVn7hg==" workbookSaltValue="h86qGiaJ/emgajeOgOUvCw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="814" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="814" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Startseite" sheetId="15" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="244">
   <si>
     <t>MOVE</t>
   </si>
@@ -661,16 +661,7 @@
     <t>Restliche Vertragslaufzeit in Monaten</t>
   </si>
   <si>
-    <t>Die ermittelten Wertbeiträge stellen eine Approximation des über den FiKo (Produktkalkulator) berechneten Wertbeitrags dar.</t>
-  </si>
-  <si>
     <t>Nach Eingabe der preisbestimmenden Parameter wird Ihnen der Wertbeitrag zur KIZ Zielkondition und zur vereinbarten Kondition angezeigt.</t>
-  </si>
-  <si>
-    <t>Marginale Abweichungen (&lt; 1 %) sind möglich.</t>
-  </si>
-  <si>
-    <t>Der zur Ermittlung der maximalen Konditionskompetenz herangezogene Wertbeitrag weicht von dem hier dargestellten Wertebeitrag ab.</t>
   </si>
   <si>
     <t>Eingabe der Marge des Altkredits</t>
@@ -997,10 +988,92 @@
     <t>Bei diesem Gesamtkreditbetrag wird die nächste 10%-Schwelle als Absicherungsmöglichkeit erreicht.</t>
   </si>
   <si>
-    <t>Gültig ab 16.12.2022</t>
+    <t>Der zur Ermittlung der maximalen Konditionskompetenz herangezogene Wertbeitrag weicht von dem hier dargestellten Wertbeitrag ab.</t>
   </si>
   <si>
-    <t>Der zur Ermittlung der maximalen Konditionskompetenz herangezogene Wertbeitrag weicht von dem hier dargestellten Wertbeitrag ab.</t>
+    <t>Bitte beachten Sie das das Kalkulationstool nur eine indikative Berechnung des Wertbeitrages vornimmt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insbesondere bei Aufstockungen sind größere Abweichungen zwischen dem Wertbeitrag im Kalkulationstool und dem Wertbeitrag im FilialKompass leider technisch nicht auszuschließen. </t>
+  </si>
+  <si>
+    <t>Je geringer der Aufstockungsbetrag und je länger die Restlaufzeit des Altkredites, desto höher ist die Abweichung.</t>
+  </si>
+  <si>
+    <t>Gültig ab 18.01.2023</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Insbesondere </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bei Aufstockungen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sind </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>größere Abweichungen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zwischen dem Wertbeitrag im Kalkulationstool und dem Wertbeitrag im FilialKompass leider technisch nicht auszuschließen. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bitte beachten Sie das das Kalkulationstool nur eine </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>indikative Berechnung des Wertbeitrages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> vornimmt.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2785,15 +2858,6 @@
     <xf numFmtId="0" fontId="16" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2812,7 +2876,16 @@
     <xf numFmtId="0" fontId="18" fillId="37" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6451,7 +6524,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -6532,12 +6605,12 @@
         <v>70</v>
       </c>
       <c r="C10" s="90" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="PE92VI+ommGNYJjtpg/9xK5fQzN2k8omOoSjW9KG7l0i5VDYEQ5CQTtpCGqkcdDBx+y+1VAc0nuyzNQh8g+mRw==" saltValue="j4QSEzBhuKGfuJxGkWqGNw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="temSBCYz7mahSiJ39Bf+V4by9SgkBbWNcvxxbwnu8Gb9qG1rc6GIvGPPKmmqNuGA67OpkWjJRCIaFmBhkNrzBg==" saltValue="wMLFQPrQDycciyUax63Oug==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -6562,12 +6635,12 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B2">
         <f>'Bewertung Aufstockung'!B6</f>
@@ -6576,7 +6649,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B3">
         <f>'Bewertung Aufstockung'!B6-Wertbeitrag!C11</f>
@@ -6585,7 +6658,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B4">
         <v>0.88</v>
@@ -6593,7 +6666,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B5" s="231">
         <v>0.55000000000000004</v>
@@ -6601,7 +6674,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B6" s="232">
         <f>'Bewertung Aufstockung'!B5</f>
@@ -6610,7 +6683,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B7" s="233" t="e">
         <f>(B2-B3)*(B2-B3+1)/B2/(B2+1)*B4*B6*B5</f>
@@ -6619,10 +6692,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C26" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -6633,7 +6706,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B27" s="240">
         <f>2.3%+C27+D27+E27</f>
@@ -6667,7 +6740,7 @@
   <dimension ref="A3:AB139"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7289,7 +7362,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C12" s="218" t="e">
         <f>C7-(C11/10000)</f>
@@ -7659,11 +7732,11 @@
         <v>148</v>
       </c>
       <c r="B18" s="120">
-        <f>IF(Kalk_Kredit2!D13="MoVe",0.85,1)</f>
+        <f>IF(Kalk_Kredit2!D13="MoVe",0.75,1)</f>
         <v>1</v>
       </c>
       <c r="C18" s="120">
-        <f>IF(Kalk_Kredit2!D13="MoVe",0.85,1)</f>
+        <f>IF(Kalk_Kredit2!D13="MoVe",0.75,1)</f>
         <v>1</v>
       </c>
       <c r="F18" s="1">
@@ -7726,11 +7799,11 @@
         <v>5</v>
       </c>
       <c r="B19" s="1">
-        <f>IF(Kalk_Kredit2!D13="DVAG",3%*'Bg WB vereinb_Kredit2'!C5,0)</f>
+        <f>IF(Kalk_Kredit2!D13="DVAG",3.5%*'Bg WB vereinb_Kredit2'!C5,0)</f>
         <v>0</v>
       </c>
       <c r="C19" s="1">
-        <f>IF(Kalk_Kredit2!D13="DVAG",3%*'Bg WB vereinb_Kredit2'!R5,0)</f>
+        <f>IF(Kalk_Kredit2!D13="DVAG",3.5%*'Bg WB vereinb_Kredit2'!R5,0)</f>
         <v>0</v>
       </c>
       <c r="F19" s="1">
@@ -14542,8 +14615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F271BF23-5F64-4067-8786-917566CE8028}">
   <dimension ref="A3:AB139"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15162,7 +15235,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C12" s="218" t="e">
         <f>C7-(C11/10000)</f>
@@ -15532,11 +15605,11 @@
         <v>148</v>
       </c>
       <c r="B18" s="120">
-        <f>IF(Kalk_Kredit2!D13="MoVe",0.85,1)</f>
+        <f>IF(Kalk_Kredit2!D13="MoVe",0.75,1)</f>
         <v>1</v>
       </c>
       <c r="C18" s="120">
-        <f>IF(Kalk_Kredit2!D13="MoVe",0.85,1)</f>
+        <f>IF(Kalk_Kredit2!D13="MoVe",0.75,1)</f>
         <v>1</v>
       </c>
       <c r="F18" s="1">
@@ -15599,11 +15672,11 @@
         <v>5</v>
       </c>
       <c r="B19" s="1">
-        <f>IF(Kalk_Kredit2!D13="DVAG",3%*'Bg Produktkalk I_Kredit2'!C5,0)</f>
+        <f>IF(Kalk_Kredit2!D13="DVAG",3.5%*'Bg Produktkalk I_Kredit2'!C5,0)</f>
         <v>0</v>
       </c>
       <c r="C19" s="1">
-        <f>IF(Kalk_Kredit2!D13="DVAG",3%*'Bg Produktkalk I_Kredit2'!R5,0)</f>
+        <f>IF(Kalk_Kredit2!D13="DVAG",3.5%*'Bg Produktkalk I_Kredit2'!R5,0)</f>
         <v>0</v>
       </c>
       <c r="F19" s="1">
@@ -22547,25 +22620,25 @@
       </c>
       <c r="V3" s="266"/>
       <c r="W3" s="266"/>
-      <c r="AB3" s="268" t="s">
+      <c r="AB3" s="273" t="s">
         <v>87</v>
       </c>
-      <c r="AC3" s="268"/>
-      <c r="AD3" s="268"/>
+      <c r="AC3" s="273"/>
+      <c r="AD3" s="273"/>
       <c r="AE3" s="108"/>
       <c r="AF3" s="108"/>
-      <c r="AI3" s="268" t="s">
+      <c r="AI3" s="273" t="s">
         <v>87</v>
       </c>
-      <c r="AJ3" s="268"/>
-      <c r="AK3" s="268"/>
+      <c r="AJ3" s="273"/>
+      <c r="AK3" s="273"/>
       <c r="AL3" s="108"/>
       <c r="AM3" s="108"/>
-      <c r="AS3" s="268" t="s">
+      <c r="AS3" s="273" t="s">
         <v>87</v>
       </c>
-      <c r="AT3" s="268"/>
-      <c r="AU3" s="268"/>
+      <c r="AT3" s="273"/>
+      <c r="AU3" s="273"/>
       <c r="AV3" s="108"/>
       <c r="AW3" s="108"/>
     </row>
@@ -22598,24 +22671,24 @@
         <f>Kalk_Kredit2!D10</f>
         <v>0</v>
       </c>
-      <c r="AB4" s="269" t="s">
+      <c r="AB4" s="274" t="s">
         <v>89</v>
       </c>
-      <c r="AC4" s="269"/>
+      <c r="AC4" s="274"/>
       <c r="AD4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AI4" s="269" t="s">
+      <c r="AI4" s="274" t="s">
         <v>91</v>
       </c>
-      <c r="AJ4" s="269"/>
+      <c r="AJ4" s="274"/>
       <c r="AK4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AS4" s="269" t="s">
+      <c r="AS4" s="274" t="s">
         <v>91</v>
       </c>
-      <c r="AT4" s="269"/>
+      <c r="AT4" s="274"/>
       <c r="AU4" s="1" t="s">
         <v>90</v>
       </c>
@@ -22630,7 +22703,7 @@
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="270" t="s">
+      <c r="H5" s="267" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="124">
@@ -22690,7 +22763,7 @@
       <c r="B6" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="271"/>
+      <c r="H6" s="268"/>
       <c r="I6" s="124">
         <v>5.01</v>
       </c>
@@ -22770,7 +22843,7 @@
       <c r="B7" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="271"/>
+      <c r="H7" s="268"/>
       <c r="I7" s="124">
         <v>10.01</v>
       </c>
@@ -22855,7 +22928,7 @@
       <c r="D8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="271"/>
+      <c r="H8" s="268"/>
       <c r="I8" s="124">
         <v>15.01</v>
       </c>
@@ -22931,7 +23004,7 @@
       <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="271"/>
+      <c r="H9" s="268"/>
       <c r="I9" s="124">
         <v>20.010000000000002</v>
       </c>
@@ -23007,7 +23080,7 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="H10" s="271"/>
+      <c r="H10" s="268"/>
       <c r="I10" s="124">
         <v>30.01</v>
       </c>
@@ -23087,7 +23160,7 @@
       <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="H11" s="271"/>
+      <c r="H11" s="268"/>
       <c r="I11" s="124">
         <v>40.01</v>
       </c>
@@ -23102,7 +23175,7 @@
         <v>22</v>
       </c>
       <c r="O11" s="202" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="P11" s="203" t="e">
         <f ca="1">LOOKUP(Wertbeitrag(Kalk_Kredit2!D10,Kalk_Kredit2!D9,Kalk_Kredit2!D8,(((((Kalk_Kredit2!D20+1)^(1/12))-1)*12)),Kalk_Kredit2!D14/10000,Kalk_Kredit2!D7,PMT((((Kalk_Kredit2!D20+1)^(1/12)-1)),Kalk_Kredit2!D8,-Kalk_Kredit2!D10),IF(Kalk_Kredit2!D9-Kalk_Kredit2!D8&gt;3,1,0),Kalk_Kredit2!D13)/Kalk_Kredit2!D10,Background2!I65:I70,Background2!K65:K70)/100</f>
@@ -23187,7 +23260,7 @@
       <c r="D12" s="1">
         <v>3</v>
       </c>
-      <c r="H12" s="271"/>
+      <c r="H12" s="268"/>
       <c r="I12" s="124">
         <v>50.01</v>
       </c>
@@ -23200,7 +23273,7 @@
       </c>
       <c r="N12" s="278"/>
       <c r="O12" s="207" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="P12" s="208" t="str">
         <f>IF(ISNUMBER(P17),IF(Kalk_Kredit2!$D$8&gt;84,Background2!P14,Background2!P13),"")</f>
@@ -23274,7 +23347,7 @@
       <c r="B13" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="271"/>
+      <c r="H13" s="268"/>
       <c r="I13" s="124">
         <v>60.01</v>
       </c>
@@ -23287,7 +23360,7 @@
       </c>
       <c r="N13" s="278"/>
       <c r="O13" s="29" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="P13" s="210" t="e">
         <f>LOOKUP($P$17,Background2!I65:I70,Background2!K65:K70)/100</f>
@@ -23353,7 +23426,7 @@
       <c r="B14" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="271"/>
+      <c r="H14" s="268"/>
       <c r="I14" s="124">
         <v>70.010000000000005</v>
       </c>
@@ -23366,7 +23439,7 @@
       </c>
       <c r="N14" s="279"/>
       <c r="O14" s="196" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="P14" s="206" t="e">
         <f>LOOKUP($P$17,Background2!N65:N70,Background2!O65:O70)/100</f>
@@ -23443,7 +23516,7 @@
         <v>44</v>
       </c>
       <c r="D15" s="99"/>
-      <c r="H15" s="271"/>
+      <c r="H15" s="268"/>
       <c r="I15" s="124">
         <v>80.010000000000005</v>
       </c>
@@ -23524,7 +23597,7 @@
       <c r="B16" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="271"/>
+      <c r="H16" s="268"/>
       <c r="I16" s="124">
         <v>90.01</v>
       </c>
@@ -23602,7 +23675,7 @@
       <c r="B17" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="271"/>
+      <c r="H17" s="268"/>
       <c r="I17" s="124">
         <v>100.01</v>
       </c>
@@ -23685,7 +23758,7 @@
       <c r="B18" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="271"/>
+      <c r="H18" s="268"/>
       <c r="I18" s="124">
         <v>125.01</v>
       </c>
@@ -23763,7 +23836,7 @@
       <c r="B19" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="271"/>
+      <c r="H19" s="268"/>
       <c r="I19" s="124">
         <v>150.01</v>
       </c>
@@ -23835,7 +23908,7 @@
       <c r="B20" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="271"/>
+      <c r="H20" s="268"/>
       <c r="I20" s="125">
         <v>175.01</v>
       </c>
@@ -23861,7 +23934,7 @@
       <c r="B21" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="H21" s="271"/>
+      <c r="H21" s="268"/>
       <c r="I21" s="125">
         <v>200.01</v>
       </c>
@@ -23882,27 +23955,27 @@
         <f>W6+V16</f>
         <v>0</v>
       </c>
-      <c r="AA21" s="269" t="s">
+      <c r="AA21" s="274" t="s">
         <v>105</v>
       </c>
-      <c r="AB21" s="269"/>
+      <c r="AB21" s="274"/>
       <c r="AC21" s="1">
         <f>LOOKUP(V16,AA5:AA13,AD5:AD13)</f>
         <v>0</v>
       </c>
-      <c r="AH21" s="269" t="s">
+      <c r="AH21" s="274" t="s">
         <v>106</v>
       </c>
-      <c r="AI21" s="269"/>
+      <c r="AI21" s="274"/>
       <c r="AJ21" s="1">
         <f>IF(ISERROR(LOOKUP(V18,AH5:AH17,AK5:AK17)),0,LOOKUP(V18,AH5:AH17,AK5:AK17))</f>
         <v>0</v>
       </c>
       <c r="AO21" s="76"/>
-      <c r="AR21" s="269" t="s">
+      <c r="AR21" s="274" t="s">
         <v>106</v>
       </c>
-      <c r="AS21" s="269"/>
+      <c r="AS21" s="274"/>
       <c r="AT21" s="1">
         <f>IF(ISERROR(LOOKUP(V18,AR5:AR17,AU5:AU17)),0,LOOKUP(V18,AR5:AR17,AU5:AU17))</f>
         <v>0</v>
@@ -23916,7 +23989,7 @@
       <c r="B22" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="271"/>
+      <c r="H22" s="268"/>
       <c r="I22" s="125">
         <v>250.01</v>
       </c>
@@ -23959,7 +24032,7 @@
       <c r="A23" s="52">
         <v>999</v>
       </c>
-      <c r="H23" s="271"/>
+      <c r="H23" s="268"/>
       <c r="I23" s="125">
         <v>300.01</v>
       </c>
@@ -23987,7 +24060,7 @@
       </c>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H24" s="271"/>
+      <c r="H24" s="268"/>
       <c r="I24" s="126">
         <v>350.01</v>
       </c>
@@ -24006,7 +24079,7 @@
       </c>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H25" s="271"/>
+      <c r="H25" s="268"/>
       <c r="I25" s="126">
         <v>400.01</v>
       </c>
@@ -24023,34 +24096,34 @@
         <f>AZ29+AT22</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA25" s="276" t="s">
+      <c r="AA25" s="275" t="s">
         <v>107</v>
       </c>
-      <c r="AB25" s="276"/>
-      <c r="AC25" s="276"/>
-      <c r="AD25" s="276"/>
-      <c r="AE25" s="276"/>
-      <c r="AF25" s="276"/>
-      <c r="AH25" s="267" t="s">
+      <c r="AB25" s="275"/>
+      <c r="AC25" s="275"/>
+      <c r="AD25" s="275"/>
+      <c r="AE25" s="275"/>
+      <c r="AF25" s="275"/>
+      <c r="AH25" s="276" t="s">
         <v>108</v>
       </c>
-      <c r="AI25" s="267"/>
-      <c r="AJ25" s="267"/>
-      <c r="AK25" s="267"/>
-      <c r="AL25" s="267"/>
-      <c r="AM25" s="267"/>
-      <c r="AN25" s="267"/>
-      <c r="AO25" s="267"/>
-      <c r="AR25" s="267" t="s">
+      <c r="AI25" s="276"/>
+      <c r="AJ25" s="276"/>
+      <c r="AK25" s="276"/>
+      <c r="AL25" s="276"/>
+      <c r="AM25" s="276"/>
+      <c r="AN25" s="276"/>
+      <c r="AO25" s="276"/>
+      <c r="AR25" s="276" t="s">
         <v>108</v>
       </c>
-      <c r="AS25" s="267"/>
-      <c r="AT25" s="267"/>
-      <c r="AU25" s="267"/>
-      <c r="AV25" s="267"/>
-      <c r="AW25" s="267"/>
-      <c r="AX25" s="267"/>
-      <c r="AY25" s="267"/>
+      <c r="AS25" s="276"/>
+      <c r="AT25" s="276"/>
+      <c r="AU25" s="276"/>
+      <c r="AV25" s="276"/>
+      <c r="AW25" s="276"/>
+      <c r="AX25" s="276"/>
+      <c r="AY25" s="276"/>
     </row>
     <row r="26" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H26" s="238"/>
@@ -24102,7 +24175,7 @@
       <c r="AY26" s="239"/>
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H27" s="272" t="s">
+      <c r="H27" s="269" t="s">
         <v>9</v>
       </c>
       <c r="I27" s="101">
@@ -24129,7 +24202,7 @@
       </c>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H28" s="273"/>
+      <c r="H28" s="270"/>
       <c r="I28" s="102">
         <v>9.9999999999999995E-7</v>
       </c>
@@ -24160,7 +24233,7 @@
       </c>
     </row>
     <row r="29" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H29" s="273"/>
+      <c r="H29" s="270"/>
       <c r="I29" s="102">
         <v>0.20000100000000001</v>
       </c>
@@ -24190,7 +24263,7 @@
       </c>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H30" s="273"/>
+      <c r="H30" s="270"/>
       <c r="I30" s="102">
         <v>0.400001</v>
       </c>
@@ -24296,7 +24369,7 @@
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H31" s="273"/>
+      <c r="H31" s="270"/>
       <c r="I31" s="102">
         <v>0.60000100000000001</v>
       </c>
@@ -24402,7 +24475,7 @@
       </c>
     </row>
     <row r="32" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H32" s="274"/>
+      <c r="H32" s="271"/>
       <c r="I32" s="103">
         <v>0.80000099999999996</v>
       </c>
@@ -24511,7 +24584,7 @@
       </c>
     </row>
     <row r="33" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H33" s="271" t="s">
+      <c r="H33" s="268" t="s">
         <v>17</v>
       </c>
       <c r="I33" s="104">
@@ -24625,7 +24698,7 @@
       </c>
     </row>
     <row r="34" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H34" s="271"/>
+      <c r="H34" s="268"/>
       <c r="I34" s="104">
         <v>0.20000100000000001</v>
       </c>
@@ -24737,7 +24810,7 @@
       </c>
     </row>
     <row r="35" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H35" s="271"/>
+      <c r="H35" s="268"/>
       <c r="I35" s="104">
         <v>0.400001</v>
       </c>
@@ -24849,7 +24922,7 @@
       </c>
     </row>
     <row r="36" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H36" s="271"/>
+      <c r="H36" s="268"/>
       <c r="I36" s="104">
         <v>0.60000100000000001</v>
       </c>
@@ -24961,7 +25034,7 @@
       </c>
     </row>
     <row r="37" spans="8:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H37" s="275"/>
+      <c r="H37" s="272"/>
       <c r="I37" s="104">
         <v>0.80000099999999996</v>
       </c>
@@ -27733,14 +27806,14 @@
     </row>
     <row r="63" spans="8:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H63" s="24" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I63" s="24"/>
       <c r="J63" s="24"/>
       <c r="K63" s="24"/>
       <c r="L63" s="24"/>
       <c r="N63" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AA63" s="1">
         <f t="shared" si="17"/>
@@ -37485,6 +37558,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="AH2:AO2"/>
+    <mergeCell ref="AR2:AY2"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AI3:AK3"/>
+    <mergeCell ref="AS3:AU3"/>
     <mergeCell ref="AR25:AY25"/>
     <mergeCell ref="H27:H32"/>
     <mergeCell ref="H33:H37"/>
@@ -37498,13 +37578,6 @@
     <mergeCell ref="AR21:AS21"/>
     <mergeCell ref="AA25:AF25"/>
     <mergeCell ref="AH25:AO25"/>
-    <mergeCell ref="AA2:AF2"/>
-    <mergeCell ref="AH2:AO2"/>
-    <mergeCell ref="AR2:AY2"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AI3:AK3"/>
-    <mergeCell ref="AS3:AU3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -37523,7 +37596,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37546,7 +37619,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="71" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="70"/>
     </row>
@@ -37563,7 +37636,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I5" s="249" t="str">
         <f>+'Bewertung Aufstockung'!F27</f>
@@ -37572,7 +37645,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="250" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I6" s="120" t="e">
         <f>+ROUNDUP(I5,1)</f>
@@ -37581,7 +37654,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="250" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I7" s="251" t="e">
         <f>+IF(I6=0.8,I17,VLOOKUP(I6,G10:I18,3,1))</f>
@@ -37601,13 +37674,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G10" s="120">
         <v>0.1</v>
       </c>
       <c r="H10" s="243" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I10" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G10)-Kalkulationstool!$D$11</f>
@@ -37616,13 +37689,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="250" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G11" s="120">
         <v>0.2</v>
       </c>
       <c r="H11" s="243" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I11" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G11)-Kalkulationstool!$D$11</f>
@@ -37631,13 +37704,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="250" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G12" s="120">
         <v>0.3</v>
       </c>
       <c r="H12" s="243" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I12" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G12)-Kalkulationstool!$D$11</f>
@@ -37649,7 +37722,7 @@
         <v>0.4</v>
       </c>
       <c r="H13" s="243" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I13" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G13)-Kalkulationstool!$D$11</f>
@@ -37661,7 +37734,7 @@
         <v>0.5</v>
       </c>
       <c r="H14" s="243" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I14" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G14)-Kalkulationstool!$D$11</f>
@@ -37673,7 +37746,7 @@
         <v>0.6</v>
       </c>
       <c r="H15" s="243" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I15" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G15)-Kalkulationstool!$D$11</f>
@@ -37685,7 +37758,7 @@
         <v>0.7</v>
       </c>
       <c r="H16" s="243" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I16" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G16)-Kalkulationstool!$D$11</f>
@@ -37697,7 +37770,7 @@
         <v>0.8</v>
       </c>
       <c r="H17" s="243" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I17" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G17)-Kalkulationstool!$D$11</f>
@@ -37709,7 +37782,7 @@
         <v>0.9</v>
       </c>
       <c r="H18" s="243" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I18" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G18)-Kalkulationstool!$D$11</f>
@@ -37729,7 +37802,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I21" s="120" t="e">
         <f>+ROUNDDOWN(I5,1)</f>
@@ -37757,7 +37830,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -37799,7 +37872,7 @@
       <c r="G2" s="67"/>
       <c r="Q2" s="241"/>
       <c r="R2" s="242" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="5.0999999999999996" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37879,7 +37952,7 @@
       </c>
       <c r="G7" s="92"/>
       <c r="H7" s="93" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I7" s="82"/>
       <c r="J7" s="82"/>
@@ -38054,7 +38127,7 @@
       </c>
       <c r="G14" s="93"/>
       <c r="H14" s="93" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I14" s="82"/>
       <c r="J14" s="82"/>
@@ -38088,7 +38161,7 @@
       <c r="C19" s="82"/>
       <c r="D19" s="122">
         <f ca="1">NOW()</f>
-        <v>44909.854944212966</v>
+        <v>44943.655650231478</v>
       </c>
       <c r="E19" s="82"/>
       <c r="F19" s="82" t="s">
@@ -38120,7 +38193,7 @@
       <c r="F20" s="100"/>
       <c r="G20" s="82"/>
       <c r="H20" s="93" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I20" s="82"/>
       <c r="J20" s="82"/>
@@ -38258,7 +38331,7 @@
         <v/>
       </c>
       <c r="I26" s="91" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J26" s="82"/>
       <c r="K26" s="82"/>
@@ -38272,7 +38345,7 @@
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="iCFBxi0/PADkWcii3he9SJslmZnH25bIPU25iAHDhYsnHiCDQncI2teCMAPkNtf4xPnxqwv3cLmfUvo6I2TJfA==" saltValue="z9Y9iXlns4vlf8z+L1C9oQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+l00WxGYIb4qoYpIo+q8yM/EDAiBYPzCzE9uo+t51RK/AfveDAfilUXMFvymMd4E65wGTQ4Fi6Mm7LG9UiSfrg==" saltValue="kfULYYEAQWvItHAUy45niw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="D8" name="Range6"/>
     <protectedRange sqref="D19" name="Range5"/>
@@ -38375,7 +38448,7 @@
     <tabColor theme="4" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="B1:XFC23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -38389,7 +38462,8 @@
     <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="73" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="1" hidden="1"/>
+    <col min="7" max="16383" width="11.42578125" style="1" hidden="1"/>
+    <col min="16384" max="16384" width="21.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="19.5" x14ac:dyDescent="0.3">
@@ -38493,7 +38567,7 @@
       </c>
       <c r="E10" s="92"/>
       <c r="F10" s="93" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -38569,7 +38643,7 @@
     </row>
     <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D18" s="154"/>
       <c r="E18" s="154"/>
@@ -38577,7 +38651,7 @@
     </row>
     <row r="19" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>167</v>
+        <v>243</v>
       </c>
       <c r="D19" s="154"/>
       <c r="E19" s="154"/>
@@ -38585,7 +38659,7 @@
     </row>
     <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>169</v>
+        <v>242</v>
       </c>
       <c r="C20" s="154"/>
       <c r="D20" s="154"/>
@@ -38593,24 +38667,29 @@
       <c r="F20" s="154"/>
     </row>
     <row r="21" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="147" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B21" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="147" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Jj1zoi8LMXLSYvcOr16BoNanpoVrFp2wnknYXanWVjsQ4Igeu6u/Gd6Uzj4CFE2C8F2YYxLOMMZUh2NrIgbO6g==" saltValue="5ap8O8NGeDobDfCH0Zf81g==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="md4XruLI5VbWansdC0cUhfCj2E8GvTFvtOHiVRMXpotxVSGvewZQJNlssjDk5o9QrGjcMGXFlJ12mnnyClsgVg==" saltValue="7L5y2Fa82BHIlu9JX6JqnQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="C11" name="Range1"/>
   </protectedRanges>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" errorTitle="Bitte prüfen Sie die Eingaben!" error="Übernehmen Sie die Laufzeit aus KFPK. " sqref="C11" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
       <formula2>120</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="90" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="78" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K000000</oddFooter>
   </headerFooter>
@@ -38656,7 +38735,7 @@
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="71" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B2" s="70"/>
       <c r="C2" s="244"/>
@@ -38668,7 +38747,7 @@
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B3" s="70"/>
       <c r="C3" s="244"/>
@@ -38694,14 +38773,14 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="100" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B5" s="227"/>
       <c r="C5" s="228">
         <v>840</v>
       </c>
       <c r="D5" s="93" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E5" s="228"/>
       <c r="F5" s="93"/>
@@ -38709,14 +38788,14 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="100" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B6" s="165"/>
       <c r="C6" s="229">
         <v>91</v>
       </c>
       <c r="D6" s="93" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E6" s="229"/>
       <c r="F6" s="92"/>
@@ -38724,14 +38803,14 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="100" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B7" s="226"/>
       <c r="C7" s="230">
         <v>1</v>
       </c>
       <c r="D7" s="93" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E7" s="230"/>
       <c r="F7" s="92"/>
@@ -38742,22 +38821,22 @@
     <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="81"/>
       <c r="B10" s="237" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C10" s="237"/>
       <c r="D10" s="237" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E10" s="237"/>
       <c r="F10" s="237" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G10" s="81"/>
       <c r="H10" s="247"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="155" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B11" s="234" t="str">
         <f>IFERROR(+Wert_Kredit2!Wertbeitrag_Zielkondition,"")</f>
@@ -38777,7 +38856,7 @@
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="155" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B12" s="235">
         <f>IFERROR(Kalk_Kredit2!D10*B7*Kalk_RKV!B27,"")</f>
@@ -38794,7 +38873,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="93" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H12" s="244"/>
     </row>
@@ -38809,7 +38888,7 @@
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="155" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B14" s="234" t="str">
         <f>IFERROR(+B12+B11,"")</f>
@@ -38826,13 +38905,13 @@
         <v/>
       </c>
       <c r="G14" s="93" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H14" s="244"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="245" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B15" s="236" t="str">
         <f>IFERROR(+B14-D14,"")</f>
@@ -38858,21 +38937,21 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="81"/>
       <c r="B18" s="237" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C18" s="237"/>
       <c r="D18" s="237" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E18" s="237"/>
       <c r="F18" s="237" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G18" s="81"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="155" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B19" s="234" t="str">
         <f>IFERROR(+Wert_Kredit2!Wertbeitrag_vereinbarter_Effektivzins,"")</f>
@@ -38892,7 +38971,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="155" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B20" s="235">
         <f>+B12</f>
@@ -38909,7 +38988,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="93" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -38923,7 +39002,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="155" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B22" s="234" t="str">
         <f>IFERROR(+B20+B19,"")</f>
@@ -38940,12 +39019,12 @@
         <v/>
       </c>
       <c r="G22" s="93" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="245" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B23" s="236" t="str">
         <f>IFERROR(+B22-D22,"")</f>
@@ -38984,14 +39063,14 @@
       <c r="D26" s="237"/>
       <c r="E26" s="237"/>
       <c r="F26" s="237" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G26" s="81"/>
       <c r="H26" s="247"/>
     </row>
     <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="82" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B27" s="82"/>
       <c r="C27" s="82"/>
@@ -39002,13 +39081,13 @@
         <v/>
       </c>
       <c r="G27" s="93" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H27" s="244"/>
     </row>
     <row r="28" spans="1:8" s="255" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="252" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B28" s="253"/>
       <c r="C28" s="253"/>
@@ -39019,13 +39098,13 @@
         <v/>
       </c>
       <c r="G28" s="93" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H28" s="258"/>
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="81" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B29" s="82"/>
       <c r="C29" s="82"/>
@@ -39036,13 +39115,13 @@
         <v/>
       </c>
       <c r="G29" s="93" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H29" s="244"/>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="82" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B30" s="82"/>
       <c r="C30" s="82"/>
@@ -39053,13 +39132,13 @@
         <v/>
       </c>
       <c r="G30" s="93" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H30" s="244"/>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="81" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B31" s="82"/>
       <c r="C31" s="82"/>
@@ -39070,7 +39149,7 @@
         <v/>
       </c>
       <c r="G31" s="93" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H31" s="244"/>
     </row>
@@ -39086,7 +39165,7 @@
     </row>
     <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="257" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B33" s="244"/>
       <c r="C33" s="244"/>
@@ -39097,7 +39176,7 @@
       <c r="H33" s="244"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/nffbkVlXtmh/i8Huza5eum3/2qPNzrkMIMXtF7vFODU7kUMYcHSLHvqOkKLrGSk35S/dcSClX8+wQEWrjvWwg==" saltValue="07hUAhFBEgmmp2TXSj7HYA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="eLkf7AnMoHJdNW6cuv9Z4k2esKfpkD2T8sehyoyiwAJIA8mBkLreKuGqsEo6PyCyUdj01CLjFspQaLiRaIhT7Q==" saltValue="cIT9pzYWUJH2XQkI6pZw6Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="B5:B7" name="Bereich1"/>
   </protectedRanges>
@@ -39146,8 +39225,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A2:AB139"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39805,7 +39884,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C12" s="218" t="e">
         <f>C7-(C11/10000)</f>
@@ -40205,11 +40284,11 @@
         <v>148</v>
       </c>
       <c r="B18" s="120">
-        <f>IF(Kalkulationstool!D13="MoVe",0.85,1)</f>
+        <f>IF(Kalkulationstool!D13="MoVe",0.75,1)</f>
         <v>1</v>
       </c>
       <c r="C18" s="120">
-        <f>IF(Kalkulationstool!D13="MoVe",0.85,1)</f>
+        <f>IF(Kalkulationstool!D13="MoVe",0.75,1)</f>
         <v>1</v>
       </c>
       <c r="F18" s="1">
@@ -40277,11 +40356,11 @@
         <v>5</v>
       </c>
       <c r="B19" s="1">
-        <f>IF(Kalkulationstool!D13="DVAG",3%*'Background WB vereinb'!C5,0)</f>
+        <f>IF(Kalkulationstool!D13="DVAG",3.5%*'Background WB vereinb'!C5,0)</f>
         <v>0</v>
       </c>
       <c r="C19" s="1">
-        <f>IF(Kalkulationstool!D13="DVAG",3%*'Background WB vereinb'!R5,0)</f>
+        <f>IF(Kalkulationstool!D13="DVAG",3.5%*'Background WB vereinb'!R5,0)</f>
         <v>0</v>
       </c>
       <c r="F19" s="1">
@@ -47119,8 +47198,8 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A3:AB139"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47740,7 +47819,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C12" s="218" t="e">
         <f>C7-(C11/10000)</f>
@@ -48110,11 +48189,11 @@
         <v>148</v>
       </c>
       <c r="B18" s="120">
-        <f>IF(Kalkulationstool!D13="MoVe",0.85,1)</f>
+        <f>IF(Kalkulationstool!D13="MoVe",0.75,1)</f>
         <v>1</v>
       </c>
       <c r="C18" s="120">
-        <f>IF(Kalkulationstool!D13="MoVe",0.85,1)</f>
+        <f>IF(Kalkulationstool!D13="MoVe",0.75,1)</f>
         <v>1</v>
       </c>
       <c r="F18" s="1">
@@ -48177,11 +48256,11 @@
         <v>5</v>
       </c>
       <c r="B19" s="1">
-        <f>IF(Kalkulationstool!D13="DVAG",3%*'Background Produktkalk I'!C5,0)</f>
+        <f>IF(Kalkulationstool!D13="DVAG",3.5%*'Background Produktkalk I'!C5,0)</f>
         <v>0</v>
       </c>
       <c r="C19" s="1">
-        <f>IF(Kalkulationstool!D13="DVAG",3%*'Background Produktkalk I'!R5,0)</f>
+        <f>IF(Kalkulationstool!D13="DVAG",3.5%*'Background Produktkalk I'!R5,0)</f>
         <v>0</v>
       </c>
       <c r="F19" s="1">
@@ -54992,7 +55071,7 @@
   <dimension ref="A1:AZ172"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55125,28 +55204,28 @@
       </c>
       <c r="V3" s="266"/>
       <c r="W3" s="266"/>
-      <c r="AB3" s="268" t="s">
+      <c r="AB3" s="273" t="s">
         <v>87</v>
       </c>
-      <c r="AC3" s="268"/>
-      <c r="AD3" s="268"/>
+      <c r="AC3" s="273"/>
+      <c r="AD3" s="273"/>
       <c r="AE3" s="108"/>
       <c r="AF3" s="108"/>
-      <c r="AI3" s="268" t="s">
+      <c r="AI3" s="273" t="s">
         <v>87</v>
       </c>
-      <c r="AJ3" s="268"/>
-      <c r="AK3" s="268"/>
+      <c r="AJ3" s="273"/>
+      <c r="AK3" s="273"/>
       <c r="AL3" s="108"/>
       <c r="AM3" s="108"/>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
-      <c r="AS3" s="268" t="s">
+      <c r="AS3" s="273" t="s">
         <v>87</v>
       </c>
-      <c r="AT3" s="268"/>
-      <c r="AU3" s="268"/>
+      <c r="AT3" s="273"/>
+      <c r="AU3" s="273"/>
       <c r="AV3" s="108"/>
       <c r="AW3" s="108"/>
       <c r="AX3" s="1"/>
@@ -55183,27 +55262,27 @@
         <f>Kalkulationstool!D10</f>
         <v>0</v>
       </c>
-      <c r="AB4" s="269" t="s">
+      <c r="AB4" s="274" t="s">
         <v>89</v>
       </c>
-      <c r="AC4" s="269"/>
+      <c r="AC4" s="274"/>
       <c r="AD4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AI4" s="269" t="s">
+      <c r="AI4" s="274" t="s">
         <v>91</v>
       </c>
-      <c r="AJ4" s="269"/>
+      <c r="AJ4" s="274"/>
       <c r="AK4" s="1" t="s">
         <v>90</v>
       </c>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
       <c r="AR4" s="1"/>
-      <c r="AS4" s="269" t="s">
+      <c r="AS4" s="274" t="s">
         <v>91</v>
       </c>
-      <c r="AT4" s="269"/>
+      <c r="AT4" s="274"/>
       <c r="AU4" s="1" t="s">
         <v>90</v>
       </c>
@@ -55223,7 +55302,7 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="270" t="s">
+      <c r="H5" s="267" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="124">
@@ -55297,7 +55376,7 @@
       <c r="B6" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="271"/>
+      <c r="H6" s="268"/>
       <c r="I6" s="124">
         <v>5.01</v>
       </c>
@@ -55388,7 +55467,7 @@
       <c r="B7" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="271"/>
+      <c r="H7" s="268"/>
       <c r="I7" s="124">
         <v>10.01</v>
       </c>
@@ -55484,7 +55563,7 @@
       <c r="D8" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="271"/>
+      <c r="H8" s="268"/>
       <c r="I8" s="124">
         <v>15.01</v>
       </c>
@@ -55573,7 +55652,7 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="H9" s="271"/>
+      <c r="H9" s="268"/>
       <c r="I9" s="124">
         <v>20.010000000000002</v>
       </c>
@@ -55662,7 +55741,7 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="H10" s="271"/>
+      <c r="H10" s="268"/>
       <c r="I10" s="124">
         <v>30.01</v>
       </c>
@@ -55755,7 +55834,7 @@
       <c r="D11">
         <v>2</v>
       </c>
-      <c r="H11" s="271"/>
+      <c r="H11" s="268"/>
       <c r="I11" s="124">
         <v>40.01</v>
       </c>
@@ -55770,7 +55849,7 @@
         <v>22</v>
       </c>
       <c r="O11" s="202" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="P11" s="203" t="e">
         <f ca="1">LOOKUP(Wertbeitrag(Kalkulationstool!D10,Kalkulationstool!D9,Kalkulationstool!D8,(((((Kalkulationstool!D20+1)^(1/12))-1)*12)),Kalkulationstool!D14/10000,Kalkulationstool!D7,PMT((((Kalkulationstool!D20+1)^(1/12)-1)),Kalkulationstool!D8,-Kalkulationstool!D10),IF(Kalkulationstool!D9-Kalkulationstool!D8&gt;3,1,0),Kalkulationstool!D13)/Kalkulationstool!D10,Background!I65:I70,Background!K65:K70)/100</f>
@@ -55862,7 +55941,7 @@
       <c r="D12">
         <v>3</v>
       </c>
-      <c r="H12" s="271"/>
+      <c r="H12" s="268"/>
       <c r="I12" s="124">
         <v>50.01</v>
       </c>
@@ -55875,7 +55954,7 @@
       </c>
       <c r="N12" s="278"/>
       <c r="O12" s="207" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="P12" s="208" t="str">
         <f>IF(ISNUMBER(P17),IF(Kalkulationstool!$D$8&gt;84,Background!P14,Background!P13),"")</f>
@@ -55956,7 +56035,7 @@
       <c r="B13" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="271"/>
+      <c r="H13" s="268"/>
       <c r="I13" s="124">
         <v>60.01</v>
       </c>
@@ -55969,7 +56048,7 @@
       </c>
       <c r="N13" s="278"/>
       <c r="O13" s="29" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="P13" s="210" t="e">
         <f>LOOKUP($P$17,Background!I65:I70,Background!K65:K70)/100</f>
@@ -56042,7 +56121,7 @@
       <c r="B14" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="271"/>
+      <c r="H14" s="268"/>
       <c r="I14" s="124">
         <v>70.010000000000005</v>
       </c>
@@ -56055,7 +56134,7 @@
       </c>
       <c r="N14" s="279"/>
       <c r="O14" s="196" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="P14" s="206" t="e">
         <f>LOOKUP($P$17,Background!N65:N70,Background!O65:O70)/100</f>
@@ -56139,7 +56218,7 @@
         <v>44</v>
       </c>
       <c r="D15" s="99"/>
-      <c r="H15" s="271"/>
+      <c r="H15" s="268"/>
       <c r="I15" s="124">
         <v>80.010000000000005</v>
       </c>
@@ -56227,7 +56306,7 @@
       <c r="B16" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="271"/>
+      <c r="H16" s="268"/>
       <c r="I16" s="124">
         <v>90.01</v>
       </c>
@@ -56312,7 +56391,7 @@
       <c r="B17" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="271"/>
+      <c r="H17" s="268"/>
       <c r="I17" s="124">
         <v>100.01</v>
       </c>
@@ -56402,7 +56481,7 @@
       <c r="B18" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="271"/>
+      <c r="H18" s="268"/>
       <c r="I18" s="124">
         <v>125.01</v>
       </c>
@@ -56488,7 +56567,7 @@
       <c r="B19" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="271"/>
+      <c r="H19" s="268"/>
       <c r="I19" s="124">
         <v>150.01</v>
       </c>
@@ -56568,7 +56647,7 @@
       <c r="B20" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="271"/>
+      <c r="H20" s="268"/>
       <c r="I20" s="125">
         <v>175.01</v>
       </c>
@@ -56605,7 +56684,7 @@
       <c r="B21" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="H21" s="271"/>
+      <c r="H21" s="268"/>
       <c r="I21" s="125">
         <v>200.01</v>
       </c>
@@ -56626,18 +56705,18 @@
         <f>W6+V16</f>
         <v>0</v>
       </c>
-      <c r="AA21" s="269" t="s">
+      <c r="AA21" s="274" t="s">
         <v>105</v>
       </c>
-      <c r="AB21" s="269"/>
+      <c r="AB21" s="274"/>
       <c r="AC21" s="1">
         <f>LOOKUP(V16,AA5:AA13,AD5:AD13)</f>
         <v>0</v>
       </c>
-      <c r="AH21" s="269" t="s">
+      <c r="AH21" s="274" t="s">
         <v>106</v>
       </c>
-      <c r="AI21" s="269"/>
+      <c r="AI21" s="274"/>
       <c r="AJ21" s="1">
         <f>IF(ISERROR(LOOKUP(V18,AH5:AH17,AK5:AK17)),0,LOOKUP(V18,AH5:AH17,AK5:AK17))</f>
         <v>0</v>
@@ -56645,10 +56724,10 @@
       <c r="AO21" s="76"/>
       <c r="AP21" s="1"/>
       <c r="AQ21" s="1"/>
-      <c r="AR21" s="269" t="s">
+      <c r="AR21" s="274" t="s">
         <v>106</v>
       </c>
-      <c r="AS21" s="269"/>
+      <c r="AS21" s="274"/>
       <c r="AT21" s="1">
         <f>IF(ISERROR(LOOKUP(V18,AR5:AR17,AU5:AU17)),0,LOOKUP(V18,AR5:AR17,AU5:AU17))</f>
         <v>0</v>
@@ -56667,7 +56746,7 @@
       <c r="B22" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="271"/>
+      <c r="H22" s="268"/>
       <c r="I22" s="125">
         <v>250.01</v>
       </c>
@@ -56719,7 +56798,7 @@
       <c r="A23" s="52">
         <v>999</v>
       </c>
-      <c r="H23" s="271"/>
+      <c r="H23" s="268"/>
       <c r="I23" s="125">
         <v>300.01</v>
       </c>
@@ -56757,7 +56836,7 @@
       <c r="AZ23" s="1"/>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H24" s="271"/>
+      <c r="H24" s="268"/>
       <c r="I24" s="126">
         <v>350.01</v>
       </c>
@@ -56788,7 +56867,7 @@
       <c r="AZ24" s="1"/>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H25" s="271"/>
+      <c r="H25" s="268"/>
       <c r="I25" s="126">
         <v>400.01</v>
       </c>
@@ -56806,36 +56885,36 @@
         <f>AZ29+AT22</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA25" s="276" t="s">
+      <c r="AA25" s="275" t="s">
         <v>107</v>
       </c>
-      <c r="AB25" s="276"/>
-      <c r="AC25" s="276"/>
-      <c r="AD25" s="276"/>
-      <c r="AE25" s="276"/>
-      <c r="AF25" s="276"/>
-      <c r="AH25" s="267" t="s">
+      <c r="AB25" s="275"/>
+      <c r="AC25" s="275"/>
+      <c r="AD25" s="275"/>
+      <c r="AE25" s="275"/>
+      <c r="AF25" s="275"/>
+      <c r="AH25" s="276" t="s">
         <v>108</v>
       </c>
-      <c r="AI25" s="267"/>
-      <c r="AJ25" s="267"/>
-      <c r="AK25" s="267"/>
-      <c r="AL25" s="267"/>
-      <c r="AM25" s="267"/>
-      <c r="AN25" s="267"/>
-      <c r="AO25" s="267"/>
+      <c r="AI25" s="276"/>
+      <c r="AJ25" s="276"/>
+      <c r="AK25" s="276"/>
+      <c r="AL25" s="276"/>
+      <c r="AM25" s="276"/>
+      <c r="AN25" s="276"/>
+      <c r="AO25" s="276"/>
       <c r="AP25" s="1"/>
       <c r="AQ25" s="1"/>
-      <c r="AR25" s="267" t="s">
+      <c r="AR25" s="276" t="s">
         <v>108</v>
       </c>
-      <c r="AS25" s="267"/>
-      <c r="AT25" s="267"/>
-      <c r="AU25" s="267"/>
-      <c r="AV25" s="267"/>
-      <c r="AW25" s="267"/>
-      <c r="AX25" s="267"/>
-      <c r="AY25" s="267"/>
+      <c r="AS25" s="276"/>
+      <c r="AT25" s="276"/>
+      <c r="AU25" s="276"/>
+      <c r="AV25" s="276"/>
+      <c r="AW25" s="276"/>
+      <c r="AX25" s="276"/>
+      <c r="AY25" s="276"/>
       <c r="AZ25" s="1"/>
     </row>
     <row r="26" spans="1:52" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -56888,7 +56967,7 @@
       <c r="AY26" s="129"/>
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H27" s="272" t="s">
+      <c r="H27" s="269" t="s">
         <v>9</v>
       </c>
       <c r="I27" s="101">
@@ -56925,7 +57004,7 @@
       <c r="AZ27" s="1"/>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H28" s="273"/>
+      <c r="H28" s="270"/>
       <c r="I28" s="102">
         <v>9.9999999999999995E-7</v>
       </c>
@@ -56966,7 +57045,7 @@
       <c r="AZ28" s="1"/>
     </row>
     <row r="29" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H29" s="273"/>
+      <c r="H29" s="270"/>
       <c r="I29" s="102">
         <v>0.20000100000000001</v>
       </c>
@@ -57005,7 +57084,7 @@
       </c>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H30" s="273"/>
+      <c r="H30" s="270"/>
       <c r="I30" s="102">
         <v>0.400001</v>
       </c>
@@ -57113,7 +57192,7 @@
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H31" s="273"/>
+      <c r="H31" s="270"/>
       <c r="I31" s="102">
         <v>0.60000100000000001</v>
       </c>
@@ -57221,7 +57300,7 @@
       </c>
     </row>
     <row r="32" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H32" s="274"/>
+      <c r="H32" s="271"/>
       <c r="I32" s="103">
         <v>0.80000099999999996</v>
       </c>
@@ -57332,7 +57411,7 @@
       </c>
     </row>
     <row r="33" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H33" s="271" t="s">
+      <c r="H33" s="268" t="s">
         <v>17</v>
       </c>
       <c r="I33" s="104">
@@ -57447,7 +57526,7 @@
       </c>
     </row>
     <row r="34" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H34" s="271"/>
+      <c r="H34" s="268"/>
       <c r="I34" s="104">
         <v>0.20000100000000001</v>
       </c>
@@ -57560,7 +57639,7 @@
       </c>
     </row>
     <row r="35" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H35" s="271"/>
+      <c r="H35" s="268"/>
       <c r="I35" s="104">
         <v>0.400001</v>
       </c>
@@ -57673,7 +57752,7 @@
       </c>
     </row>
     <row r="36" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H36" s="271"/>
+      <c r="H36" s="268"/>
       <c r="I36" s="104">
         <v>0.60000100000000001</v>
       </c>
@@ -57786,7 +57865,7 @@
       </c>
     </row>
     <row r="37" spans="8:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H37" s="275"/>
+      <c r="H37" s="272"/>
       <c r="I37" s="104">
         <v>0.80000099999999996</v>
       </c>
@@ -60612,14 +60691,14 @@
     </row>
     <row r="63" spans="8:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H63" s="24" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I63" s="24"/>
       <c r="J63" s="24"/>
       <c r="K63" s="24"/>
       <c r="L63" s="24"/>
       <c r="N63" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AA63" s="1">
         <f t="shared" si="17"/>
@@ -70551,6 +70630,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AR25:AY25"/>
+    <mergeCell ref="AR2:AY2"/>
+    <mergeCell ref="AS3:AU3"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AR21:AS21"/>
     <mergeCell ref="H5:H25"/>
     <mergeCell ref="H27:H32"/>
     <mergeCell ref="H33:H37"/>
@@ -70566,11 +70650,6 @@
     <mergeCell ref="AA25:AF25"/>
     <mergeCell ref="AH25:AO25"/>
     <mergeCell ref="N11:N14"/>
-    <mergeCell ref="AR25:AY25"/>
-    <mergeCell ref="AR2:AY2"/>
-    <mergeCell ref="AS3:AU3"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AR21:AS21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -70626,7 +70705,7 @@
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="71" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C2" s="70"/>
       <c r="D2" s="70"/>
@@ -70645,7 +70724,7 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="220" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F4" s="67"/>
       <c r="G4" s="67"/>
@@ -70712,7 +70791,7 @@
       <c r="F7" s="123"/>
       <c r="G7" s="92"/>
       <c r="H7" s="93" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I7" s="82"/>
       <c r="J7" s="82"/>
@@ -70738,7 +70817,7 @@
       <c r="F8" s="92"/>
       <c r="G8" s="93"/>
       <c r="H8" s="93" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I8" s="82"/>
       <c r="J8" s="82"/>
@@ -70764,7 +70843,7 @@
       <c r="F9" s="92"/>
       <c r="G9" s="93"/>
       <c r="H9" s="93" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I9" s="82"/>
       <c r="J9" s="82"/>
@@ -70790,7 +70869,7 @@
       <c r="F10" s="94"/>
       <c r="G10" s="93"/>
       <c r="H10" s="93" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I10" s="82"/>
       <c r="J10" s="82"/>
@@ -70815,7 +70894,7 @@
       <c r="F11" s="94"/>
       <c r="G11" s="93"/>
       <c r="H11" s="93" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="82"/>
@@ -70841,7 +70920,7 @@
       <c r="F12" s="94"/>
       <c r="G12" s="93"/>
       <c r="H12" s="93" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I12" s="82"/>
       <c r="J12" s="82"/>
@@ -70867,7 +70946,7 @@
       <c r="F13" s="92"/>
       <c r="G13" s="93"/>
       <c r="H13" s="93" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I13" s="82"/>
       <c r="J13" s="82"/>
@@ -70893,7 +70972,7 @@
       <c r="F14" s="92"/>
       <c r="G14" s="93"/>
       <c r="H14" s="93" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I14" s="82"/>
       <c r="J14" s="82"/>
@@ -70925,7 +71004,7 @@
       <c r="C19" s="82"/>
       <c r="D19" s="122">
         <f ca="1">NOW()</f>
-        <v>44909.854944212966</v>
+        <v>44943.655650231478</v>
       </c>
       <c r="E19" s="82"/>
       <c r="F19" s="82" t="s">
@@ -71212,10 +71291,10 @@
     <tabColor theme="4" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -71225,7 +71304,7 @@
     <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="73" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="94.85546875" style="1" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="1" hidden="1"/>
   </cols>
   <sheetData>
@@ -71243,7 +71322,7 @@
     </row>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="220" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C3" s="70"/>
     </row>
@@ -71274,7 +71353,7 @@
       </c>
       <c r="E5" s="92"/>
       <c r="F5" s="93" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -71288,7 +71367,7 @@
       <c r="D6" s="151"/>
       <c r="E6" s="152"/>
       <c r="F6" s="93" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -71317,7 +71396,7 @@
       <c r="D9" s="151"/>
       <c r="E9" s="93"/>
       <c r="F9" s="93" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -71328,7 +71407,7 @@
       <c r="D10" s="146"/>
       <c r="E10" s="92"/>
       <c r="F10" s="93" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -71339,7 +71418,7 @@
       <c r="D11" s="92"/>
       <c r="E11" s="92"/>
       <c r="F11" s="93" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -71402,7 +71481,7 @@
     </row>
     <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D18" s="154"/>
       <c r="E18" s="154"/>
@@ -71410,7 +71489,7 @@
     </row>
     <row r="19" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>167</v>
+        <v>238</v>
       </c>
       <c r="D19" s="154"/>
       <c r="E19" s="154"/>
@@ -71418,7 +71497,7 @@
     </row>
     <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>169</v>
+        <v>239</v>
       </c>
       <c r="C20" s="154"/>
       <c r="D20" s="154"/>
@@ -71426,11 +71505,16 @@
       <c r="F20" s="154"/>
     </row>
     <row r="21" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="147" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B21" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="147" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <protectedRanges>

</xml_diff>

<commit_message>
Neue Kompetenzspannen ab 1.4.2023
</commit_message>
<xml_diff>
--- a/ExcelBlanko.xlsx
+++ b/ExcelBlanko.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\V\DATEN\BN_BSS11\T_PRO_PKG\Performance\DB Verprobung\Vertriebstool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07A89781-C5D2-4FF0-9952-8938F62F6B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="wJFlHBhF99Wnc1g+0/u0ACNiHmTzjlFIDlICnHtkYn+yyomZ0UkjA+fw9BBXroFt6P8XaPp63Hl6G4XiQVn7hg==" workbookSaltValue="h86qGiaJ/emgajeOgOUvCw==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328FDBF1-0BFE-4717-A1A3-47129F7B3CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="814" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,16 +17,16 @@
     <sheet name="Kalkulationstool" sheetId="13" r:id="rId2"/>
     <sheet name="Wertbeitrag" sheetId="16" r:id="rId3"/>
     <sheet name="Bewertung Aufstockung" sheetId="26" r:id="rId4"/>
-    <sheet name="Background WB vereinb" sheetId="18" state="hidden" r:id="rId5"/>
-    <sheet name="Background Produktkalk I" sheetId="19" state="hidden" r:id="rId6"/>
-    <sheet name="Background" sheetId="14" state="hidden" r:id="rId7"/>
-    <sheet name="Kalk_Kredit2" sheetId="21" state="hidden" r:id="rId8"/>
-    <sheet name="Wert_Kredit2" sheetId="22" state="hidden" r:id="rId9"/>
-    <sheet name="Kalk_RKV" sheetId="25" state="hidden" r:id="rId10"/>
-    <sheet name="Bg WB vereinb_Kredit2" sheetId="23" state="hidden" r:id="rId11"/>
-    <sheet name="Bg Produktkalk I_Kredit2" sheetId="24" state="hidden" r:id="rId12"/>
-    <sheet name="Background2" sheetId="27" state="hidden" r:id="rId13"/>
-    <sheet name="Aufstockungsquoten" sheetId="28" state="hidden" r:id="rId14"/>
+    <sheet name="Background WB vereinb" sheetId="18" r:id="rId5"/>
+    <sheet name="Background Produktkalk I" sheetId="19" r:id="rId6"/>
+    <sheet name="Background" sheetId="14" r:id="rId7"/>
+    <sheet name="Kalk_Kredit2" sheetId="21" r:id="rId8"/>
+    <sheet name="Wert_Kredit2" sheetId="22" r:id="rId9"/>
+    <sheet name="Kalk_RKV" sheetId="25" r:id="rId10"/>
+    <sheet name="Bg WB vereinb_Kredit2" sheetId="23" r:id="rId11"/>
+    <sheet name="Bg Produktkalk I_Kredit2" sheetId="24" r:id="rId12"/>
+    <sheet name="Background2" sheetId="27" r:id="rId13"/>
+    <sheet name="Aufstockungsquoten" sheetId="28" r:id="rId14"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId15"/>
@@ -1000,9 +999,6 @@
     <t>Je geringer der Aufstockungsbetrag und je länger die Restlaufzeit des Altkredites, desto höher ist die Abweichung.</t>
   </si>
   <si>
-    <t>Gültig ab 18.01.2023</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Insbesondere </t>
     </r>
@@ -1074,6 +1070,9 @@
       </rPr>
       <t xml:space="preserve"> vornimmt.</t>
     </r>
+  </si>
+  <si>
+    <t>Gültig ab 01.04.2023</t>
   </si>
 </sst>
 </file>
@@ -5820,15 +5819,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>639536</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>721179</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>77561</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>14967</xdr:rowOff>
+      <xdr:colOff>159204</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>55789</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5858,7 +5857,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11212286" y="4381499"/>
+          <a:off x="11293929" y="7688035"/>
           <a:ext cx="3424918" cy="1362075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5874,6 +5873,50 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>639536</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>13609</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1415143</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>67080</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7A26DD5-29C1-A71D-35C3-F730D6F934C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11212286" y="9007930"/>
+          <a:ext cx="5660571" cy="1985686"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -6524,7 +6567,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -6610,7 +6653,6 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="temSBCYz7mahSiJ39Bf+V4by9SgkBbWNcvxxbwnu8Gb9qG1rc6GIvGPPKmmqNuGA67OpkWjJRCIaFmBhkNrzBg==" saltValue="wMLFQPrQDycciyUax63Oug==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -22486,7 +22528,7 @@
   <dimension ref="A1:AZ163"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22711,7 +22753,7 @@
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="12">
-        <v>-1.3</v>
+        <v>-1.5</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>25</v>
@@ -22769,7 +22811,7 @@
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="13">
-        <v>-1.1000000000000001</v>
+        <v>-1.2</v>
       </c>
       <c r="L6" s="120">
         <v>6</v>
@@ -22849,7 +22891,7 @@
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="13">
-        <v>-0.9</v>
+        <v>-1</v>
       </c>
       <c r="L7" s="120">
         <v>11</v>
@@ -28519,7 +28561,7 @@
       </c>
       <c r="J69" s="34"/>
       <c r="K69" s="33">
-        <v>-2</v>
+        <v>-2.5</v>
       </c>
       <c r="L69" s="35">
         <v>-4</v>
@@ -28529,7 +28571,7 @@
       </c>
       <c r="O69" s="33">
         <f t="shared" si="34"/>
-        <v>-2</v>
+        <v>-2.5</v>
       </c>
       <c r="P69" s="35">
         <f t="shared" si="34"/>
@@ -28639,7 +28681,7 @@
       </c>
       <c r="J70" s="37"/>
       <c r="K70" s="36">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="L70" s="38">
         <v>-6</v>
@@ -28649,7 +28691,7 @@
       </c>
       <c r="O70" s="36">
         <f t="shared" si="34"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="P70" s="38">
         <f t="shared" si="34"/>
@@ -37830,7 +37872,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -37872,7 +37914,7 @@
       <c r="G2" s="67"/>
       <c r="Q2" s="241"/>
       <c r="R2" s="242" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="5.0999999999999996" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -38161,7 +38203,7 @@
       <c r="C19" s="82"/>
       <c r="D19" s="122">
         <f ca="1">NOW()</f>
-        <v>44943.655650231478</v>
+        <v>45008.746126851853</v>
       </c>
       <c r="E19" s="82"/>
       <c r="F19" s="82" t="s">
@@ -38345,7 +38387,7 @@
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="+l00WxGYIb4qoYpIo+q8yM/EDAiBYPzCzE9uo+t51RK/AfveDAfilUXMFvymMd4E65wGTQ4Fi6Mm7LG9UiSfrg==" saltValue="kfULYYEAQWvItHAUy45niw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="D8" name="Range6"/>
     <protectedRange sqref="D19" name="Range5"/>
@@ -38451,7 +38493,7 @@
   <dimension ref="B1:XFC23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -38651,7 +38693,7 @@
     </row>
     <row r="19" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D19" s="154"/>
       <c r="E19" s="154"/>
@@ -38659,7 +38701,7 @@
     </row>
     <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C20" s="154"/>
       <c r="D20" s="154"/>
@@ -38678,7 +38720,7 @@
     </row>
     <row r="23" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="md4XruLI5VbWansdC0cUhfCj2E8GvTFvtOHiVRMXpotxVSGvewZQJNlssjDk5o9QrGjcMGXFlJ12mnnyClsgVg==" saltValue="7L5y2Fa82BHIlu9JX6JqnQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="C11" name="Range1"/>
   </protectedRanges>
@@ -39176,7 +39218,6 @@
       <c r="H33" s="244"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="eLkf7AnMoHJdNW6cuv9Z4k2esKfpkD2T8sehyoyiwAJIA8mBkLreKuGqsEo6PyCyUdj01CLjFspQaLiRaIhT7Q==" saltValue="cIT9pzYWUJH2XQkI6pZw6Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="B5:B7" name="Bereich1"/>
   </protectedRanges>
@@ -55070,9 +55111,7 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AZ172"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -55310,7 +55349,7 @@
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="12">
-        <v>-1.3</v>
+        <v>-1.5</v>
       </c>
       <c r="L5" s="1"/>
       <c r="N5" s="5" t="s">
@@ -55382,7 +55421,7 @@
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="13">
-        <v>-1.1000000000000001</v>
+        <v>-1.2</v>
       </c>
       <c r="L6" s="120">
         <v>6</v>
@@ -55473,7 +55512,7 @@
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="13">
-        <v>-0.9</v>
+        <v>-1</v>
       </c>
       <c r="L7" s="120">
         <v>11</v>
@@ -61410,7 +61449,7 @@
       </c>
       <c r="J69" s="34"/>
       <c r="K69" s="33">
-        <v>-2</v>
+        <v>-2.5</v>
       </c>
       <c r="L69" s="35">
         <v>-4</v>
@@ -61420,7 +61459,7 @@
       </c>
       <c r="O69" s="33">
         <f t="shared" si="34"/>
-        <v>-2</v>
+        <v>-2.5</v>
       </c>
       <c r="P69" s="35">
         <f t="shared" si="34"/>
@@ -61531,7 +61570,7 @@
       </c>
       <c r="J70" s="37"/>
       <c r="K70" s="36">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="L70" s="38">
         <v>-6</v>
@@ -61541,7 +61580,7 @@
       </c>
       <c r="O70" s="36">
         <f t="shared" si="34"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="P70" s="38">
         <f t="shared" si="34"/>
@@ -71004,7 +71043,7 @@
       <c r="C19" s="82"/>
       <c r="D19" s="122">
         <f ca="1">NOW()</f>
-        <v>44943.655650231478</v>
+        <v>45008.746126851853</v>
       </c>
       <c r="E19" s="82"/>
       <c r="F19" s="82" t="s">
@@ -71527,7 +71566,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="90" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="78" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K000000</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
geänderte Version nach Ausweitung Soko-Spannen
</commit_message>
<xml_diff>
--- a/ExcelBlanko.xlsx
+++ b/ExcelBlanko.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\V\DATEN\BN_BSS11\T_PRO_PKG\Performance\DB Verprobung\Vertriebstool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\oneLine_Backoffice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328FDBF1-0BFE-4717-A1A3-47129F7B3CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{656C7995-4956-4C74-B86A-F70CEB8566CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="gm2dPiWxIMNsDKrisWsc5WLNjjitri0iA4syQpFqL5RaTEuj7VAd2m49uxgfC9kizD2K5A2upTNioENqEvF98w==" workbookSaltValue="l4enb28rPm+jfY9sBLjxmw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="814" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="814" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Startseite" sheetId="15" r:id="rId1"/>
     <sheet name="Kalkulationstool" sheetId="13" r:id="rId2"/>
     <sheet name="Wertbeitrag" sheetId="16" r:id="rId3"/>
     <sheet name="Bewertung Aufstockung" sheetId="26" r:id="rId4"/>
-    <sheet name="Background WB vereinb" sheetId="18" r:id="rId5"/>
-    <sheet name="Background Produktkalk I" sheetId="19" r:id="rId6"/>
-    <sheet name="Background" sheetId="14" r:id="rId7"/>
-    <sheet name="Kalk_Kredit2" sheetId="21" r:id="rId8"/>
-    <sheet name="Wert_Kredit2" sheetId="22" r:id="rId9"/>
-    <sheet name="Kalk_RKV" sheetId="25" r:id="rId10"/>
-    <sheet name="Bg WB vereinb_Kredit2" sheetId="23" r:id="rId11"/>
-    <sheet name="Bg Produktkalk I_Kredit2" sheetId="24" r:id="rId12"/>
-    <sheet name="Background2" sheetId="27" r:id="rId13"/>
-    <sheet name="Aufstockungsquoten" sheetId="28" r:id="rId14"/>
+    <sheet name="Background WB vereinb" sheetId="18" state="hidden" r:id="rId5"/>
+    <sheet name="Background Produktkalk I" sheetId="19" state="hidden" r:id="rId6"/>
+    <sheet name="Background" sheetId="14" state="hidden" r:id="rId7"/>
+    <sheet name="Kalk_Kredit2" sheetId="21" state="hidden" r:id="rId8"/>
+    <sheet name="Wert_Kredit2" sheetId="22" state="hidden" r:id="rId9"/>
+    <sheet name="Kalk_RKV" sheetId="25" state="hidden" r:id="rId10"/>
+    <sheet name="Bg WB vereinb_Kredit2" sheetId="23" state="hidden" r:id="rId11"/>
+    <sheet name="Bg Produktkalk I_Kredit2" sheetId="24" state="hidden" r:id="rId12"/>
+    <sheet name="Background2" sheetId="27" state="hidden" r:id="rId13"/>
+    <sheet name="Aufstockungsquoten" sheetId="28" state="hidden" r:id="rId14"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId15"/>
@@ -2857,6 +2858,15 @@
     <xf numFmtId="0" fontId="16" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2875,16 +2885,7 @@
     <xf numFmtId="0" fontId="18" fillId="37" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6653,6 +6654,7 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="rDIr7MXL5rTEMxNi8zBfWb3TU3wFh8y2xOXyMx7JNWxvwgviUHWidQttwbHNKCIEg51Rqs5wvLTeIeygK1vuPQ==" saltValue="JhqFqNARO6mfghGm/mFxVA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -22662,25 +22664,25 @@
       </c>
       <c r="V3" s="266"/>
       <c r="W3" s="266"/>
-      <c r="AB3" s="273" t="s">
+      <c r="AB3" s="268" t="s">
         <v>87</v>
       </c>
-      <c r="AC3" s="273"/>
-      <c r="AD3" s="273"/>
+      <c r="AC3" s="268"/>
+      <c r="AD3" s="268"/>
       <c r="AE3" s="108"/>
       <c r="AF3" s="108"/>
-      <c r="AI3" s="273" t="s">
+      <c r="AI3" s="268" t="s">
         <v>87</v>
       </c>
-      <c r="AJ3" s="273"/>
-      <c r="AK3" s="273"/>
+      <c r="AJ3" s="268"/>
+      <c r="AK3" s="268"/>
       <c r="AL3" s="108"/>
       <c r="AM3" s="108"/>
-      <c r="AS3" s="273" t="s">
+      <c r="AS3" s="268" t="s">
         <v>87</v>
       </c>
-      <c r="AT3" s="273"/>
-      <c r="AU3" s="273"/>
+      <c r="AT3" s="268"/>
+      <c r="AU3" s="268"/>
       <c r="AV3" s="108"/>
       <c r="AW3" s="108"/>
     </row>
@@ -22713,24 +22715,24 @@
         <f>Kalk_Kredit2!D10</f>
         <v>0</v>
       </c>
-      <c r="AB4" s="274" t="s">
+      <c r="AB4" s="269" t="s">
         <v>89</v>
       </c>
-      <c r="AC4" s="274"/>
+      <c r="AC4" s="269"/>
       <c r="AD4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AI4" s="274" t="s">
+      <c r="AI4" s="269" t="s">
         <v>91</v>
       </c>
-      <c r="AJ4" s="274"/>
+      <c r="AJ4" s="269"/>
       <c r="AK4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AS4" s="274" t="s">
+      <c r="AS4" s="269" t="s">
         <v>91</v>
       </c>
-      <c r="AT4" s="274"/>
+      <c r="AT4" s="269"/>
       <c r="AU4" s="1" t="s">
         <v>90</v>
       </c>
@@ -22745,7 +22747,7 @@
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="267" t="s">
+      <c r="H5" s="270" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="124">
@@ -22805,7 +22807,7 @@
       <c r="B6" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="268"/>
+      <c r="H6" s="271"/>
       <c r="I6" s="124">
         <v>5.01</v>
       </c>
@@ -22885,7 +22887,7 @@
       <c r="B7" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="268"/>
+      <c r="H7" s="271"/>
       <c r="I7" s="124">
         <v>10.01</v>
       </c>
@@ -22970,7 +22972,7 @@
       <c r="D8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="268"/>
+      <c r="H8" s="271"/>
       <c r="I8" s="124">
         <v>15.01</v>
       </c>
@@ -23046,7 +23048,7 @@
       <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="268"/>
+      <c r="H9" s="271"/>
       <c r="I9" s="124">
         <v>20.010000000000002</v>
       </c>
@@ -23122,7 +23124,7 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="H10" s="268"/>
+      <c r="H10" s="271"/>
       <c r="I10" s="124">
         <v>30.01</v>
       </c>
@@ -23202,7 +23204,7 @@
       <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="H11" s="268"/>
+      <c r="H11" s="271"/>
       <c r="I11" s="124">
         <v>40.01</v>
       </c>
@@ -23302,7 +23304,7 @@
       <c r="D12" s="1">
         <v>3</v>
       </c>
-      <c r="H12" s="268"/>
+      <c r="H12" s="271"/>
       <c r="I12" s="124">
         <v>50.01</v>
       </c>
@@ -23389,7 +23391,7 @@
       <c r="B13" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="268"/>
+      <c r="H13" s="271"/>
       <c r="I13" s="124">
         <v>60.01</v>
       </c>
@@ -23468,7 +23470,7 @@
       <c r="B14" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="268"/>
+      <c r="H14" s="271"/>
       <c r="I14" s="124">
         <v>70.010000000000005</v>
       </c>
@@ -23558,7 +23560,7 @@
         <v>44</v>
       </c>
       <c r="D15" s="99"/>
-      <c r="H15" s="268"/>
+      <c r="H15" s="271"/>
       <c r="I15" s="124">
         <v>80.010000000000005</v>
       </c>
@@ -23639,7 +23641,7 @@
       <c r="B16" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="268"/>
+      <c r="H16" s="271"/>
       <c r="I16" s="124">
         <v>90.01</v>
       </c>
@@ -23717,7 +23719,7 @@
       <c r="B17" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="268"/>
+      <c r="H17" s="271"/>
       <c r="I17" s="124">
         <v>100.01</v>
       </c>
@@ -23800,7 +23802,7 @@
       <c r="B18" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="268"/>
+      <c r="H18" s="271"/>
       <c r="I18" s="124">
         <v>125.01</v>
       </c>
@@ -23878,7 +23880,7 @@
       <c r="B19" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="268"/>
+      <c r="H19" s="271"/>
       <c r="I19" s="124">
         <v>150.01</v>
       </c>
@@ -23950,7 +23952,7 @@
       <c r="B20" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="268"/>
+      <c r="H20" s="271"/>
       <c r="I20" s="125">
         <v>175.01</v>
       </c>
@@ -23976,7 +23978,7 @@
       <c r="B21" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="H21" s="268"/>
+      <c r="H21" s="271"/>
       <c r="I21" s="125">
         <v>200.01</v>
       </c>
@@ -23997,27 +23999,27 @@
         <f>W6+V16</f>
         <v>0</v>
       </c>
-      <c r="AA21" s="274" t="s">
+      <c r="AA21" s="269" t="s">
         <v>105</v>
       </c>
-      <c r="AB21" s="274"/>
+      <c r="AB21" s="269"/>
       <c r="AC21" s="1">
         <f>LOOKUP(V16,AA5:AA13,AD5:AD13)</f>
         <v>0</v>
       </c>
-      <c r="AH21" s="274" t="s">
+      <c r="AH21" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="AI21" s="274"/>
+      <c r="AI21" s="269"/>
       <c r="AJ21" s="1">
         <f>IF(ISERROR(LOOKUP(V18,AH5:AH17,AK5:AK17)),0,LOOKUP(V18,AH5:AH17,AK5:AK17))</f>
         <v>0</v>
       </c>
       <c r="AO21" s="76"/>
-      <c r="AR21" s="274" t="s">
+      <c r="AR21" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="AS21" s="274"/>
+      <c r="AS21" s="269"/>
       <c r="AT21" s="1">
         <f>IF(ISERROR(LOOKUP(V18,AR5:AR17,AU5:AU17)),0,LOOKUP(V18,AR5:AR17,AU5:AU17))</f>
         <v>0</v>
@@ -24031,7 +24033,7 @@
       <c r="B22" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="268"/>
+      <c r="H22" s="271"/>
       <c r="I22" s="125">
         <v>250.01</v>
       </c>
@@ -24074,7 +24076,7 @@
       <c r="A23" s="52">
         <v>999</v>
       </c>
-      <c r="H23" s="268"/>
+      <c r="H23" s="271"/>
       <c r="I23" s="125">
         <v>300.01</v>
       </c>
@@ -24102,7 +24104,7 @@
       </c>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H24" s="268"/>
+      <c r="H24" s="271"/>
       <c r="I24" s="126">
         <v>350.01</v>
       </c>
@@ -24121,7 +24123,7 @@
       </c>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H25" s="268"/>
+      <c r="H25" s="271"/>
       <c r="I25" s="126">
         <v>400.01</v>
       </c>
@@ -24138,34 +24140,34 @@
         <f>AZ29+AT22</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA25" s="275" t="s">
+      <c r="AA25" s="276" t="s">
         <v>107</v>
       </c>
-      <c r="AB25" s="275"/>
-      <c r="AC25" s="275"/>
-      <c r="AD25" s="275"/>
-      <c r="AE25" s="275"/>
-      <c r="AF25" s="275"/>
-      <c r="AH25" s="276" t="s">
+      <c r="AB25" s="276"/>
+      <c r="AC25" s="276"/>
+      <c r="AD25" s="276"/>
+      <c r="AE25" s="276"/>
+      <c r="AF25" s="276"/>
+      <c r="AH25" s="267" t="s">
         <v>108</v>
       </c>
-      <c r="AI25" s="276"/>
-      <c r="AJ25" s="276"/>
-      <c r="AK25" s="276"/>
-      <c r="AL25" s="276"/>
-      <c r="AM25" s="276"/>
-      <c r="AN25" s="276"/>
-      <c r="AO25" s="276"/>
-      <c r="AR25" s="276" t="s">
+      <c r="AI25" s="267"/>
+      <c r="AJ25" s="267"/>
+      <c r="AK25" s="267"/>
+      <c r="AL25" s="267"/>
+      <c r="AM25" s="267"/>
+      <c r="AN25" s="267"/>
+      <c r="AO25" s="267"/>
+      <c r="AR25" s="267" t="s">
         <v>108</v>
       </c>
-      <c r="AS25" s="276"/>
-      <c r="AT25" s="276"/>
-      <c r="AU25" s="276"/>
-      <c r="AV25" s="276"/>
-      <c r="AW25" s="276"/>
-      <c r="AX25" s="276"/>
-      <c r="AY25" s="276"/>
+      <c r="AS25" s="267"/>
+      <c r="AT25" s="267"/>
+      <c r="AU25" s="267"/>
+      <c r="AV25" s="267"/>
+      <c r="AW25" s="267"/>
+      <c r="AX25" s="267"/>
+      <c r="AY25" s="267"/>
     </row>
     <row r="26" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H26" s="238"/>
@@ -24217,7 +24219,7 @@
       <c r="AY26" s="239"/>
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H27" s="269" t="s">
+      <c r="H27" s="272" t="s">
         <v>9</v>
       </c>
       <c r="I27" s="101">
@@ -24244,7 +24246,7 @@
       </c>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H28" s="270"/>
+      <c r="H28" s="273"/>
       <c r="I28" s="102">
         <v>9.9999999999999995E-7</v>
       </c>
@@ -24275,7 +24277,7 @@
       </c>
     </row>
     <row r="29" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H29" s="270"/>
+      <c r="H29" s="273"/>
       <c r="I29" s="102">
         <v>0.20000100000000001</v>
       </c>
@@ -24305,7 +24307,7 @@
       </c>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H30" s="270"/>
+      <c r="H30" s="273"/>
       <c r="I30" s="102">
         <v>0.400001</v>
       </c>
@@ -24411,7 +24413,7 @@
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H31" s="270"/>
+      <c r="H31" s="273"/>
       <c r="I31" s="102">
         <v>0.60000100000000001</v>
       </c>
@@ -24517,7 +24519,7 @@
       </c>
     </row>
     <row r="32" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H32" s="271"/>
+      <c r="H32" s="274"/>
       <c r="I32" s="103">
         <v>0.80000099999999996</v>
       </c>
@@ -24626,7 +24628,7 @@
       </c>
     </row>
     <row r="33" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H33" s="268" t="s">
+      <c r="H33" s="271" t="s">
         <v>17</v>
       </c>
       <c r="I33" s="104">
@@ -24740,7 +24742,7 @@
       </c>
     </row>
     <row r="34" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H34" s="268"/>
+      <c r="H34" s="271"/>
       <c r="I34" s="104">
         <v>0.20000100000000001</v>
       </c>
@@ -24852,7 +24854,7 @@
       </c>
     </row>
     <row r="35" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H35" s="268"/>
+      <c r="H35" s="271"/>
       <c r="I35" s="104">
         <v>0.400001</v>
       </c>
@@ -24964,7 +24966,7 @@
       </c>
     </row>
     <row r="36" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H36" s="268"/>
+      <c r="H36" s="271"/>
       <c r="I36" s="104">
         <v>0.60000100000000001</v>
       </c>
@@ -25076,7 +25078,7 @@
       </c>
     </row>
     <row r="37" spans="8:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H37" s="272"/>
+      <c r="H37" s="275"/>
       <c r="I37" s="104">
         <v>0.80000099999999996</v>
       </c>
@@ -37600,13 +37602,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AF2"/>
-    <mergeCell ref="AH2:AO2"/>
-    <mergeCell ref="AR2:AY2"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AI3:AK3"/>
-    <mergeCell ref="AS3:AU3"/>
     <mergeCell ref="AR25:AY25"/>
     <mergeCell ref="H27:H32"/>
     <mergeCell ref="H33:H37"/>
@@ -37620,6 +37615,13 @@
     <mergeCell ref="AR21:AS21"/>
     <mergeCell ref="AA25:AF25"/>
     <mergeCell ref="AH25:AO25"/>
+    <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="AH2:AO2"/>
+    <mergeCell ref="AR2:AY2"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AI3:AK3"/>
+    <mergeCell ref="AS3:AU3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -37872,7 +37874,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -38203,7 +38205,7 @@
       <c r="C19" s="82"/>
       <c r="D19" s="122">
         <f ca="1">NOW()</f>
-        <v>45008.746126851853</v>
+        <v>45014.848979861112</v>
       </c>
       <c r="E19" s="82"/>
       <c r="F19" s="82" t="s">
@@ -38387,7 +38389,7 @@
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="8CpCEHi2iB/wdzB0Lb/z5jCvw11A9lO9rETlaNvirFDYdaFk51swq0LoZbMyentEWLaeo9OtI12MB010SPcC5Q==" saltValue="CNqprhqmzpr/rDlt/Xo6jg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="D8" name="Range6"/>
     <protectedRange sqref="D19" name="Range5"/>
@@ -38493,7 +38495,7 @@
   <dimension ref="B1:XFC23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -38720,7 +38722,7 @@
     </row>
     <row r="23" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2foKn/wSAnbmvYG2f0fP2sOXHQEl0giobNGFI0sYLSKmOMWmu4v1cEok9XdLdyDHH6hek6TL1LCM16skcSr/DA==" saltValue="iwXAWv/V6Isde4AGUsQnQg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="C11" name="Range1"/>
   </protectedRanges>
@@ -39218,6 +39220,7 @@
       <c r="H33" s="244"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="3MA5Uu4/i5+lr7jhSWrJzk3rsvUPFqDdpEPGgE5VEPK2lfTZDtLyklJZLDVTbzeAfgT1vv19R88qd+WeI+DZMg==" saltValue="chhSDgF2OJboQGJHEz4/aA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="B5:B7" name="Bereich1"/>
   </protectedRanges>
@@ -55243,28 +55246,28 @@
       </c>
       <c r="V3" s="266"/>
       <c r="W3" s="266"/>
-      <c r="AB3" s="273" t="s">
+      <c r="AB3" s="268" t="s">
         <v>87</v>
       </c>
-      <c r="AC3" s="273"/>
-      <c r="AD3" s="273"/>
+      <c r="AC3" s="268"/>
+      <c r="AD3" s="268"/>
       <c r="AE3" s="108"/>
       <c r="AF3" s="108"/>
-      <c r="AI3" s="273" t="s">
+      <c r="AI3" s="268" t="s">
         <v>87</v>
       </c>
-      <c r="AJ3" s="273"/>
-      <c r="AK3" s="273"/>
+      <c r="AJ3" s="268"/>
+      <c r="AK3" s="268"/>
       <c r="AL3" s="108"/>
       <c r="AM3" s="108"/>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
-      <c r="AS3" s="273" t="s">
+      <c r="AS3" s="268" t="s">
         <v>87</v>
       </c>
-      <c r="AT3" s="273"/>
-      <c r="AU3" s="273"/>
+      <c r="AT3" s="268"/>
+      <c r="AU3" s="268"/>
       <c r="AV3" s="108"/>
       <c r="AW3" s="108"/>
       <c r="AX3" s="1"/>
@@ -55301,27 +55304,27 @@
         <f>Kalkulationstool!D10</f>
         <v>0</v>
       </c>
-      <c r="AB4" s="274" t="s">
+      <c r="AB4" s="269" t="s">
         <v>89</v>
       </c>
-      <c r="AC4" s="274"/>
+      <c r="AC4" s="269"/>
       <c r="AD4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AI4" s="274" t="s">
+      <c r="AI4" s="269" t="s">
         <v>91</v>
       </c>
-      <c r="AJ4" s="274"/>
+      <c r="AJ4" s="269"/>
       <c r="AK4" s="1" t="s">
         <v>90</v>
       </c>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
       <c r="AR4" s="1"/>
-      <c r="AS4" s="274" t="s">
+      <c r="AS4" s="269" t="s">
         <v>91</v>
       </c>
-      <c r="AT4" s="274"/>
+      <c r="AT4" s="269"/>
       <c r="AU4" s="1" t="s">
         <v>90</v>
       </c>
@@ -55341,7 +55344,7 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="267" t="s">
+      <c r="H5" s="270" t="s">
         <v>16</v>
       </c>
       <c r="I5" s="124">
@@ -55415,7 +55418,7 @@
       <c r="B6" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="268"/>
+      <c r="H6" s="271"/>
       <c r="I6" s="124">
         <v>5.01</v>
       </c>
@@ -55506,7 +55509,7 @@
       <c r="B7" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="268"/>
+      <c r="H7" s="271"/>
       <c r="I7" s="124">
         <v>10.01</v>
       </c>
@@ -55602,7 +55605,7 @@
       <c r="D8" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="268"/>
+      <c r="H8" s="271"/>
       <c r="I8" s="124">
         <v>15.01</v>
       </c>
@@ -55691,7 +55694,7 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="H9" s="268"/>
+      <c r="H9" s="271"/>
       <c r="I9" s="124">
         <v>20.010000000000002</v>
       </c>
@@ -55780,7 +55783,7 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="H10" s="268"/>
+      <c r="H10" s="271"/>
       <c r="I10" s="124">
         <v>30.01</v>
       </c>
@@ -55873,7 +55876,7 @@
       <c r="D11">
         <v>2</v>
       </c>
-      <c r="H11" s="268"/>
+      <c r="H11" s="271"/>
       <c r="I11" s="124">
         <v>40.01</v>
       </c>
@@ -55980,7 +55983,7 @@
       <c r="D12">
         <v>3</v>
       </c>
-      <c r="H12" s="268"/>
+      <c r="H12" s="271"/>
       <c r="I12" s="124">
         <v>50.01</v>
       </c>
@@ -56074,7 +56077,7 @@
       <c r="B13" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="268"/>
+      <c r="H13" s="271"/>
       <c r="I13" s="124">
         <v>60.01</v>
       </c>
@@ -56160,7 +56163,7 @@
       <c r="B14" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="268"/>
+      <c r="H14" s="271"/>
       <c r="I14" s="124">
         <v>70.010000000000005</v>
       </c>
@@ -56257,7 +56260,7 @@
         <v>44</v>
       </c>
       <c r="D15" s="99"/>
-      <c r="H15" s="268"/>
+      <c r="H15" s="271"/>
       <c r="I15" s="124">
         <v>80.010000000000005</v>
       </c>
@@ -56345,7 +56348,7 @@
       <c r="B16" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="268"/>
+      <c r="H16" s="271"/>
       <c r="I16" s="124">
         <v>90.01</v>
       </c>
@@ -56430,7 +56433,7 @@
       <c r="B17" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="268"/>
+      <c r="H17" s="271"/>
       <c r="I17" s="124">
         <v>100.01</v>
       </c>
@@ -56520,7 +56523,7 @@
       <c r="B18" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="268"/>
+      <c r="H18" s="271"/>
       <c r="I18" s="124">
         <v>125.01</v>
       </c>
@@ -56606,7 +56609,7 @@
       <c r="B19" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="268"/>
+      <c r="H19" s="271"/>
       <c r="I19" s="124">
         <v>150.01</v>
       </c>
@@ -56686,7 +56689,7 @@
       <c r="B20" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="268"/>
+      <c r="H20" s="271"/>
       <c r="I20" s="125">
         <v>175.01</v>
       </c>
@@ -56723,7 +56726,7 @@
       <c r="B21" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="H21" s="268"/>
+      <c r="H21" s="271"/>
       <c r="I21" s="125">
         <v>200.01</v>
       </c>
@@ -56744,18 +56747,18 @@
         <f>W6+V16</f>
         <v>0</v>
       </c>
-      <c r="AA21" s="274" t="s">
+      <c r="AA21" s="269" t="s">
         <v>105</v>
       </c>
-      <c r="AB21" s="274"/>
+      <c r="AB21" s="269"/>
       <c r="AC21" s="1">
         <f>LOOKUP(V16,AA5:AA13,AD5:AD13)</f>
         <v>0</v>
       </c>
-      <c r="AH21" s="274" t="s">
+      <c r="AH21" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="AI21" s="274"/>
+      <c r="AI21" s="269"/>
       <c r="AJ21" s="1">
         <f>IF(ISERROR(LOOKUP(V18,AH5:AH17,AK5:AK17)),0,LOOKUP(V18,AH5:AH17,AK5:AK17))</f>
         <v>0</v>
@@ -56763,10 +56766,10 @@
       <c r="AO21" s="76"/>
       <c r="AP21" s="1"/>
       <c r="AQ21" s="1"/>
-      <c r="AR21" s="274" t="s">
+      <c r="AR21" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="AS21" s="274"/>
+      <c r="AS21" s="269"/>
       <c r="AT21" s="1">
         <f>IF(ISERROR(LOOKUP(V18,AR5:AR17,AU5:AU17)),0,LOOKUP(V18,AR5:AR17,AU5:AU17))</f>
         <v>0</v>
@@ -56785,7 +56788,7 @@
       <c r="B22" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="268"/>
+      <c r="H22" s="271"/>
       <c r="I22" s="125">
         <v>250.01</v>
       </c>
@@ -56837,7 +56840,7 @@
       <c r="A23" s="52">
         <v>999</v>
       </c>
-      <c r="H23" s="268"/>
+      <c r="H23" s="271"/>
       <c r="I23" s="125">
         <v>300.01</v>
       </c>
@@ -56875,7 +56878,7 @@
       <c r="AZ23" s="1"/>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H24" s="268"/>
+      <c r="H24" s="271"/>
       <c r="I24" s="126">
         <v>350.01</v>
       </c>
@@ -56906,7 +56909,7 @@
       <c r="AZ24" s="1"/>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H25" s="268"/>
+      <c r="H25" s="271"/>
       <c r="I25" s="126">
         <v>400.01</v>
       </c>
@@ -56924,36 +56927,36 @@
         <f>AZ29+AT22</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AA25" s="275" t="s">
+      <c r="AA25" s="276" t="s">
         <v>107</v>
       </c>
-      <c r="AB25" s="275"/>
-      <c r="AC25" s="275"/>
-      <c r="AD25" s="275"/>
-      <c r="AE25" s="275"/>
-      <c r="AF25" s="275"/>
-      <c r="AH25" s="276" t="s">
+      <c r="AB25" s="276"/>
+      <c r="AC25" s="276"/>
+      <c r="AD25" s="276"/>
+      <c r="AE25" s="276"/>
+      <c r="AF25" s="276"/>
+      <c r="AH25" s="267" t="s">
         <v>108</v>
       </c>
-      <c r="AI25" s="276"/>
-      <c r="AJ25" s="276"/>
-      <c r="AK25" s="276"/>
-      <c r="AL25" s="276"/>
-      <c r="AM25" s="276"/>
-      <c r="AN25" s="276"/>
-      <c r="AO25" s="276"/>
+      <c r="AI25" s="267"/>
+      <c r="AJ25" s="267"/>
+      <c r="AK25" s="267"/>
+      <c r="AL25" s="267"/>
+      <c r="AM25" s="267"/>
+      <c r="AN25" s="267"/>
+      <c r="AO25" s="267"/>
       <c r="AP25" s="1"/>
       <c r="AQ25" s="1"/>
-      <c r="AR25" s="276" t="s">
+      <c r="AR25" s="267" t="s">
         <v>108</v>
       </c>
-      <c r="AS25" s="276"/>
-      <c r="AT25" s="276"/>
-      <c r="AU25" s="276"/>
-      <c r="AV25" s="276"/>
-      <c r="AW25" s="276"/>
-      <c r="AX25" s="276"/>
-      <c r="AY25" s="276"/>
+      <c r="AS25" s="267"/>
+      <c r="AT25" s="267"/>
+      <c r="AU25" s="267"/>
+      <c r="AV25" s="267"/>
+      <c r="AW25" s="267"/>
+      <c r="AX25" s="267"/>
+      <c r="AY25" s="267"/>
       <c r="AZ25" s="1"/>
     </row>
     <row r="26" spans="1:52" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -57006,7 +57009,7 @@
       <c r="AY26" s="129"/>
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H27" s="269" t="s">
+      <c r="H27" s="272" t="s">
         <v>9</v>
       </c>
       <c r="I27" s="101">
@@ -57043,7 +57046,7 @@
       <c r="AZ27" s="1"/>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H28" s="270"/>
+      <c r="H28" s="273"/>
       <c r="I28" s="102">
         <v>9.9999999999999995E-7</v>
       </c>
@@ -57084,7 +57087,7 @@
       <c r="AZ28" s="1"/>
     </row>
     <row r="29" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H29" s="270"/>
+      <c r="H29" s="273"/>
       <c r="I29" s="102">
         <v>0.20000100000000001</v>
       </c>
@@ -57123,7 +57126,7 @@
       </c>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H30" s="270"/>
+      <c r="H30" s="273"/>
       <c r="I30" s="102">
         <v>0.400001</v>
       </c>
@@ -57231,7 +57234,7 @@
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="H31" s="270"/>
+      <c r="H31" s="273"/>
       <c r="I31" s="102">
         <v>0.60000100000000001</v>
       </c>
@@ -57339,7 +57342,7 @@
       </c>
     </row>
     <row r="32" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H32" s="271"/>
+      <c r="H32" s="274"/>
       <c r="I32" s="103">
         <v>0.80000099999999996</v>
       </c>
@@ -57450,7 +57453,7 @@
       </c>
     </row>
     <row r="33" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H33" s="268" t="s">
+      <c r="H33" s="271" t="s">
         <v>17</v>
       </c>
       <c r="I33" s="104">
@@ -57565,7 +57568,7 @@
       </c>
     </row>
     <row r="34" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H34" s="268"/>
+      <c r="H34" s="271"/>
       <c r="I34" s="104">
         <v>0.20000100000000001</v>
       </c>
@@ -57678,7 +57681,7 @@
       </c>
     </row>
     <row r="35" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H35" s="268"/>
+      <c r="H35" s="271"/>
       <c r="I35" s="104">
         <v>0.400001</v>
       </c>
@@ -57791,7 +57794,7 @@
       </c>
     </row>
     <row r="36" spans="8:52" x14ac:dyDescent="0.25">
-      <c r="H36" s="268"/>
+      <c r="H36" s="271"/>
       <c r="I36" s="104">
         <v>0.60000100000000001</v>
       </c>
@@ -57904,7 +57907,7 @@
       </c>
     </row>
     <row r="37" spans="8:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H37" s="272"/>
+      <c r="H37" s="275"/>
       <c r="I37" s="104">
         <v>0.80000099999999996</v>
       </c>
@@ -70669,11 +70672,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AR25:AY25"/>
-    <mergeCell ref="AR2:AY2"/>
-    <mergeCell ref="AS3:AU3"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AR21:AS21"/>
     <mergeCell ref="H5:H25"/>
     <mergeCell ref="H27:H32"/>
     <mergeCell ref="H33:H37"/>
@@ -70689,6 +70687,11 @@
     <mergeCell ref="AA25:AF25"/>
     <mergeCell ref="AH25:AO25"/>
     <mergeCell ref="N11:N14"/>
+    <mergeCell ref="AR25:AY25"/>
+    <mergeCell ref="AR2:AY2"/>
+    <mergeCell ref="AS3:AU3"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AR21:AS21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -71043,7 +71046,7 @@
       <c r="C19" s="82"/>
       <c r="D19" s="122">
         <f ca="1">NOW()</f>
-        <v>45008.746126851853</v>
+        <v>45014.848979861112</v>
       </c>
       <c r="E19" s="82"/>
       <c r="F19" s="82" t="s">

</xml_diff>

<commit_message>
neue Version aus oneline
</commit_message>
<xml_diff>
--- a/ExcelBlanko.xlsx
+++ b/ExcelBlanko.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\oneLine_Backoffice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\V\DATEN\BN_BSS11\T_PRO_PKG\Performance\DB Verprobung\Vertriebstool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{656C7995-4956-4C74-B86A-F70CEB8566CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="gm2dPiWxIMNsDKrisWsc5WLNjjitri0iA4syQpFqL5RaTEuj7VAd2m49uxgfC9kizD2K5A2upTNioENqEvF98w==" workbookSaltValue="l4enb28rPm+jfY9sBLjxmw==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B6E123B-28FC-4840-953F-15553391E78B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="U6OeW677PhkCsvg060uaR0jRIVpiu2xJnEzrkOUDQNe/VgSLNLovv//MwJaNNYmjivE91VL6pryWP9UMMw1T+w==" workbookSaltValue="X8hiuY1VfA88t8tWhomzQg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="814" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12450" yWindow="1905" windowWidth="38700" windowHeight="15435" tabRatio="814" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Startseite" sheetId="15" r:id="rId1"/>
@@ -1073,7 +1073,7 @@
     </r>
   </si>
   <si>
-    <t>Gültig ab 01.04.2023</t>
+    <t>Gültig ab 11.04.2023</t>
   </si>
 </sst>
 </file>
@@ -6654,7 +6654,7 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rDIr7MXL5rTEMxNi8zBfWb3TU3wFh8y2xOXyMx7JNWxvwgviUHWidQttwbHNKCIEg51Rqs5wvLTeIeygK1vuPQ==" saltValue="JhqFqNARO6mfghGm/mFxVA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Tr68tLJvjhh0lclI5lklQewhd0tQl+zgJSYXFMLvC1s6QYr4Msn3oTKVuFeMGmUlyiUUER+27TfyhqKhLZmLkQ==" saltValue="5LMchhYLBc33iVn/YmT0zg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -22529,8 +22529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{255CCD47-8ECF-49F3-970E-FBDD02F87F6C}">
   <dimension ref="A1:AZ163"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView topLeftCell="F36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28083,7 +28083,7 @@
       </c>
       <c r="J65" s="31"/>
       <c r="K65" s="30">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="L65" s="32">
         <v>-1</v>
@@ -28093,7 +28093,7 @@
       </c>
       <c r="O65" s="30">
         <f>K65</f>
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="P65" s="32">
         <f>L65</f>
@@ -28203,7 +28203,7 @@
       </c>
       <c r="J66" s="34"/>
       <c r="K66" s="33">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="L66" s="35">
         <v>-1</v>
@@ -28213,7 +28213,7 @@
       </c>
       <c r="O66" s="33">
         <f>K66</f>
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="P66" s="35">
         <f>L66</f>
@@ -28323,7 +28323,7 @@
       </c>
       <c r="J67" s="34"/>
       <c r="K67" s="33">
-        <v>-1.3</v>
+        <v>-2</v>
       </c>
       <c r="L67" s="35">
         <v>-2.5</v>
@@ -28333,7 +28333,7 @@
       </c>
       <c r="O67" s="33">
         <f>O66</f>
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="P67" s="35">
         <f>P66</f>
@@ -28443,7 +28443,7 @@
       </c>
       <c r="J68" s="34"/>
       <c r="K68" s="33">
-        <v>-1.3</v>
+        <v>-2</v>
       </c>
       <c r="L68" s="35">
         <v>-2.5</v>
@@ -28453,7 +28453,7 @@
       </c>
       <c r="O68" s="33">
         <f t="shared" ref="O68:P70" si="34">K68</f>
-        <v>-1.3</v>
+        <v>-2</v>
       </c>
       <c r="P68" s="35">
         <f t="shared" si="34"/>
@@ -38205,7 +38205,7 @@
       <c r="C19" s="82"/>
       <c r="D19" s="122">
         <f ca="1">NOW()</f>
-        <v>45014.848979861112</v>
+        <v>45022.498831481484</v>
       </c>
       <c r="E19" s="82"/>
       <c r="F19" s="82" t="s">
@@ -38389,7 +38389,7 @@
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8CpCEHi2iB/wdzB0Lb/z5jCvw11A9lO9rETlaNvirFDYdaFk51swq0LoZbMyentEWLaeo9OtI12MB010SPcC5Q==" saltValue="CNqprhqmzpr/rDlt/Xo6jg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="wNeyTXmYAzOi/HG781SbgKQsQCePe0B/s5RffCEcHluuTs4tb6N6c6Uv39/HqvC6eAHTcd+48E7I4txN+plEVQ==" saltValue="Euv5l4o3Gi39J7xodgIAQw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="D8" name="Range6"/>
     <protectedRange sqref="D19" name="Range5"/>
@@ -38722,7 +38722,7 @@
     </row>
     <row r="23" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="2foKn/wSAnbmvYG2f0fP2sOXHQEl0giobNGFI0sYLSKmOMWmu4v1cEok9XdLdyDHH6hek6TL1LCM16skcSr/DA==" saltValue="iwXAWv/V6Isde4AGUsQnQg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="7zNha2TEYi5hVVmUgGTSWP5P8H0SVovzp3hJ2v/VlrkfB+uw+Rasnn/G9qHfkvsp2B0s2FLCWcJcFPU0NB0Avw==" saltValue="0hdeKSF9vEw/fz8aavC9tw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="C11" name="Range1"/>
   </protectedRanges>
@@ -39220,7 +39220,7 @@
       <c r="H33" s="244"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="3MA5Uu4/i5+lr7jhSWrJzk3rsvUPFqDdpEPGgE5VEPK2lfTZDtLyklJZLDVTbzeAfgT1vv19R88qd+WeI+DZMg==" saltValue="chhSDgF2OJboQGJHEz4/aA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="oAXT+M352vho6cdk+GKADXO7xXSxAZobwb0af7ifpqb7bWfsp2bmjr5lJiYzRofdPbtccU1tMy9C2t4wWgMOHA==" saltValue="DWCAuZI/AZA3g/BTH11E/A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="B5:B7" name="Bereich1"/>
   </protectedRanges>
@@ -55114,7 +55114,9 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AZ172"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O67" sqref="O67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -60968,7 +60970,7 @@
       </c>
       <c r="J65" s="31"/>
       <c r="K65" s="30">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="L65" s="32">
         <v>-1</v>
@@ -60978,7 +60980,7 @@
       </c>
       <c r="O65" s="30">
         <f>K65</f>
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="P65" s="32">
         <f>L65</f>
@@ -61089,7 +61091,7 @@
       </c>
       <c r="J66" s="34"/>
       <c r="K66" s="33">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="L66" s="35">
         <v>-1</v>
@@ -61099,7 +61101,7 @@
       </c>
       <c r="O66" s="33">
         <f>K66</f>
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="P66" s="35">
         <f>L66</f>
@@ -61210,7 +61212,7 @@
       </c>
       <c r="J67" s="34"/>
       <c r="K67" s="33">
-        <v>-1.3</v>
+        <v>-2</v>
       </c>
       <c r="L67" s="35">
         <v>-2.5</v>
@@ -61220,7 +61222,7 @@
       </c>
       <c r="O67" s="33">
         <f>O66</f>
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="P67" s="35">
         <f>P66</f>
@@ -61331,7 +61333,7 @@
       </c>
       <c r="J68" s="34"/>
       <c r="K68" s="33">
-        <v>-1.3</v>
+        <v>-2</v>
       </c>
       <c r="L68" s="35">
         <v>-2.5</v>
@@ -61341,7 +61343,7 @@
       </c>
       <c r="O68" s="33">
         <f t="shared" ref="O68:P70" si="34">K68</f>
-        <v>-1.3</v>
+        <v>-2</v>
       </c>
       <c r="P68" s="35">
         <f t="shared" si="34"/>
@@ -71046,7 +71048,7 @@
       <c r="C19" s="82"/>
       <c r="D19" s="122">
         <f ca="1">NOW()</f>
-        <v>45014.848979861112</v>
+        <v>45022.498831481484</v>
       </c>
       <c r="E19" s="82"/>
       <c r="F19" s="82" t="s">

</xml_diff>

<commit_message>
neue Version ab 15.9.
</commit_message>
<xml_diff>
--- a/ExcelBlanko.xlsx
+++ b/ExcelBlanko.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luk130\OneDrive - Deutsche Bank AG\Backoffice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deutschebank-my.sharepoint.com/personal/kerstin_stein_db_com/Documents/Backoffice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3799C6F3-0645-4ADD-A09B-2130C2612043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="4WUuFQo3TFtO2ZDnsWgPOMCWvjV1I5GpyR7OiMoy0AarlTS2khtGcBls6kS/MjqMXAHEoiK1Dy1usQKJOHh8pQ==" workbookSaltValue="3DvrHNnh5B7ScaOiurXTaA==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CDBEC78-B3DC-4EE2-BB01-8EDF229BFC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="aAM27QD5Wrb878yYK9U9KS9IjI9dlWWgnq1ydCKZE9blqlqEZWUG7X6H7mXegXSf2VwQTTN1iWkIhfSU9lf2sw==" workbookSaltValue="t/eGG2kYKX0l0gn4GNWevg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="814" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,25 +37,26 @@
     <definedName name="Anzahl_der_Raten">Kalkulationstool!$D$8</definedName>
     <definedName name="Bezahlter_RKV_Einmalbeitrag_für_den_Altkredit">'Bewertung Aufstockung'!$B$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">Kalk_Kredit2!$A$1:$R$26</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Kalkulationstool!$A$1:$R$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Kalkulationstool!$A$1:$R$27</definedName>
     <definedName name="Eigenablösebetrag" localSheetId="13">[1]Kalkulationstool!$D$11</definedName>
     <definedName name="Eigenablösebetrag" localSheetId="7">Kalk_Kredit2!$D$11</definedName>
-    <definedName name="Eigenablösebetrag">Kalkulationstool!$D$11</definedName>
+    <definedName name="Eigenablösebetrag_DB">Kalkulationstool!$D$11</definedName>
+    <definedName name="Eigenablösebetrag_PoBa_DSL" localSheetId="1">Kalkulationstool!$D$12</definedName>
     <definedName name="Expected_Loss" localSheetId="7">Kalk_Kredit2!$D$7</definedName>
     <definedName name="Expected_Loss">Kalkulationstool!$D$7</definedName>
     <definedName name="Fremdablösebetrag" localSheetId="7">Kalk_Kredit2!$D$12</definedName>
-    <definedName name="Fremdablösebetrag">Kalkulationstool!$D$12</definedName>
+    <definedName name="Fremdablösebetrag">Kalkulationstool!$D$13</definedName>
     <definedName name="Gesamtkreditbetrag" localSheetId="13">[1]Kalkulationstool!$D$10</definedName>
     <definedName name="Gesamtkreditbetrag" localSheetId="7">Kalk_Kredit2!$D$10</definedName>
     <definedName name="Gesamtkreditbetrag">Kalkulationstool!$D$10</definedName>
     <definedName name="Höchste_Absicherungsquote_des_Neukredits" localSheetId="13">'[1]Bewertung Aufstockung'!$B$7</definedName>
     <definedName name="Höchste_Absicherungsquote_des_Neukredits">'Bewertung Aufstockung'!$B$7</definedName>
     <definedName name="IVS" localSheetId="7">Kalk_Kredit2!$D$14</definedName>
-    <definedName name="IVS">Kalkulationstool!$D$14</definedName>
+    <definedName name="IVS">Kalkulationstool!$D$15</definedName>
     <definedName name="Konditionskompetenz_Filiale_RBC" localSheetId="7">Kalk_Kredit2!$D$26</definedName>
-    <definedName name="Konditionskompetenz_Filiale_RBC">Kalkulationstool!$D$26</definedName>
+    <definedName name="Konditionskompetenz_Filiale_RBC">Kalkulationstool!$D$27</definedName>
     <definedName name="Konditionskompetenz_MGL_LRBC_RL" localSheetId="7">Kalk_Kredit2!$H$26</definedName>
-    <definedName name="Konditionskompetenz_MGL_LRBC_RL">Kalkulationstool!$H$26</definedName>
+    <definedName name="Konditionskompetenz_MGL_LRBC_RL">Kalkulationstool!$H$27</definedName>
     <definedName name="Laufzeit_in_Monaten" localSheetId="7">Kalk_Kredit2!$D$9</definedName>
     <definedName name="Laufzeit_in_Monaten">Kalkulationstool!$D$9</definedName>
     <definedName name="Marge_Altkredit" localSheetId="8">Wert_Kredit2!$C$10</definedName>
@@ -74,12 +75,12 @@
     <definedName name="Wertbeitrag_Zielkondition" localSheetId="8">Wert_Kredit2!$C$13</definedName>
     <definedName name="Wertbeitrag_Zielkondition">Wertbeitrag!$C$13</definedName>
     <definedName name="Zielkondition_effektiv" localSheetId="7">Kalk_Kredit2!$D$20</definedName>
-    <definedName name="Zielkondition_effektiv">Kalkulationstool!$D$20</definedName>
+    <definedName name="Zielkondition_effektiv">Kalkulationstool!$D$21</definedName>
     <definedName name="Zielkondition_nominal" localSheetId="7">Kalk_Kredit2!$D$21</definedName>
-    <definedName name="Zielkondition_nominal">Kalkulationstool!$D$21</definedName>
+    <definedName name="Zielkondition_nominal">Kalkulationstool!$D$22</definedName>
     <definedName name="Zuführer" localSheetId="13">[1]Kalkulationstool!$D$13</definedName>
     <definedName name="Zuführer" localSheetId="7">Kalk_Kredit2!$D$13</definedName>
-    <definedName name="Zuführer">Kalkulationstool!$D$13</definedName>
+    <definedName name="Zuführer">Kalkulationstool!$D$14</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentManualCount="2"/>
   <extLst>
@@ -97,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="250">
   <si>
     <t>MOVE</t>
   </si>
@@ -331,9 +332,6 @@
     <t>Anzahl der vertraglich definierten Raten (nicht die Vertragslaufzeit)</t>
   </si>
   <si>
-    <t>Ausstehender Kreditbetrag des abzulösenden Kredits zum Zeitpunkt der Ablöse</t>
-  </si>
-  <si>
     <t>Beim Wettbewerb abzulösender Kreditbetrag zum Zeitpunkt der Ablöse</t>
   </si>
   <si>
@@ -444,9 +442,6 @@
   </si>
   <si>
     <t>Was trage ich bei einer Fremdablösung ein?</t>
-  </si>
-  <si>
-    <t>Es ist der Gesamtkreditbetrag entsprechend des neuen Kreditvertrags einzutragen (Zelle D10). Der Fremdablöse-Anteil ist in Zelle D12 einzutragen. Sollte keine Fremdablösung vorliegen, ist hier eine 0 einzutragen.</t>
   </si>
   <si>
     <t>Aktion Q1</t>
@@ -611,33 +606,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Es ist der Gesamtkreditbetrag entsprechend des neuen Kreditvertrags einzutragen (Zelle D10) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ohne Abzug des Ablöseanteils</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Der Ablöseanteil ist separat in dem dafür vorgesehenen Feld auszuweisen (Zelle D11). Sollte keine Aufstockung vorliegen, ist hier eine 0 einzutragen. Im FilialKompass ist das Geschäft nach Abschluss wie üblich einzutragen (das Excel-Tool führt hier zu keinen Veränderungen).
-Im Tabellenblatt "Wertbeitrag" sind ensprechend die Marge des Altkredits sowie Restlaufzeit in Monaten einzutragen</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Erläuterung </t>
     </r>
     <r>
@@ -689,10 +657,6 @@
   </si>
   <si>
     <t>Ein interner Verrechnungssatz von 0,10% wird hier mit 10 Basispunkten eingetragen</t>
-  </si>
-  <si>
-    <t>Dieser ist analog zur Berechnung der Marge im FilialKompass einzugeben. D.h. bei Errechnung der Marge für den FilialKompass ziehen Sie den internen Verrechnungssatz vom Nominalzins ab. Im Tool sollte dieser in Basispunkten eingegeben werden (Zelle 14).
-Die tagesaktuellen internen Verrechnungssätze (IVS) sind dem Tradefinder zu entnehmen.</t>
   </si>
   <si>
     <t>Systemseitig berechneter EL p.a. in Basispunkten</t>
@@ -810,9 +774,6 @@
   </si>
   <si>
     <t>Auf die Zielkondition dürfen bis zu 150 Basispunkte aufgeschlagen werden. Bei Aufstockergeschäften ist ein Aufschlag bis zu 300 Basispunkte erlaubt.</t>
-  </si>
-  <si>
-    <t>Die neue absolute Preisuntergrenze liegt bei 3,99% eff. nach Konditionskompetenzen, bei DVAG-Geschäften bei 4,49% eff. (Ausnahme: RL-Sonderkondition)</t>
   </si>
   <si>
     <t>Bezogen auf das neue (=aufgestockte) Kreditvolumen; bei mehreren Bausteinen gilt die höchste Absicherungsquote; Achtung: Eingabe in KFPK bei Delta-Variante abweichend (da bezogen auf den Gesamtkredit)</t>
@@ -1047,8 +1008,72 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">     davon: Fremdablöse-Betrag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     davon: Eigenablöse-Betrag DB</t>
+  </si>
+  <si>
+    <t>Ablösebetrag DB</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Bitte beachten Sie das das Kalkulationstool nur eine </t>
+      <t xml:space="preserve">Ausstehender Kreditbetrag des abzulösenden Kredits der Marke </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Deutsche Bank</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zum Zeitpunkt der Ablöse</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">     davon: Eigenablöse-Betrag PoBa / DSL</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ausstehender Kreditbetrag des abzulösenden Kredits der Marke </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Postbank / DSL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zum Zeitpunkt der Ablöse</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bitte beachten Sie, dass das Kalkulationstool nur eine </t>
     </r>
     <r>
       <rPr>
@@ -1073,7 +1098,47 @@
     </r>
   </si>
   <si>
-    <t>Gültig ab 19.07.2023</t>
+    <t>Bitte beachten Sie, dass bei der Wertbeitragsermittlung im Falle einer Eigenablöse nur der abzulösende Kredit der Marge Deutsche Bank berücksichtigt wird.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Es ist der Gesamtkreditbetrag entsprechend des neuen Kreditvertrags einzutragen (Zelle D10) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ohne Abzug des Ablöseanteils</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Der Ablöseanteil ist separat in dem dafür vorgesehenen Feld auszuweisen (Zelle D11/D12). Sollte keine Aufstockung vorliegen, ist hier eine 0 einzutragen. Im FilialKompass ist das Geschäft nach Abschluss wie üblich einzutragen (das Excel-Tool führt hier zu keinen Veränderungen).
+Im Tabellenblatt "Wertbeitrag" sind ensprechend die Marge des Altkredits sowie Restlaufzeit in Monaten einzutragen</t>
+    </r>
+  </si>
+  <si>
+    <t>Es ist der Gesamtkreditbetrag entsprechend des neuen Kreditvertrags einzutragen (Zelle D10). Der Fremdablöse-Anteil ist in Zelle D13 einzutragen. Sollte keine Fremdablösung vorliegen, ist hier eine 0 einzutragen.</t>
+  </si>
+  <si>
+    <t>Dieser ist analog zur Berechnung der Marge im FilialKompass einzugeben. D.h. bei Errechnung der Marge für den FilialKompass ziehen Sie den internen Verrechnungssatz vom Nominalzins ab. Im Tool sollte dieser in Basispunkten eingegeben werden (Zelle D15).
+Die tagesaktuellen internen Verrechnungssätze (IVS) sind dem Tradefinder zu entnehmen.</t>
+  </si>
+  <si>
+    <t>Gültig ab 15.09.2023</t>
+  </si>
+  <si>
+    <t>Die neue absolute Preisuntergrenze liegt bei 4,49% eff. nach Konditionskompetenzen, bei DVAG-Geschäften bei 4,99% eff. (Ausnahme: RL-Sonderkondition)</t>
   </si>
 </sst>
 </file>
@@ -6585,7 +6650,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -6604,12 +6669,12 @@
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="71" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="182" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C3" s="96"/>
     </row>
@@ -6626,7 +6691,7 @@
         <v>73</v>
       </c>
       <c r="C5" s="90" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="60" x14ac:dyDescent="0.25">
@@ -6634,7 +6699,7 @@
         <v>74</v>
       </c>
       <c r="C6" s="90" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -6642,7 +6707,7 @@
         <v>71</v>
       </c>
       <c r="C7" s="90" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="60" x14ac:dyDescent="0.25">
@@ -6650,15 +6715,15 @@
         <v>69</v>
       </c>
       <c r="C8" s="90" t="s">
-        <v>162</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="95" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="90" t="s">
-        <v>115</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="45" x14ac:dyDescent="0.25">
@@ -6666,12 +6731,12 @@
         <v>70</v>
       </c>
       <c r="C10" s="90" t="s">
-        <v>177</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="L4CBpg2xv7d3PtpNnmIXSgsE7tWeppnTp0v/Q76PDRHHVtUx83ZW1ztuHtImZwBKirxfHms5HjSVCj9sokjz7w==" saltValue="h62Vgdm8WZLRKRCVrqiXeA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="/rH6nDBNoAnMb6FVfBz+Cu6UV5ecwBfifhEFFWLFw9jx0JGK815G5rNxCK7PeNyXBPfyKnW25+ld4IywYgc7Kw==" saltValue="t/LVrOSpmoDuZSH5wWf+zQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -6696,12 +6761,12 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B2">
         <f>'Bewertung Aufstockung'!B6</f>
@@ -6710,7 +6775,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B3">
         <f>'Bewertung Aufstockung'!B6-Wertbeitrag!C11</f>
@@ -6719,7 +6784,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B4">
         <v>0.88</v>
@@ -6727,7 +6792,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B5" s="231">
         <v>0.55000000000000004</v>
@@ -6735,7 +6800,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B6" s="232">
         <f>'Bewertung Aufstockung'!B5</f>
@@ -6744,7 +6809,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B7" s="233" t="e">
         <f>(B2-B3)*(B2-B3+1)/B2/(B2+1)*B4*B6*B5</f>
@@ -6753,10 +6818,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C26" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -6767,7 +6832,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B27" s="240">
         <f>2.3%+C27+D27+E27</f>
@@ -6826,7 +6891,7 @@
   <sheetData>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F3" s="265" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G3" s="265"/>
       <c r="H3" s="265"/>
@@ -6838,7 +6903,7 @@
       <c r="N3" s="170"/>
       <c r="O3" s="170"/>
       <c r="U3" s="265" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V3" s="265"/>
       <c r="W3" s="265"/>
@@ -6850,29 +6915,29 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="266" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B4" s="266"/>
       <c r="C4" s="266"/>
       <c r="D4" s="266"/>
       <c r="E4" s="168"/>
       <c r="F4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>23</v>
@@ -6881,40 +6946,40 @@
         <v>23</v>
       </c>
       <c r="P4" s="266" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Q4" s="266"/>
       <c r="R4" s="266"/>
       <c r="S4" s="266"/>
       <c r="T4" s="168"/>
       <c r="U4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C5" s="119">
         <f>Kalk_Kredit2!D10</f>
@@ -6946,7 +7011,7 @@
       </c>
       <c r="O5" s="171"/>
       <c r="P5" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R5" s="221">
         <v>0</v>
@@ -7021,7 +7086,7 @@
       </c>
       <c r="O6" s="176"/>
       <c r="P6" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R6" s="1">
         <f>Wertbeitrag!C11</f>
@@ -7061,7 +7126,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" s="79" t="e">
         <f>Wert_Kredit2!C6</f>
@@ -7104,7 +7169,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R7" s="79">
         <f>Wertbeitrag!C10</f>
@@ -7149,7 +7214,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C8" s="79" t="e">
         <f>EFFECT(C7,12)</f>
@@ -7253,7 +7318,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R9" s="132" t="e">
         <f>-PMT(R7/12,R6,R5)</f>
@@ -7293,7 +7358,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="132" t="e">
         <f>-PMT(C7/12,C6,C5)</f>
@@ -7360,7 +7425,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="132">
         <f>Kalk_Kredit2!D14</f>
@@ -7423,7 +7488,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C12" s="218" t="e">
         <f>C7-(C11/10000)</f>
@@ -7728,7 +7793,7 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B17" s="219" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
@@ -7790,7 +7855,7 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B18" s="120">
         <f>IF(Kalk_Kredit2!D13="MoVe",0.75,1)</f>
@@ -14702,7 +14767,7 @@
   <sheetData>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F3" s="265" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G3" s="265"/>
       <c r="H3" s="265"/>
@@ -14714,7 +14779,7 @@
       <c r="N3" s="170"/>
       <c r="O3" s="170"/>
       <c r="U3" s="265" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V3" s="265"/>
       <c r="W3" s="265"/>
@@ -14726,29 +14791,29 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="266" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B4" s="266"/>
       <c r="C4" s="266"/>
       <c r="D4" s="266"/>
       <c r="E4" s="168"/>
       <c r="F4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>23</v>
@@ -14757,40 +14822,40 @@
         <v>23</v>
       </c>
       <c r="P4" s="266" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Q4" s="266"/>
       <c r="R4" s="266"/>
       <c r="S4" s="266"/>
       <c r="T4" s="168"/>
       <c r="U4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C5" s="119">
         <f>Kalk_Kredit2!D10</f>
@@ -14823,7 +14888,7 @@
       <c r="N5" s="171"/>
       <c r="O5" s="171"/>
       <c r="P5" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R5" s="221">
         <v>0</v>
@@ -14893,7 +14958,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R6" s="1">
         <f>Wertbeitrag!C11</f>
@@ -14933,7 +14998,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" s="79" t="e">
         <f>Background2!P7</f>
@@ -14977,7 +15042,7 @@
       </c>
       <c r="O7" s="176"/>
       <c r="P7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R7" s="79">
         <f>Wertbeitrag!C10</f>
@@ -15022,7 +15087,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C8" s="79" t="e">
         <f>EFFECT(C7,12)</f>
@@ -15126,7 +15191,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R9" s="132" t="e">
         <f>-PMT(R7/12,R6,R5)</f>
@@ -15166,7 +15231,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="132" t="e">
         <f>-PMT(C7/12,C6,C5)</f>
@@ -15233,7 +15298,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="132">
         <f>Kalk_Kredit2!D14</f>
@@ -15296,7 +15361,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C12" s="218" t="e">
         <f>C7-(C11/10000)</f>
@@ -15601,7 +15666,7 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B17" s="219" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
@@ -15663,7 +15728,7 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B18" s="120">
         <f>IF(Kalk_Kredit2!D13="MoVe",0.75,1)</f>
@@ -22546,8 +22611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{255CCD47-8ECF-49F3-970E-FBDD02F87F6C}">
   <dimension ref="A1:AZ163"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView topLeftCell="E45" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22624,7 +22689,7 @@
       <c r="J2" s="25"/>
       <c r="K2" s="25"/>
       <c r="AA2" s="265" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AB2" s="265"/>
       <c r="AC2" s="265"/>
@@ -22632,7 +22697,7 @@
       <c r="AE2" s="265"/>
       <c r="AF2" s="265"/>
       <c r="AH2" s="265" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AI2" s="265"/>
       <c r="AJ2" s="265"/>
@@ -22642,7 +22707,7 @@
       <c r="AN2" s="265"/>
       <c r="AO2" s="265"/>
       <c r="AR2" s="265" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AS2" s="265"/>
       <c r="AT2" s="265"/>
@@ -22677,26 +22742,26 @@
       </c>
       <c r="L3" s="23"/>
       <c r="U3" s="266" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V3" s="266"/>
       <c r="W3" s="266"/>
       <c r="AB3" s="273" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC3" s="273"/>
       <c r="AD3" s="273"/>
       <c r="AE3" s="108"/>
       <c r="AF3" s="108"/>
       <c r="AI3" s="273" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AJ3" s="273"/>
       <c r="AK3" s="273"/>
       <c r="AL3" s="108"/>
       <c r="AM3" s="108"/>
       <c r="AS3" s="273" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AT3" s="273"/>
       <c r="AU3" s="273"/>
@@ -22720,12 +22785,12 @@
         <v>8</v>
       </c>
       <c r="I4" s="22">
-        <v>9.69</v>
+        <v>10.19</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="8"/>
       <c r="U4" s="109" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V4" s="110"/>
       <c r="W4" s="111">
@@ -22733,25 +22798,25 @@
         <v>0</v>
       </c>
       <c r="AB4" s="274" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AC4" s="274"/>
       <c r="AD4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI4" s="274" t="s">
         <v>90</v>
-      </c>
-      <c r="AI4" s="274" t="s">
-        <v>91</v>
       </c>
       <c r="AJ4" s="274"/>
       <c r="AK4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AS4" s="274" t="s">
         <v>90</v>
-      </c>
-      <c r="AS4" s="274" t="s">
-        <v>91</v>
       </c>
       <c r="AT4" s="274"/>
       <c r="AU4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.25">
@@ -22772,7 +22837,7 @@
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="12">
-        <v>-1.3</v>
+        <v>-1.8</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>25</v>
@@ -22830,7 +22895,7 @@
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="13">
-        <v>-1.1000000000000001</v>
+        <v>-1.5</v>
       </c>
       <c r="L6" s="120">
         <v>6</v>
@@ -22839,12 +22904,12 @@
         <v>55</v>
       </c>
       <c r="P6" s="78" t="e">
-        <f>IF((Background2!$I$4+LOOKUP(Kalk_Kredit2!$D$7,Background2!$I$5:$I$26,Background2!$K$5:$K$26)+LOOKUP(Kalk_Kredit2!$D$10,Background2!$I$38:$I$45,Background2!$K$38:$K$45)+LOOKUP((Kalk_Kredit2!$D$11/Kalk_Kredit2!$D$10),Background2!$I$27:$I$32,Background2!$K$27:$K$32)+LOOKUP((Kalk_Kredit2!$D$12/Kalk_Kredit2!$D$10),Background2!$I$33:$I$37,Background2!$K$33:$K$37)+LOOKUP(Kalk_Kredit2!$D$8,Background2!$I$48:$I$53,Background2!$K$48:$K$53))&gt;Background2!$K$60,Background2!$K$60,IF((Background2!$I$4+LOOKUP(Kalk_Kredit2!$D$7,Background2!$I$5:$I$26,Background2!$K$5:$K$26)+LOOKUP(Kalk_Kredit2!$D$10,Background2!$I$38:$I$45,Background2!$K$38:$K$45)+LOOKUP((Kalk_Kredit2!$D$11/Kalk_Kredit2!$D$10),Background2!$I$27:$I$32,Background2!$K$27:$K$32)+LOOKUP((Kalk_Kredit2!$D$12/Kalk_Kredit2!$D$10),Background2!$I$33:$I$37,Background2!$K$33:$K$37)+LOOKUP(Kalk_Kredit2!$D$8,Background2!$I$48:$I$53,Background2!$K$48:$K$53))&lt;Background2!$K$61,Background2!$K$61,Background2!$I$4+LOOKUP(Kalk_Kredit2!$D$7,Background2!$I$5:$I$26,Background2!$K$5:$K$26)+LOOKUP(Kalk_Kredit2!$D$10,Background2!$I$38:$I$45,Background2!$K$38:$K$45)+LOOKUP((Kalk_Kredit2!$D$11/Kalk_Kredit2!$D$10),Background2!$I$27:$I$32,Background2!$K$27:$K$32)+LOOKUP((Kalk_Kredit2!$D$12/Kalk_Kredit2!$D$10),Background2!$I$33:$I$37,Background2!$K$33:$K$37)+LOOKUP(Kalk_Kredit2!$D$8,Background2!$I$48:$I$53,Background2!$K$48:$K$53)))/100</f>
+        <f>IF((Background2!$I$4+LOOKUP(Kalk_Kredit2!$D$7,Background2!$I$5:$I$26,Background2!$K$5:$K$26)+LOOKUP(Kalk_Kredit2!$D$10,Background2!$I$38:$I$45,Background2!$K$38:$K$45)+LOOKUP((SUM(Kalk_Kredit2!$D$11,Kalk_Kredit2!$D$12)/Kalk_Kredit2!$D$10),Background2!$I$27:$I$32,Background2!$K$27:$K$32)+LOOKUP((Kalk_Kredit2!$D$12/Kalk_Kredit2!$D$10),Background2!$I$33:$I$37,Background2!$K$33:$K$37)+LOOKUP(Kalk_Kredit2!$D$8,Background2!$I$48:$I$53,Background2!$K$48:$K$53))&gt;Background2!$K$60,Background2!$K$60,IF((Background2!$I$4+LOOKUP(Kalk_Kredit2!$D$7,Background2!$I$5:$I$26,Background2!$K$5:$K$26)+LOOKUP(Kalk_Kredit2!$D$10,Background2!$I$38:$I$45,Background2!$K$38:$K$45)+LOOKUP((SUM(Kalk_Kredit2!$D$11,Kalk_Kredit2!$D$12)/Kalk_Kredit2!$D$10),Background2!$I$27:$I$32,Background2!$K$27:$K$32)+LOOKUP((Kalk_Kredit2!$D$12/Kalk_Kredit2!$D$10),Background2!$I$33:$I$37,Background2!$K$33:$K$37)+LOOKUP(Kalk_Kredit2!$D$8,Background2!$I$48:$I$53,Background2!$K$48:$K$53))&lt;Background2!$K$61,Background2!$K$61,Background2!$I$4+LOOKUP(Kalk_Kredit2!$D$7,Background2!$I$5:$I$26,Background2!$K$5:$K$26)+LOOKUP(Kalk_Kredit2!$D$10,Background2!$I$38:$I$45,Background2!$K$38:$K$45)+LOOKUP((SUM(Kalk_Kredit2!$D$11,Kalk_Kredit2!$D$12)/Kalk_Kredit2!$D$10),Background2!$I$27:$I$32,Background2!$K$27:$K$32)+LOOKUP((Kalk_Kredit2!$D$12/Kalk_Kredit2!$D$10),Background2!$I$33:$I$37,Background2!$K$33:$K$37)+LOOKUP(Kalk_Kredit2!$D$8,Background2!$I$48:$I$53,Background2!$K$48:$K$53)))/100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q6" s="75"/>
       <c r="U6" s="112" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V6" s="29"/>
       <c r="W6" s="113">
@@ -22910,7 +22975,7 @@
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="13">
-        <v>-0.9</v>
+        <v>-1.2</v>
       </c>
       <c r="L7" s="120">
         <v>11</v>
@@ -22923,10 +22988,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q7" s="75" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="U7" s="112" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V7" s="29"/>
       <c r="W7" s="115" t="e">
@@ -22995,14 +23060,14 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="13">
-        <v>-0.7</v>
+        <v>-0.8</v>
       </c>
       <c r="L8" s="120">
         <v>16</v>
       </c>
       <c r="Q8" s="76"/>
       <c r="U8" s="112" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V8" s="29"/>
       <c r="W8" s="113">
@@ -23071,7 +23136,7 @@
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="13">
-        <v>-0.5</v>
+        <v>-0.4</v>
       </c>
       <c r="L9" s="120">
         <v>21</v>
@@ -23147,14 +23212,14 @@
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="13">
-        <v>-0.3</v>
+        <v>-0.2</v>
       </c>
       <c r="L10" s="120">
         <v>31</v>
       </c>
       <c r="Q10" s="76"/>
       <c r="U10" s="112" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V10" s="29"/>
       <c r="W10" s="130" t="e">
@@ -23227,7 +23292,7 @@
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="13">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="120">
         <v>41</v>
@@ -23236,7 +23301,7 @@
         <v>22</v>
       </c>
       <c r="O11" s="202" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="P11" s="203" t="e">
         <f ca="1">LOOKUP(Wertbeitrag(Kalk_Kredit2!D10,Kalk_Kredit2!D9,Kalk_Kredit2!D8,(((((Kalk_Kredit2!D20+1)^(1/12))-1)*12)),Kalk_Kredit2!D14/10000,Kalk_Kredit2!D7,PMT((((Kalk_Kredit2!D20+1)^(1/12)-1)),Kalk_Kredit2!D8,-Kalk_Kredit2!D10),IF(Kalk_Kredit2!D9-Kalk_Kredit2!D8&gt;3,1,0),Kalk_Kredit2!D13)/Kalk_Kredit2!D10,Background2!I65:I70,Background2!K65:K70)/100</f>
@@ -23258,7 +23323,7 @@
         <v>0</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Y11" s="132" t="e">
         <f>PMT((((Kalk_Kredit2!D20+1)^(1/12)-1)),Kalk_Kredit2!D8,-Kalk_Kredit2!D10)</f>
@@ -23327,14 +23392,14 @@
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="13">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="L12" s="120">
         <v>51</v>
       </c>
       <c r="N12" s="278"/>
       <c r="O12" s="207" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="P12" s="208" t="str">
         <f>IF(ISNUMBER(P17),IF(Kalk_Kredit2!$D$8&gt;84,Background2!P14,Background2!P13),"")</f>
@@ -23414,14 +23479,14 @@
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="13">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="L13" s="120">
         <v>61</v>
       </c>
       <c r="N13" s="278"/>
       <c r="O13" s="29" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="P13" s="210" t="e">
         <f>LOOKUP($P$17,Background2!I65:I70,Background2!K65:K70)/100</f>
@@ -23493,14 +23558,14 @@
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="13">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="L14" s="120">
         <v>71</v>
       </c>
       <c r="N14" s="279"/>
       <c r="O14" s="196" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="P14" s="206" t="e">
         <f>LOOKUP($P$17,Background2!N65:N70,Background2!O65:O70)/100</f>
@@ -23514,14 +23579,14 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V14" s="79" t="e">
         <f>W7-W8/10000</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W14" s="118" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AA14" s="1">
         <v>9</v>
@@ -23583,27 +23648,27 @@
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="13">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="L15" s="120">
         <v>81</v>
       </c>
       <c r="N15" s="200" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O15" s="201" t="e">
         <f ca="1">Wertbeitrag(Kalk_Kredit2!D10,Kalk_Kredit2!D9,Kalk_Kredit2!D8,(((((Kalk_Kredit2!D20+1)^(1/12))-1)*12)),Kalk_Kredit2!D14/10000,Kalk_Kredit2!D7,PMT((((Kalk_Kredit2!D20+1)^(1/12)-1)),Kalk_Kredit2!D8,-Kalk_Kredit2!D10),IF(Kalk_Kredit2!D9-Kalk_Kredit2!D8&gt;3,1,0),Kalk_Kredit2!D13)</f>
         <v>#NAME?</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V15" s="119">
         <f>W4</f>
         <v>0</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AA15" s="1">
         <v>10</v>
@@ -23664,20 +23729,20 @@
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="13">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="L16" s="120">
         <v>91</v>
       </c>
       <c r="N16" s="105" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O16" s="106" t="e">
         <f ca="1">O15/Kalk_Kredit2!D10</f>
         <v>#NAME?</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="V16" s="119">
         <f>W5-W6</f>
@@ -23742,13 +23807,13 @@
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="13">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="L17" s="120">
         <v>101</v>
       </c>
       <c r="N17" s="143" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="O17" s="144" t="e">
         <f>IF(W11=1,AY27,AF27)</f>
@@ -23760,7 +23825,7 @@
       </c>
       <c r="Q17" s="79"/>
       <c r="U17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="V17" s="1">
         <f>V16*2+1</f>
@@ -23825,7 +23890,7 @@
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="13">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="L18" s="120">
         <v>126</v>
@@ -23835,14 +23900,14 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V18" s="133">
         <f>IF(W5-W6-W6/12&lt;0,1,W5-W6-W6/12)</f>
         <v>0</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AA18" s="1">
         <v>13</v>
@@ -23903,7 +23968,7 @@
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="13">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="L19" s="120">
         <v>151</v>
@@ -23975,13 +24040,13 @@
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="15">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="L20" s="120">
         <v>176</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="V20" s="1">
         <f>W6+V18+W6/12</f>
@@ -24001,7 +24066,7 @@
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="15">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="L21" s="120">
         <v>201</v>
@@ -24010,14 +24075,14 @@
       <c r="O21" s="144"/>
       <c r="P21" s="148"/>
       <c r="U21" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="V21" s="1">
         <f>W6+V16</f>
         <v>0</v>
       </c>
       <c r="AA21" s="274" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AB21" s="274"/>
       <c r="AC21" s="1">
@@ -24025,7 +24090,7 @@
         <v>0</v>
       </c>
       <c r="AH21" s="274" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AI21" s="274"/>
       <c r="AJ21" s="1">
@@ -24034,7 +24099,7 @@
       </c>
       <c r="AO21" s="76"/>
       <c r="AR21" s="274" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AS21" s="274"/>
       <c r="AT21" s="1">
@@ -24056,13 +24121,13 @@
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="15">
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L22" s="120">
         <v>251</v>
       </c>
       <c r="U22" s="134" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="V22" s="135">
         <f>IF(W5-W6&lt;5,W6-W6/12/2+2,IF(W5-W6&lt;8,W6-W6/12/2+1,(W6-W6/12/2)))</f>
@@ -24099,13 +24164,13 @@
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="15">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="L23" s="120">
         <v>301</v>
       </c>
       <c r="U23" s="136" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="V23" s="137" t="e">
         <f>AJ22+AP29</f>
@@ -24126,13 +24191,13 @@
         <v>350.01</v>
       </c>
       <c r="K24" s="15">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="L24" s="120">
         <v>351</v>
       </c>
       <c r="U24" s="136" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="V24" s="138" t="e">
         <f>V23-W5</f>
@@ -24145,20 +24210,20 @@
         <v>400.01</v>
       </c>
       <c r="K25" s="15">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="L25" s="120">
         <v>401</v>
       </c>
       <c r="U25" s="139" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="V25" s="140" t="e">
         <f>AZ29+AT22</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AA25" s="275" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AB25" s="275"/>
       <c r="AC25" s="275"/>
@@ -24166,7 +24231,7 @@
       <c r="AE25" s="275"/>
       <c r="AF25" s="275"/>
       <c r="AH25" s="276" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AI25" s="276"/>
       <c r="AJ25" s="276"/>
@@ -24176,7 +24241,7 @@
       <c r="AN25" s="276"/>
       <c r="AO25" s="276"/>
       <c r="AR25" s="276" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AS25" s="276"/>
       <c r="AT25" s="276"/>
@@ -24196,23 +24261,23 @@
       </c>
       <c r="L26" s="120"/>
       <c r="U26" s="141" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="V26" s="142" t="e">
         <f>V25-W5</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AA26" s="239" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB26" s="239" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC26" s="239" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD26" s="239" t="s">
         <v>131</v>
-      </c>
-      <c r="AB26" s="239" t="s">
-        <v>132</v>
-      </c>
-      <c r="AC26" s="239" t="s">
-        <v>134</v>
-      </c>
-      <c r="AD26" s="239" t="s">
-        <v>133</v>
       </c>
       <c r="AE26" s="239" t="s">
         <v>23</v>
@@ -24272,21 +24337,21 @@
         <v>0.1</v>
       </c>
       <c r="AA28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AF28" s="120" t="e">
         <f>SUM(AF30:AF150)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AJ28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AO28" s="120" t="e">
         <f>SUM(AO30:AO163)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AT28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AY28" s="120" t="e">
         <f>SUM(AY30:AY163)</f>
@@ -24545,7 +24610,7 @@
         <v>1.4</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AA32" s="1">
         <f t="shared" ref="AA32:AA95" si="17">1+AA31</f>
@@ -27559,7 +27624,7 @@
       </c>
       <c r="J60" s="18"/>
       <c r="K60" s="14">
-        <v>11.99</v>
+        <v>12.99</v>
       </c>
       <c r="AA60" s="1">
         <f t="shared" si="17"/>
@@ -27665,7 +27730,7 @@
       </c>
       <c r="J61" s="21"/>
       <c r="K61" s="16">
-        <v>3.99</v>
+        <v>4.49</v>
       </c>
       <c r="AA61" s="1">
         <f t="shared" si="17"/>
@@ -27867,14 +27932,14 @@
     </row>
     <row r="63" spans="8:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H63" s="24" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I63" s="24"/>
       <c r="J63" s="24"/>
       <c r="K63" s="24"/>
       <c r="L63" s="24"/>
       <c r="N63" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="AA63" s="1">
         <f t="shared" si="17"/>
@@ -37680,7 +37745,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="71" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B2" s="70"/>
     </row>
@@ -37697,7 +37762,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I5" s="249" t="str">
         <f>+'Bewertung Aufstockung'!F27</f>
@@ -37706,7 +37771,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="250" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I6" s="120" t="e">
         <f>+ROUNDUP(I5,1)</f>
@@ -37715,7 +37780,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="250" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I7" s="251" t="e">
         <f>+IF(I6=0.8,I17,VLOOKUP(I6,G10:I18,3,1))</f>
@@ -37735,13 +37800,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="G10" s="120">
         <v>0.1</v>
       </c>
       <c r="H10" s="243" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I10" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G10)-Kalkulationstool!$D$11</f>
@@ -37750,13 +37815,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="250" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G11" s="120">
         <v>0.2</v>
       </c>
       <c r="H11" s="243" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I11" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G11)-Kalkulationstool!$D$11</f>
@@ -37765,13 +37830,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="250" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G12" s="120">
         <v>0.3</v>
       </c>
       <c r="H12" s="243" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I12" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G12)-Kalkulationstool!$D$11</f>
@@ -37783,7 +37848,7 @@
         <v>0.4</v>
       </c>
       <c r="H13" s="243" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I13" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G13)-Kalkulationstool!$D$11</f>
@@ -37795,7 +37860,7 @@
         <v>0.5</v>
       </c>
       <c r="H14" s="243" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I14" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G14)-Kalkulationstool!$D$11</f>
@@ -37807,7 +37872,7 @@
         <v>0.6</v>
       </c>
       <c r="H15" s="243" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I15" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G15)-Kalkulationstool!$D$11</f>
@@ -37819,7 +37884,7 @@
         <v>0.7</v>
       </c>
       <c r="H16" s="243" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I16" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G16)-Kalkulationstool!$D$11</f>
@@ -37831,7 +37896,7 @@
         <v>0.8</v>
       </c>
       <c r="H17" s="243" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I17" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G17)-Kalkulationstool!$D$11</f>
@@ -37843,7 +37908,7 @@
         <v>0.9</v>
       </c>
       <c r="H18" s="243" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I18" s="251">
         <f>+Kalkulationstool!$D$11/(1-Aufstockungsquoten!G18)-Kalkulationstool!$D$11</f>
@@ -37863,7 +37928,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="I21" s="120" t="e">
         <f>+ROUNDDOWN(I5,1)</f>
@@ -37888,16 +37953,16 @@
     <tabColor theme="4" tint="-0.499984740745262"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
     <col min="3" max="3" width="4.140625" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="5.140625" style="1" customWidth="1"/>
@@ -37924,7 +37989,7 @@
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="71" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" s="70"/>
       <c r="D2" s="70"/>
@@ -37933,7 +37998,7 @@
       <c r="G2" s="67"/>
       <c r="Q2" s="241"/>
       <c r="R2" s="242" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="5.0999999999999996" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -37947,7 +38012,7 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="77" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F4" s="67"/>
       <c r="G4" s="67"/>
@@ -37988,7 +38053,7 @@
       </c>
       <c r="G6" s="191"/>
       <c r="H6" s="192" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I6" s="82"/>
       <c r="J6" s="82"/>
@@ -38013,7 +38078,7 @@
       </c>
       <c r="G7" s="92"/>
       <c r="H7" s="93" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="I7" s="82"/>
       <c r="J7" s="82"/>
@@ -38088,7 +38153,7 @@
       </c>
       <c r="G10" s="93"/>
       <c r="H10" s="93" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I10" s="82"/>
       <c r="J10" s="82"/>
@@ -38103,7 +38168,7 @@
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="82" t="s">
-        <v>63</v>
+        <v>238</v>
       </c>
       <c r="C11" s="82"/>
       <c r="D11" s="216"/>
@@ -38113,7 +38178,7 @@
       </c>
       <c r="G11" s="93"/>
       <c r="H11" s="93" t="s">
-        <v>77</v>
+        <v>240</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="82"/>
@@ -38126,9 +38191,9 @@
       <c r="Q11" s="82"/>
       <c r="R11" s="82"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="82" t="s">
-        <v>64</v>
+        <v>241</v>
       </c>
       <c r="C12" s="82"/>
       <c r="D12" s="216"/>
@@ -38138,7 +38203,7 @@
       </c>
       <c r="G12" s="93"/>
       <c r="H12" s="93" t="s">
-        <v>78</v>
+        <v>242</v>
       </c>
       <c r="I12" s="82"/>
       <c r="J12" s="82"/>
@@ -38153,17 +38218,17 @@
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="82" t="s">
-        <v>12</v>
+        <v>237</v>
       </c>
       <c r="C13" s="82"/>
-      <c r="D13" s="215" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="85"/>
-      <c r="F13" s="92"/>
+      <c r="D13" s="216"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="94">
+        <v>5000</v>
+      </c>
       <c r="G13" s="93"/>
       <c r="H13" s="93" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="I13" s="82"/>
       <c r="J13" s="82"/>
@@ -38176,19 +38241,19 @@
       <c r="Q13" s="82"/>
       <c r="R13" s="82"/>
     </row>
-    <row r="14" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="82" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C14" s="82"/>
-      <c r="D14" s="217"/>
+      <c r="D14" s="215" t="s">
+        <v>1</v>
+      </c>
       <c r="E14" s="85"/>
-      <c r="F14" s="92">
-        <v>10</v>
-      </c>
+      <c r="F14" s="92"/>
       <c r="G14" s="93"/>
       <c r="H14" s="93" t="s">
-        <v>176</v>
+        <v>65</v>
       </c>
       <c r="I14" s="82"/>
       <c r="J14" s="82"/>
@@ -38201,61 +38266,60 @@
       <c r="Q14" s="82"/>
       <c r="R14" s="82"/>
     </row>
-    <row r="15" spans="2:18" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="74"/>
-    </row>
-    <row r="16" spans="2:18" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="82" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="82"/>
+      <c r="D15" s="217"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="92">
+        <v>10</v>
+      </c>
+      <c r="G15" s="93"/>
+      <c r="H15" s="93" t="s">
+        <v>173</v>
+      </c>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="82"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82"/>
+      <c r="P15" s="82"/>
+      <c r="Q15" s="82"/>
+      <c r="R15" s="82"/>
+    </row>
+    <row r="16" spans="2:18" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B16"/>
+      <c r="C16"/>
       <c r="D16" s="80"/>
       <c r="E16" s="45"/>
       <c r="F16" s="74"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:18" ht="11.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="80"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="74"/>
+    </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="81" t="s">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="82"/>
-      <c r="D19" s="122">
+      <c r="C20" s="82"/>
+      <c r="D20" s="122">
         <f ca="1">NOW()</f>
-        <v>45125.744189004632</v>
-      </c>
-      <c r="E19" s="82"/>
-      <c r="F19" s="82" t="s">
-        <v>150</v>
-      </c>
-      <c r="G19" s="82"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="82"/>
-      <c r="J19" s="82"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="82"/>
-      <c r="M19" s="82"/>
-      <c r="N19" s="82"/>
-      <c r="O19" s="82"/>
-      <c r="P19" s="82"/>
-      <c r="Q19" s="82"/>
-      <c r="R19" s="82"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="82" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="82"/>
-      <c r="D20" s="184" t="str">
-        <f>IF(AND(ISNUMBER(D7),ISNUMBER(D8),ISNUMBER(D9),ISNUMBER(D10)),IF(D7&gt;780,"",Background!P6),"")</f>
-        <v/>
-      </c>
-      <c r="E20" s="87"/>
-      <c r="F20" s="100"/>
+        <v>45182.664424074072</v>
+      </c>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82" t="s">
+        <v>148</v>
+      </c>
       <c r="G20" s="82"/>
-      <c r="H20" s="93" t="s">
-        <v>216</v>
-      </c>
+      <c r="H20" s="82"/>
       <c r="I20" s="82"/>
       <c r="J20" s="82"/>
       <c r="K20" s="82"/>
@@ -38269,17 +38333,19 @@
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="82" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" s="82"/>
-      <c r="D21" s="185" t="str">
-        <f>IF(D20="","",ROUND(NOMINAL(Kalkulationstool!D20,12),4))</f>
+      <c r="D21" s="184" t="str">
+        <f>IF(AND(ISNUMBER(D7),ISNUMBER(D8),ISNUMBER(D9),ISNUMBER(D10)),IF(D7&gt;780,"",Background!P6),"")</f>
         <v/>
       </c>
       <c r="E21" s="87"/>
-      <c r="F21" s="82"/>
+      <c r="F21" s="100"/>
       <c r="G21" s="82"/>
-      <c r="H21" s="93"/>
+      <c r="H21" s="93" t="s">
+        <v>212</v>
+      </c>
       <c r="I21" s="82"/>
       <c r="J21" s="82"/>
       <c r="K21" s="82"/>
@@ -38292,18 +38358,23 @@
       <c r="R21" s="82"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="82"/>
+      <c r="B22" s="82" t="s">
+        <v>79</v>
+      </c>
       <c r="C22" s="82"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="82"/>
+      <c r="D22" s="185" t="str">
+        <f>IF(D21="","",ROUND(NOMINAL(Kalkulationstool!D21,12),4))</f>
+        <v/>
+      </c>
+      <c r="E22" s="87"/>
       <c r="F22" s="82"/>
       <c r="G22" s="82"/>
-      <c r="H22" s="82"/>
+      <c r="H22" s="93"/>
       <c r="I22" s="82"/>
       <c r="J22" s="82"/>
       <c r="K22" s="82"/>
       <c r="L22" s="82"/>
-      <c r="M22" s="88"/>
+      <c r="M22" s="82"/>
       <c r="N22" s="82"/>
       <c r="O22" s="82"/>
       <c r="P22" s="82"/>
@@ -38313,20 +38384,16 @@
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="82"/>
       <c r="C23" s="82"/>
-      <c r="D23" s="259" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="260"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="82"/>
       <c r="F23" s="82"/>
       <c r="G23" s="82"/>
-      <c r="H23" s="180" t="s">
-        <v>22</v>
-      </c>
+      <c r="H23" s="82"/>
       <c r="I23" s="82"/>
       <c r="J23" s="82"/>
       <c r="K23" s="82"/>
       <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
+      <c r="M23" s="88"/>
       <c r="N23" s="82"/>
       <c r="O23" s="82"/>
       <c r="P23" s="82"/>
@@ -38336,14 +38403,14 @@
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="82"/>
       <c r="C24" s="82"/>
-      <c r="D24" s="261" t="s">
-        <v>152</v>
-      </c>
-      <c r="E24" s="262"/>
+      <c r="D24" s="259" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="260"/>
       <c r="F24" s="82"/>
       <c r="G24" s="82"/>
-      <c r="H24" s="181" t="s">
-        <v>153</v>
+      <c r="H24" s="180" t="s">
+        <v>22</v>
       </c>
       <c r="I24" s="82"/>
       <c r="J24" s="82"/>
@@ -38356,14 +38423,18 @@
       <c r="Q24" s="82"/>
       <c r="R24" s="82"/>
     </row>
-    <row r="25" spans="2:18" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="82"/>
       <c r="C25" s="82"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="82"/>
+      <c r="D25" s="261" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="262"/>
       <c r="F25" s="82"/>
       <c r="G25" s="82"/>
-      <c r="H25" s="82"/>
+      <c r="H25" s="181" t="s">
+        <v>151</v>
+      </c>
       <c r="I25" s="82"/>
       <c r="J25" s="82"/>
       <c r="K25" s="82"/>
@@ -38375,25 +38446,15 @@
       <c r="Q25" s="82"/>
       <c r="R25" s="82"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="82" t="s">
-        <v>66</v>
-      </c>
+    <row r="26" spans="2:18" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="82"/>
       <c r="C26" s="82"/>
-      <c r="D26" s="263" t="str">
-        <f>IF(ISNUMBER(D20),Background!P12,"")</f>
-        <v/>
-      </c>
-      <c r="E26" s="264"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="82"/>
       <c r="F26" s="82"/>
       <c r="G26" s="82"/>
-      <c r="H26" s="186" t="str">
-        <f>IF(ISNUMBER(D20),Background!T12,"")</f>
-        <v/>
-      </c>
-      <c r="I26" s="91" t="s">
-        <v>217</v>
-      </c>
+      <c r="H26" s="82"/>
+      <c r="I26" s="82"/>
       <c r="J26" s="82"/>
       <c r="K26" s="82"/>
       <c r="L26" s="82"/>
@@ -38404,37 +38465,66 @@
       <c r="Q26" s="82"/>
       <c r="R26" s="82"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="82" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="82"/>
+      <c r="D27" s="263" t="str">
+        <f>IF(ISNUMBER(D21),Background!P12,"")</f>
+        <v/>
+      </c>
+      <c r="E27" s="264"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="186" t="str">
+        <f>IF(ISNUMBER(D21),Background!T12,"")</f>
+        <v/>
+      </c>
+      <c r="I27" s="91" t="s">
+        <v>249</v>
+      </c>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="82"/>
+      <c r="N27" s="82"/>
+      <c r="O27" s="82"/>
+      <c r="P27" s="82"/>
+      <c r="Q27" s="82"/>
+      <c r="R27" s="82"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9rs3Twp0Qxo3xLQVeq9B1Ee4TriI/Lz221yMRenO+HaFOBCrrrZmR1y2j65y4GKiZssdTSNZWyJSU1/dCPtOdA==" saltValue="vH8OjAUfBNQdxWqkIXJt6w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="i3wrhqIQva1x5gnzViW3v92VJZa+gT0jX2Z85mEAjSI4hb9HrpT+X8GOovj+sc8pFvLxcuH7rO0RifGMTFJ3mg==" saltValue="HS1bT1xgAAy1cLSDiO8VCQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="D8" name="Range6"/>
-    <protectedRange sqref="D19" name="Range5"/>
-    <protectedRange sqref="D7 D9:D14" name="Range1"/>
-    <protectedRange sqref="D20:D21" name="Range2"/>
-    <protectedRange sqref="D26" name="Range3"/>
-    <protectedRange sqref="H26" name="Range4"/>
-    <protectedRange sqref="I26" name="Range7"/>
+    <protectedRange sqref="D20" name="Range5"/>
+    <protectedRange sqref="D7 D9:D15" name="Range1"/>
+    <protectedRange sqref="D21:D22" name="Range2"/>
+    <protectedRange sqref="D27" name="Range3"/>
+    <protectedRange sqref="H27" name="Range4"/>
+    <protectedRange sqref="I27" name="Range7"/>
   </protectedRanges>
   <mergeCells count="3">
-    <mergeCell ref="D23:E23"/>
     <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D27:E27"/>
   </mergeCells>
-  <dataValidations count="11">
+  <dataValidations count="12">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>1</formula1>
       <formula2>84</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E11" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E12" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>0</formula1>
       <formula2>75000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>0</formula1>
       <formula2>75000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Bitte überprüfen Sie die Eingabe" error="Bitte geben Sie den internen Verrechnungssatz in Basispunkten ein d.h. für 0,10 dann 10 Basispunkte!" sqref="D14" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Bitte überprüfen Sie die Eingabe" error="Bitte geben Sie den internen Verrechnungssatz in Basispunkten ein d.h. für 0,10 dann 10 Basispunkte!" sqref="D15" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>0</formula1>
       <formula2>999</formula2>
     </dataValidation>
@@ -38442,20 +38532,20 @@
       <formula1>D8</formula1>
       <formula2>D8+10+4</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15" xr:uid="{00000000-0002-0000-0100-000005000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>0</formula1>
       <formula2>199</formula2>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Bitte überprüfen Sie die Eingabe" error="Die maximal zulässige Anzahl an Raten oder der maximal zulässige EL wurden überschritten." sqref="D8" xr:uid="{00000000-0002-0000-0100-000006000000}">
       <formula1>IF($D$7&lt;=780,AND($D$8&lt;=120,$D$8&gt;=1),AND($D$8&lt;=120,$D$8&gt;=1,$D$7&lt;=780))</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Bitte überprüfen Sie die Eingabe" error="Der Fremdablöse-Betrag darf nicht größer sein als der Gesamtkreditbetrag abzüglich der Eigenablöse (wenn relevant)!" sqref="D12" xr:uid="{00000000-0002-0000-0100-000007000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" errorTitle="Bitte überprüfen Sie die Eingabe" error="Der Fremdablöse-Betrag darf nicht größer als der Gesamtkreditbetrag abzüglich des Eigenablöse-Betrags sein." sqref="D13" xr:uid="{00000000-0002-0000-0100-000007000000}">
       <formula1>0</formula1>
-      <formula2>D10-D11</formula2>
+      <formula2>D10-IF(ISNUMBER(D11),D11,0)-IF(ISNUMBER(D12),D12,0)</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Bitte überprüfen Sie die Eingabe" error="Der Eigenablöse-Betrag darf nicht größer sein als der Gesamtkreditbetrag!" sqref="D11" xr:uid="{00000000-0002-0000-0100-000008000000}">
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" errorTitle="Bitte überprüfen Sie die Eingabe" error="Der Eigenablöse-Betrag darf nicht größer als der Gesamtkreditbetrag abzüglich des Fremdablöse-Betrags sein." sqref="D12" xr:uid="{00000000-0002-0000-0100-000008000000}">
       <formula1>0</formula1>
-      <formula2>D10</formula2>
+      <formula2>D10-IF(ISNUMBER(D11),D11,0)-IF(ISNUMBER(D13),D13,0)</formula2>
     </dataValidation>
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" errorTitle="Bitte überprüfen Sie die Eingabe" error="Der Maximalkreditbetrag beträgt 80.000€. Der Mindestkreditbetrag liegt bei 1.000€." sqref="D10" xr:uid="{00000000-0002-0000-0100-000009000000}">
       <formula1>1000</formula1>
@@ -38464,9 +38554,13 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Bitte überprüfen Sie die Eingabe" error="Bitte geben Sie hier den Expected Loss ein.  _x000a_Sie können lediglich bis zu zwei Nachkommastellen eingeben." sqref="D7" xr:uid="{00000000-0002-0000-0100-00000A000000}">
       <formula1>AND(MOD(ROUND($D$7*100,2),1)=0,$D$7&lt;999,$D$7&gt;=0)</formula1>
     </dataValidation>
+    <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" errorTitle="Bitte überprüfen Sie die Eingabe" error="Der Eigenablöse-Betrag darf nicht größer als der Gesamtkreditbetrag abzüglich des Fremdablöse-Betrags sein." sqref="D11" xr:uid="{9B701144-1442-4FB9-AF11-FB446215184E}">
+      <formula1>0</formula1>
+      <formula2>D10-IF(ISNUMBER(D12),D12,0)-IF(ISNUMBER(D13),D13,0)</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="66" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K000000</oddFooter>
   </headerFooter>
@@ -38480,13 +38574,13 @@
           <x14:formula1>
             <xm:f>Background!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E13:E14 D13</xm:sqref>
+          <xm:sqref>E14:E15 D14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
           <x14:formula1>
             <xm:f>Background!$E$3:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E15</xm:sqref>
+          <xm:sqref>E16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
           <x14:formula1>
@@ -38509,7 +38603,7 @@
     <tabColor theme="4" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:XFC23"/>
+  <dimension ref="B1:XFC24"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -38522,7 +38616,7 @@
     <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="73" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="96.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16383" width="11.42578125" style="1" hidden="1"/>
     <col min="16384" max="16384" width="21.85546875" style="1" customWidth="1"/>
   </cols>
@@ -38535,13 +38629,13 @@
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="71" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C2" s="70"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="77" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3" s="70"/>
     </row>
@@ -38553,28 +38647,28 @@
         <v>52</v>
       </c>
       <c r="D4" s="195" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E4" s="97"/>
       <c r="F4" s="98"/>
     </row>
     <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="100" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C5" s="177"/>
       <c r="D5" s="178" t="str">
-        <f>IF(Kalkulationstool!D20="","",Kalkulationstool!D20)</f>
+        <f>IF(Kalkulationstool!D21="","",Kalkulationstool!D21)</f>
         <v/>
       </c>
       <c r="E5" s="92"/>
       <c r="F5" s="93" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="150" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C6" s="164" t="str">
         <f>IF(C5&gt;0,ROUND(NOMINAL(C5,12),4),"")</f>
@@ -38583,7 +38677,7 @@
       <c r="D6" s="151"/>
       <c r="E6" s="152"/>
       <c r="F6" s="153" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -38595,7 +38689,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="81" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C8" s="84"/>
       <c r="D8" s="193" t="s">
@@ -38606,7 +38700,7 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="100" t="s">
-        <v>140</v>
+        <v>239</v>
       </c>
       <c r="C9" s="163">
         <f>IF(Kalkulationstool!D11&gt;=0,Kalkulationstool!D11,"")</f>
@@ -38615,12 +38709,12 @@
       <c r="D9" s="151"/>
       <c r="E9" s="93"/>
       <c r="F9" s="93" t="s">
-        <v>77</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="100" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C10" s="145"/>
       <c r="D10" s="146">
@@ -38628,12 +38722,12 @@
       </c>
       <c r="E10" s="92"/>
       <c r="F10" s="93" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="100" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C11" s="165"/>
       <c r="D11" s="92">
@@ -38641,7 +38735,7 @@
       </c>
       <c r="E11" s="92"/>
       <c r="F11" s="93" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -38653,7 +38747,7 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="155" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C13" s="189" t="str">
         <f>IF(ISNUMBER('Background Produktkalk I'!B15),'Background Produktkalk I'!B15,"")</f>
@@ -38665,7 +38759,7 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="155" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C14" s="190" t="str">
         <f>IF(ISNUMBER('Background WB vereinb'!B15),'Background WB vereinb'!B15,"")</f>
@@ -38695,7 +38789,7 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="160" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C17" s="154"/>
       <c r="D17" s="154"/>
@@ -38704,7 +38798,7 @@
     </row>
     <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D18" s="154"/>
       <c r="E18" s="154"/>
@@ -38712,7 +38806,7 @@
     </row>
     <row r="19" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D19" s="154"/>
       <c r="E19" s="154"/>
@@ -38720,7 +38814,7 @@
     </row>
     <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C20" s="154"/>
       <c r="D20" s="154"/>
@@ -38729,28 +38823,33 @@
     </row>
     <row r="21" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="147" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="147" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="iQ8F1lbpNsOg7R743+tK/SXNDLUiJ7tsTt/nXQPjr96WOZYt8PB/8sH7SM9UiMX6Jnz1LcOrkpfLTzyyZTzoLg==" saltValue="CnVcheKYBg+mwd2obaKW5Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="y1kZ52IX4GuPoXU0pMfPkw+c4/XNhUJ6hhkVzHWJtiOTbolq6WF28uMb7PMph+uKNWERyBmBsx0U8a0c2HQwQQ==" saltValue="htLyQkySI7B5sMAfz52tvw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="C11" name="Range1"/>
   </protectedRanges>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" errorTitle="Bitte prüfen Sie die Eingaben!" error="Übernehmen Sie die Laufzeit aus KFPK. " sqref="C11" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
       <formula2>120</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="78" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="77" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K000000</oddFooter>
   </headerFooter>
@@ -38796,7 +38895,7 @@
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="71" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B2" s="70"/>
       <c r="C2" s="244"/>
@@ -38808,7 +38907,7 @@
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B3" s="70"/>
       <c r="C3" s="244"/>
@@ -38834,14 +38933,14 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="100" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B5" s="227"/>
       <c r="C5" s="228">
         <v>840</v>
       </c>
       <c r="D5" s="93" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E5" s="228"/>
       <c r="F5" s="93"/>
@@ -38849,14 +38948,14 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="100" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B6" s="165"/>
       <c r="C6" s="229">
         <v>91</v>
       </c>
       <c r="D6" s="93" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E6" s="229"/>
       <c r="F6" s="92"/>
@@ -38864,14 +38963,14 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="100" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B7" s="226"/>
       <c r="C7" s="230">
         <v>1</v>
       </c>
       <c r="D7" s="93" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E7" s="230"/>
       <c r="F7" s="92"/>
@@ -38882,22 +38981,22 @@
     <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="81"/>
       <c r="B10" s="237" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C10" s="237"/>
       <c r="D10" s="237" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E10" s="237"/>
       <c r="F10" s="237" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G10" s="81"/>
       <c r="H10" s="247"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="155" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B11" s="234" t="str">
         <f>IFERROR(+Wert_Kredit2!Wertbeitrag_Zielkondition,"")</f>
@@ -38917,7 +39016,7 @@
     </row>
     <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="155" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B12" s="235">
         <f>IFERROR(Kalk_Kredit2!D10*B7*Kalk_RKV!B27,"")</f>
@@ -38934,7 +39033,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="93" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H12" s="244"/>
     </row>
@@ -38949,7 +39048,7 @@
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="155" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B14" s="234" t="str">
         <f>IFERROR(+B12+B11,"")</f>
@@ -38966,13 +39065,13 @@
         <v/>
       </c>
       <c r="G14" s="93" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="H14" s="244"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="245" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B15" s="236" t="str">
         <f>IFERROR(+B14-D14,"")</f>
@@ -38998,21 +39097,21 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="81"/>
       <c r="B18" s="237" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C18" s="237"/>
       <c r="D18" s="237" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E18" s="237"/>
       <c r="F18" s="237" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G18" s="81"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="155" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B19" s="234" t="str">
         <f>IFERROR(+Wert_Kredit2!Wertbeitrag_vereinbarter_Effektivzins,"")</f>
@@ -39032,7 +39131,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="155" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B20" s="235">
         <f>+B12</f>
@@ -39049,7 +39148,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="93" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -39063,7 +39162,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="155" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B22" s="234" t="str">
         <f>IFERROR(+B20+B19,"")</f>
@@ -39080,12 +39179,12 @@
         <v/>
       </c>
       <c r="G22" s="93" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="245" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B23" s="236" t="str">
         <f>IFERROR(+B22-D22,"")</f>
@@ -39124,48 +39223,48 @@
       <c r="D26" s="237"/>
       <c r="E26" s="237"/>
       <c r="F26" s="237" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G26" s="81"/>
       <c r="H26" s="247"/>
     </row>
     <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="82" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B27" s="82"/>
       <c r="C27" s="82"/>
       <c r="D27" s="82"/>
       <c r="E27" s="82"/>
       <c r="F27" s="249" t="str">
-        <f>+IFERROR((Gesamtkreditbetrag-Eigenablösebetrag)/Gesamtkreditbetrag,"")</f>
+        <f>+IFERROR((Gesamtkreditbetrag-Eigenablösebetrag_DB)/Gesamtkreditbetrag,"")</f>
         <v/>
       </c>
       <c r="G27" s="93" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="H27" s="244"/>
     </row>
     <row r="28" spans="1:8" s="255" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="252" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B28" s="253"/>
       <c r="C28" s="253"/>
       <c r="D28" s="253"/>
       <c r="E28" s="253"/>
       <c r="F28" s="254" t="str">
-        <f>+IFERROR(Gesamtkreditbetrag-Eigenablösebetrag-Gesamtkreditbetrag*Aufstockungsquoten!I21,"")</f>
+        <f>+IFERROR(Gesamtkreditbetrag-Eigenablösebetrag_DB-Gesamtkreditbetrag*Aufstockungsquoten!I21,"")</f>
         <v/>
       </c>
       <c r="G28" s="93" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H28" s="258"/>
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="81" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B29" s="82"/>
       <c r="C29" s="82"/>
@@ -39176,30 +39275,30 @@
         <v/>
       </c>
       <c r="G29" s="93" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="H29" s="244"/>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="82" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B30" s="82"/>
       <c r="C30" s="82"/>
       <c r="D30" s="82"/>
       <c r="E30" s="82"/>
       <c r="F30" s="256" t="str">
-        <f>+IFERROR(F29-(Gesamtkreditbetrag-Eigenablösebetrag),"")</f>
+        <f>+IFERROR(F29-(Gesamtkreditbetrag-Eigenablösebetrag_DB),"")</f>
         <v/>
       </c>
       <c r="G30" s="93" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="H30" s="244"/>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="81" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B31" s="82"/>
       <c r="C31" s="82"/>
@@ -39210,7 +39309,7 @@
         <v/>
       </c>
       <c r="G31" s="93" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="H31" s="244"/>
     </row>
@@ -39226,7 +39325,7 @@
     </row>
     <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="257" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B33" s="244"/>
       <c r="C33" s="244"/>
@@ -39237,7 +39336,7 @@
       <c r="H33" s="244"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="NFNn4i7e0qDMdWtxAgxNCKBwwDZ0Q2ruDX7higTQ+4BTJnY2/+NmQtWqlLOpaZVxI97Cg4QZNT8AsVySs4HBEA==" saltValue="q106HgGSgPCg3mUsdcamIQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xfC1XPYMkNsXiPH/kD7hUMGlXOzUrly4+yxSA/xDcYGBqoif/7iPd6oTFr1FE7vyO1FC0i+oxL9eAAIItzGe/g==" saltValue="2OtiQXumJq65KLjuk13wlg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="B5:B7" name="Bereich1"/>
   </protectedRanges>
@@ -39322,7 +39421,7 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F3" s="265" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G3" s="265"/>
       <c r="H3" s="265"/>
@@ -39338,7 +39437,7 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="U3" s="265" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V3" s="265"/>
       <c r="W3" s="265"/>
@@ -39350,29 +39449,29 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="266" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B4" s="266"/>
       <c r="C4" s="266"/>
       <c r="D4" s="266"/>
       <c r="E4" s="168"/>
       <c r="F4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>23</v>
@@ -39381,40 +39480,40 @@
         <v>23</v>
       </c>
       <c r="P4" s="266" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Q4" s="266"/>
       <c r="R4" s="266"/>
       <c r="S4" s="266"/>
       <c r="T4" s="168"/>
       <c r="U4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C5" s="119">
         <f>Kalkulationstool!D10</f>
@@ -39446,7 +39545,7 @@
       </c>
       <c r="O5" s="171"/>
       <c r="P5" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="119">
@@ -39525,7 +39624,7 @@
       </c>
       <c r="O6" s="176"/>
       <c r="P6" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1">
@@ -39567,7 +39666,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" s="79" t="str">
         <f>Wertbeitrag!C6</f>
@@ -39610,7 +39709,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="79">
@@ -39656,7 +39755,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C8" s="79" t="e">
         <f>EFFECT(C7,12)</f>
@@ -39763,7 +39862,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="132" t="e">
@@ -39805,7 +39904,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="132" t="e">
         <f>-PMT(C7/12,C6,C5)</f>
@@ -39877,10 +39976,10 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="132">
-        <f>Kalkulationstool!D14</f>
+        <f>Kalkulationstool!D15</f>
         <v>0</v>
       </c>
       <c r="F11" s="1">
@@ -39945,7 +40044,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C12" s="218" t="e">
         <f>C7-(C11/10000)</f>
@@ -40275,7 +40374,7 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B17" s="149" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
@@ -40342,14 +40441,14 @@
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B18" s="120">
-        <f>IF(Kalkulationstool!D13="MoVe",0.75,1)</f>
+        <f>IF(Kalkulationstool!D14="MoVe",0.75,1)</f>
         <v>1</v>
       </c>
       <c r="C18" s="120">
-        <f>IF(Kalkulationstool!D13="MoVe",0.75,1)</f>
+        <f>IF(Kalkulationstool!D14="MoVe",0.75,1)</f>
         <v>1</v>
       </c>
       <c r="F18" s="1">
@@ -40417,11 +40516,11 @@
         <v>5</v>
       </c>
       <c r="B19" s="1">
-        <f>IF(Kalkulationstool!D13="DVAG",3.5%*'Background WB vereinb'!C5,0)</f>
+        <f>IF(Kalkulationstool!D14="DVAG",3.5%*'Background WB vereinb'!C5,0)</f>
         <v>0</v>
       </c>
       <c r="C19" s="1">
-        <f>IF(Kalkulationstool!D13="DVAG",3.5%*'Background WB vereinb'!R5,0)</f>
+        <f>IF(Kalkulationstool!D14="DVAG",3.5%*'Background WB vereinb'!R5,0)</f>
         <v>0</v>
       </c>
       <c r="F19" s="1">
@@ -40489,11 +40588,11 @@
         <v>6</v>
       </c>
       <c r="B20" s="1">
-        <f>IF(Kalkulationstool!D13="Sonstige",3%*'Background WB vereinb'!C5,0)</f>
+        <f>IF(Kalkulationstool!D14="Sonstige",3%*'Background WB vereinb'!C5,0)</f>
         <v>0</v>
       </c>
       <c r="C20" s="1">
-        <f>IF(Kalkulationstool!D13="Sonstige",3%*'Background WB vereinb'!R5,0)</f>
+        <f>IF(Kalkulationstool!D14="Sonstige",3%*'Background WB vereinb'!R5,0)</f>
         <v>0</v>
       </c>
       <c r="F20" s="1">
@@ -47285,7 +47384,7 @@
   <sheetData>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F3" s="265" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G3" s="265"/>
       <c r="H3" s="265"/>
@@ -47297,7 +47396,7 @@
       <c r="N3" s="170"/>
       <c r="O3" s="170"/>
       <c r="U3" s="265" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V3" s="265"/>
       <c r="W3" s="265"/>
@@ -47309,29 +47408,29 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="266" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B4" s="266"/>
       <c r="C4" s="266"/>
       <c r="D4" s="266"/>
       <c r="E4" s="168"/>
       <c r="F4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>23</v>
@@ -47340,40 +47439,40 @@
         <v>23</v>
       </c>
       <c r="P4" s="266" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Q4" s="266"/>
       <c r="R4" s="266"/>
       <c r="S4" s="266"/>
       <c r="T4" s="168"/>
       <c r="U4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C5" s="119">
         <f>Kalkulationstool!D10</f>
@@ -47406,7 +47505,7 @@
       <c r="N5" s="171"/>
       <c r="O5" s="171"/>
       <c r="P5" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R5" s="119">
         <f>Wertbeitrag!C9</f>
@@ -47477,7 +47576,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R6" s="1">
         <f>Wertbeitrag!C11</f>
@@ -47517,7 +47616,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" s="79" t="e">
         <f>Background!P7</f>
@@ -47561,7 +47660,7 @@
       </c>
       <c r="O7" s="176"/>
       <c r="P7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R7" s="79">
         <f>Wertbeitrag!C10</f>
@@ -47606,7 +47705,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C8" s="79" t="e">
         <f>EFFECT(C7,12)</f>
@@ -47710,7 +47809,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R9" s="132" t="e">
         <f>-PMT(R7/12,R6,R5)</f>
@@ -47750,7 +47849,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="132" t="e">
         <f>-PMT(C7/12,C6,C5)</f>
@@ -47817,10 +47916,10 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="132">
-        <f>Kalkulationstool!D14</f>
+        <f>Kalkulationstool!D15</f>
         <v>0</v>
       </c>
       <c r="F11" s="1">
@@ -47880,7 +47979,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C12" s="218" t="e">
         <f>C7-(C11/10000)</f>
@@ -48185,7 +48284,7 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B17" s="149" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
@@ -48247,14 +48346,14 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B18" s="120">
-        <f>IF(Kalkulationstool!D13="MoVe",0.75,1)</f>
+        <f>IF(Kalkulationstool!D14="MoVe",0.75,1)</f>
         <v>1</v>
       </c>
       <c r="C18" s="120">
-        <f>IF(Kalkulationstool!D13="MoVe",0.75,1)</f>
+        <f>IF(Kalkulationstool!D14="MoVe",0.75,1)</f>
         <v>1</v>
       </c>
       <c r="F18" s="1">
@@ -48317,11 +48416,11 @@
         <v>5</v>
       </c>
       <c r="B19" s="1">
-        <f>IF(Kalkulationstool!D13="DVAG",3.5%*'Background Produktkalk I'!C5,0)</f>
+        <f>IF(Kalkulationstool!D14="DVAG",3.5%*'Background Produktkalk I'!C5,0)</f>
         <v>0</v>
       </c>
       <c r="C19" s="1">
-        <f>IF(Kalkulationstool!D13="DVAG",3.5%*'Background Produktkalk I'!R5,0)</f>
+        <f>IF(Kalkulationstool!D14="DVAG",3.5%*'Background Produktkalk I'!R5,0)</f>
         <v>0</v>
       </c>
       <c r="F19" s="1">
@@ -48384,11 +48483,11 @@
         <v>6</v>
       </c>
       <c r="B20" s="1">
-        <f>IF(Kalkulationstool!D13="Sonstige",3%*'Background Produktkalk I'!C5,0)</f>
+        <f>IF(Kalkulationstool!D14="Sonstige",3%*'Background Produktkalk I'!C5,0)</f>
         <v>0</v>
       </c>
       <c r="C20" s="1">
-        <f>IF(Kalkulationstool!D13="Sonstige",3%*'Background Produktkalk I'!R5,0)</f>
+        <f>IF(Kalkulationstool!D14="Sonstige",3%*'Background Produktkalk I'!R5,0)</f>
         <v>0</v>
       </c>
       <c r="F20" s="1">
@@ -55131,8 +55230,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AZ172"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55205,7 +55304,7 @@
       <c r="K2" s="25"/>
       <c r="L2" s="1"/>
       <c r="AA2" s="265" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AB2" s="265"/>
       <c r="AC2" s="265"/>
@@ -55213,7 +55312,7 @@
       <c r="AE2" s="265"/>
       <c r="AF2" s="265"/>
       <c r="AH2" s="265" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AI2" s="265"/>
       <c r="AJ2" s="265"/>
@@ -55225,7 +55324,7 @@
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
       <c r="AR2" s="265" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AS2" s="265"/>
       <c r="AT2" s="265"/>
@@ -55261,19 +55360,19 @@
       </c>
       <c r="L3" s="23"/>
       <c r="U3" s="266" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V3" s="266"/>
       <c r="W3" s="266"/>
       <c r="AB3" s="273" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AC3" s="273"/>
       <c r="AD3" s="273"/>
       <c r="AE3" s="108"/>
       <c r="AF3" s="108"/>
       <c r="AI3" s="273" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AJ3" s="273"/>
       <c r="AK3" s="273"/>
@@ -55283,7 +55382,7 @@
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
       <c r="AS3" s="273" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AT3" s="273"/>
       <c r="AU3" s="273"/>
@@ -55310,13 +55409,13 @@
         <v>8</v>
       </c>
       <c r="I4" s="22">
-        <v>9.69</v>
+        <v>10.19</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="8"/>
       <c r="L4" s="1"/>
       <c r="U4" s="109" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V4" s="110"/>
       <c r="W4" s="111">
@@ -55324,28 +55423,28 @@
         <v>0</v>
       </c>
       <c r="AB4" s="274" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AC4" s="274"/>
       <c r="AD4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI4" s="274" t="s">
         <v>90</v>
-      </c>
-      <c r="AI4" s="274" t="s">
-        <v>91</v>
       </c>
       <c r="AJ4" s="274"/>
       <c r="AK4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
       <c r="AR4" s="1"/>
       <c r="AS4" s="274" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AT4" s="274"/>
       <c r="AU4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
@@ -55371,7 +55470,7 @@
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="12">
-        <v>-1.3</v>
+        <v>-1.8</v>
       </c>
       <c r="L5" s="1"/>
       <c r="N5" s="5" t="s">
@@ -55443,7 +55542,7 @@
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="13">
-        <v>-1.1000000000000001</v>
+        <v>-1.5</v>
       </c>
       <c r="L6" s="120">
         <v>6</v>
@@ -55453,7 +55552,7 @@
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="78" t="e">
-        <f>IF((Background!$I$4+LOOKUP(Kalkulationstool!$D$7,Background!$I$5:$I$26,Background!$K$5:$K$26)+LOOKUP(Kalkulationstool!$D$10,Background!$I$38:$I$45,Background!$K$38:$K$45)+LOOKUP((Kalkulationstool!$D$11/Kalkulationstool!$D$10),Background!$I$27:$I$32,Background!$K$27:$K$32)+LOOKUP((Kalkulationstool!$D$12/Kalkulationstool!$D$10),Background!$I$33:$I$37,Background!$K$33:$K$37)+LOOKUP(Kalkulationstool!$D$8,Background!$I$48:$I$53,Background!$K$48:$K$53))&gt;Background!$K$60,Background!$K$60,IF((Background!$I$4+LOOKUP(Kalkulationstool!$D$7,Background!$I$5:$I$26,Background!$K$5:$K$26)+LOOKUP(Kalkulationstool!$D$10,Background!$I$38:$I$45,Background!$K$38:$K$45)+LOOKUP((Kalkulationstool!$D$11/Kalkulationstool!$D$10),Background!$I$27:$I$32,Background!$K$27:$K$32)+LOOKUP((Kalkulationstool!$D$12/Kalkulationstool!$D$10),Background!$I$33:$I$37,Background!$K$33:$K$37)+LOOKUP(Kalkulationstool!$D$8,Background!$I$48:$I$53,Background!$K$48:$K$53))&lt;Background!$K$61,Background!$K$61,Background!$I$4+LOOKUP(Kalkulationstool!$D$7,Background!$I$5:$I$26,Background!$K$5:$K$26)+LOOKUP(Kalkulationstool!$D$10,Background!$I$38:$I$45,Background!$K$38:$K$45)+LOOKUP((Kalkulationstool!$D$11/Kalkulationstool!$D$10),Background!$I$27:$I$32,Background!$K$27:$K$32)+LOOKUP((Kalkulationstool!$D$12/Kalkulationstool!$D$10),Background!$I$33:$I$37,Background!$K$33:$K$37)+LOOKUP(Kalkulationstool!$D$8,Background!$I$48:$I$53,Background!$K$48:$K$53)))/100</f>
+        <f>IF((Background!$I$4+LOOKUP(Kalkulationstool!$D$7,Background!$I$5:$I$26,Background!$K$5:$K$26)+LOOKUP(Kalkulationstool!$D$10,Background!$I$38:$I$45,Background!$K$38:$K$45)+LOOKUP((SUM(Kalkulationstool!$D$11,Kalkulationstool!$D$12)/Kalkulationstool!$D$10),Background!$I$27:$I$32,Background!$K$27:$K$32)+LOOKUP((Kalkulationstool!$D$13/Kalkulationstool!$D$10),Background!$I$33:$I$37,Background!$K$33:$K$37)+LOOKUP(Kalkulationstool!$D$8,Background!$I$48:$I$53,Background!$K$48:$K$53))&gt;Background!$K$60,Background!$K$60,IF((Background!$I$4+LOOKUP(Kalkulationstool!$D$7,Background!$I$5:$I$26,Background!$K$5:$K$26)+LOOKUP(Kalkulationstool!$D$10,Background!$I$38:$I$45,Background!$K$38:$K$45)+LOOKUP((SUM(Kalkulationstool!$D$11,Kalkulationstool!$D$12)/Kalkulationstool!$D$10),Background!$I$27:$I$32,Background!$K$27:$K$32)+LOOKUP((Kalkulationstool!$D$13/Kalkulationstool!$D$10),Background!$I$33:$I$37,Background!$K$33:$K$37)+LOOKUP(Kalkulationstool!$D$8,Background!$I$48:$I$53,Background!$K$48:$K$53))&lt;Background!$K$61,Background!$K$61,Background!$I$4+LOOKUP(Kalkulationstool!$D$7,Background!$I$5:$I$26,Background!$K$5:$K$26)+LOOKUP(Kalkulationstool!$D$10,Background!$I$38:$I$45,Background!$K$38:$K$45)+LOOKUP((SUM(Kalkulationstool!$D$11,Kalkulationstool!$D$12)/Kalkulationstool!$D$10),Background!$I$27:$I$32,Background!$K$27:$K$32)+LOOKUP((Kalkulationstool!$D$13/Kalkulationstool!$D$10),Background!$I$33:$I$37,Background!$K$33:$K$37)+LOOKUP(Kalkulationstool!$D$8,Background!$I$48:$I$53,Background!$K$48:$K$53)))/100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q6" s="75"/>
@@ -55461,7 +55560,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="112" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V6" s="29"/>
       <c r="W6" s="113">
@@ -55534,7 +55633,7 @@
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="13">
-        <v>-0.9</v>
+        <v>-1.2</v>
       </c>
       <c r="L7" s="120">
         <v>11</v>
@@ -55548,13 +55647,13 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q7" s="75" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="112" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V7" s="29"/>
       <c r="W7" s="115" t="e">
@@ -55630,7 +55729,7 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="13">
-        <v>-0.7</v>
+        <v>-0.8</v>
       </c>
       <c r="L8" s="120">
         <v>16</v>
@@ -55643,11 +55742,11 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="112" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V8" s="29"/>
       <c r="W8" s="113">
-        <f>Kalkulationstool!D14</f>
+        <f>Kalkulationstool!D15</f>
         <v>0</v>
       </c>
       <c r="AA8" s="1">
@@ -55719,7 +55818,7 @@
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="13">
-        <v>-0.5</v>
+        <v>-0.4</v>
       </c>
       <c r="L9" s="120">
         <v>21</v>
@@ -55808,7 +55907,7 @@
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="13">
-        <v>-0.3</v>
+        <v>-0.2</v>
       </c>
       <c r="L10" s="120">
         <v>31</v>
@@ -55821,7 +55920,7 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="112" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V10" s="29"/>
       <c r="W10" s="130" t="e">
@@ -55901,7 +56000,7 @@
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="13">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="120">
         <v>41</v>
@@ -55910,17 +56009,17 @@
         <v>22</v>
       </c>
       <c r="O11" s="202" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="P11" s="203" t="e">
-        <f ca="1">LOOKUP(Wertbeitrag(Kalkulationstool!D10,Kalkulationstool!D9,Kalkulationstool!D8,(((((Kalkulationstool!D20+1)^(1/12))-1)*12)),Kalkulationstool!D14/10000,Kalkulationstool!D7,PMT((((Kalkulationstool!D20+1)^(1/12)-1)),Kalkulationstool!D8,-Kalkulationstool!D10),IF(Kalkulationstool!D9-Kalkulationstool!D8&gt;3,1,0),Kalkulationstool!D13)/Kalkulationstool!D10,Background!I65:I70,Background!K65:K70)/100</f>
+        <f ca="1">LOOKUP(Wertbeitrag(Kalkulationstool!D10,Kalkulationstool!D9,Kalkulationstool!D8,(((((Kalkulationstool!D21+1)^(1/12))-1)*12)),Kalkulationstool!D15/10000,Kalkulationstool!D7,PMT((((Kalkulationstool!D21+1)^(1/12)-1)),Kalkulationstool!D8,-Kalkulationstool!D10),IF(Kalkulationstool!D9-Kalkulationstool!D8&gt;3,1,0),Kalkulationstool!D14)/Kalkulationstool!D10,Background!I65:I70,Background!K65:K70)/100</f>
         <v>#NAME?</v>
       </c>
       <c r="Q11" s="204"/>
       <c r="R11" s="202"/>
       <c r="S11" s="202"/>
       <c r="T11" s="205" t="e">
-        <f ca="1">LOOKUP(Wertbeitrag(Kalkulationstool!D10,Kalkulationstool!D9,Kalkulationstool!D8,(((((Kalkulationstool!D20+1)^(1/12))-1)*12)),Kalkulationstool!D14/10000,Kalkulationstool!D7,PMT((((Kalkulationstool!D20+1)^(1/12)-1)),Kalkulationstool!D8,-Kalkulationstool!D10),IF(Kalkulationstool!D9-Kalkulationstool!D8&gt;3,1,0),Kalkulationstool!D13)/Kalkulationstool!D10,Background!I65:I70,Background!L65:L70)/100</f>
+        <f ca="1">LOOKUP(Wertbeitrag(Kalkulationstool!D10,Kalkulationstool!D9,Kalkulationstool!D8,(((((Kalkulationstool!D21+1)^(1/12))-1)*12)),Kalkulationstool!D15/10000,Kalkulationstool!D7,PMT((((Kalkulationstool!D21+1)^(1/12)-1)),Kalkulationstool!D8,-Kalkulationstool!D10),IF(Kalkulationstool!D9-Kalkulationstool!D8&gt;3,1,0),Kalkulationstool!D14)/Kalkulationstool!D10,Background!I65:I70,Background!L65:L70)/100</f>
         <v>#NAME?</v>
       </c>
       <c r="U11" s="29" t="s">
@@ -55932,10 +56031,10 @@
         <v>0</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Y11" s="132" t="e">
-        <f>PMT((((Kalkulationstool!D20+1)^(1/12)-1)),Kalkulationstool!D8,-Kalkulationstool!D10)</f>
+        <f>PMT((((Kalkulationstool!D21+1)^(1/12)-1)),Kalkulationstool!D8,-Kalkulationstool!D10)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AA11" s="1">
@@ -56008,14 +56107,14 @@
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="13">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="L12" s="120">
         <v>51</v>
       </c>
       <c r="N12" s="278"/>
       <c r="O12" s="207" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="P12" s="208" t="str">
         <f>IF(ISNUMBER(P17),IF(Kalkulationstool!$D$8&gt;84,Background!P14,Background!P13),"")</f>
@@ -56033,7 +56132,7 @@
       </c>
       <c r="V12" s="116"/>
       <c r="W12" s="117" t="str">
-        <f>Kalkulationstool!D13</f>
+        <f>Kalkulationstool!D14</f>
         <v>-</v>
       </c>
       <c r="AA12" s="1">
@@ -56102,14 +56201,14 @@
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="13">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="L13" s="120">
         <v>61</v>
       </c>
       <c r="N13" s="278"/>
       <c r="O13" s="29" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="P13" s="210" t="e">
         <f>LOOKUP($P$17,Background!I65:I70,Background!K65:K70)/100</f>
@@ -56188,14 +56287,14 @@
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="13">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="L14" s="120">
         <v>71</v>
       </c>
       <c r="N14" s="279"/>
       <c r="O14" s="196" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="P14" s="206" t="e">
         <f>LOOKUP($P$17,Background!N65:N70,Background!O65:O70)/100</f>
@@ -56209,14 +56308,14 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V14" s="79" t="e">
         <f>W7-W8/10000</f>
         <v>#DIV/0!</v>
       </c>
       <c r="W14" s="118" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AA14" s="1">
         <v>9</v>
@@ -56285,27 +56384,27 @@
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="13">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="L15" s="120">
         <v>81</v>
       </c>
       <c r="N15" s="200" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O15" s="201" t="e">
-        <f ca="1">Wertbeitrag(Kalkulationstool!D10,Kalkulationstool!D9,Kalkulationstool!D8,(((((Kalkulationstool!D20+1)^(1/12))-1)*12)),Kalkulationstool!D14/10000,Kalkulationstool!D7,PMT((((Kalkulationstool!D20+1)^(1/12)-1)),Kalkulationstool!D8,-Kalkulationstool!D10),IF(Kalkulationstool!D9-Kalkulationstool!D8&gt;3,1,0),Kalkulationstool!D13)</f>
+        <f ca="1">Wertbeitrag(Kalkulationstool!D10,Kalkulationstool!D9,Kalkulationstool!D8,(((((Kalkulationstool!D21+1)^(1/12))-1)*12)),Kalkulationstool!D15/10000,Kalkulationstool!D7,PMT((((Kalkulationstool!D21+1)^(1/12)-1)),Kalkulationstool!D8,-Kalkulationstool!D10),IF(Kalkulationstool!D9-Kalkulationstool!D8&gt;3,1,0),Kalkulationstool!D14)</f>
         <v>#NAME?</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V15" s="119">
         <f>W4</f>
         <v>0</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AA15" s="1">
         <v>10</v>
@@ -56373,20 +56472,20 @@
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="13">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="L16" s="120">
         <v>91</v>
       </c>
       <c r="N16" s="105" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O16" s="106" t="e">
         <f ca="1">O15/Kalkulationstool!D10</f>
         <v>#NAME?</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="V16" s="119">
         <f>W5-W6</f>
@@ -56458,13 +56557,13 @@
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="13">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="L17" s="120">
         <v>101</v>
       </c>
       <c r="N17" s="143" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="O17" s="144" t="e">
         <f>IF(W11=1,AY27,AF27)</f>
@@ -56476,7 +56575,7 @@
       </c>
       <c r="Q17" s="79"/>
       <c r="U17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="V17" s="1">
         <f>V16*2+1</f>
@@ -56548,7 +56647,7 @@
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="13">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="L18" s="120">
         <v>126</v>
@@ -56559,14 +56658,14 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V18" s="133">
         <f>IF(W5-W6-W6/12&lt;0,1,W5-W6-W6/12)</f>
         <v>0</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AA18" s="1">
         <v>13</v>
@@ -56634,7 +56733,7 @@
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="13">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="L19" s="120">
         <v>151</v>
@@ -56714,13 +56813,13 @@
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="15">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="L20" s="120">
         <v>176</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="V20" s="1">
         <f>W6+V18+W6/12</f>
@@ -56751,7 +56850,7 @@
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="15">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="L21" s="120">
         <v>201</v>
@@ -56760,14 +56859,14 @@
       <c r="O21" s="144"/>
       <c r="P21" s="148"/>
       <c r="U21" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="V21" s="1">
         <f>W6+V16</f>
         <v>0</v>
       </c>
       <c r="AA21" s="274" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AB21" s="274"/>
       <c r="AC21" s="1">
@@ -56775,7 +56874,7 @@
         <v>0</v>
       </c>
       <c r="AH21" s="274" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AI21" s="274"/>
       <c r="AJ21" s="1">
@@ -56786,7 +56885,7 @@
       <c r="AP21" s="1"/>
       <c r="AQ21" s="1"/>
       <c r="AR21" s="274" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AS21" s="274"/>
       <c r="AT21" s="1">
@@ -56813,13 +56912,13 @@
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="15">
-        <v>2.1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L22" s="120">
         <v>251</v>
       </c>
       <c r="U22" s="134" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="V22" s="135">
         <f>IF(W5-W6&lt;5,W6-W6/12/2+2,IF(W5-W6&lt;8,W6-W6/12/2+1,(W6-W6/12/2)))</f>
@@ -56865,13 +56964,13 @@
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="15">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="L23" s="120">
         <v>301</v>
       </c>
       <c r="U23" s="136" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="V23" s="137" t="e">
         <f>AJ22+AP29</f>
@@ -56903,13 +57002,13 @@
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="15">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="L24" s="120">
         <v>351</v>
       </c>
       <c r="U24" s="136" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="V24" s="138" t="e">
         <f>V23-W5</f>
@@ -56934,20 +57033,20 @@
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="15">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="L25" s="120">
         <v>401</v>
       </c>
       <c r="U25" s="139" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="V25" s="140" t="e">
         <f>AZ29+AT22</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AA25" s="275" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AB25" s="275"/>
       <c r="AC25" s="275"/>
@@ -56955,7 +57054,7 @@
       <c r="AE25" s="275"/>
       <c r="AF25" s="275"/>
       <c r="AH25" s="276" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AI25" s="276"/>
       <c r="AJ25" s="276"/>
@@ -56967,7 +57066,7 @@
       <c r="AP25" s="1"/>
       <c r="AQ25" s="1"/>
       <c r="AR25" s="276" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AS25" s="276"/>
       <c r="AT25" s="276"/>
@@ -56988,23 +57087,23 @@
       </c>
       <c r="L26" s="120"/>
       <c r="U26" s="141" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="V26" s="142" t="e">
         <f>V25-W5</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AA26" s="128" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB26" s="128" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC26" s="128" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD26" s="128" t="s">
         <v>131</v>
-      </c>
-      <c r="AB26" s="128" t="s">
-        <v>132</v>
-      </c>
-      <c r="AC26" s="128" t="s">
-        <v>134</v>
-      </c>
-      <c r="AD26" s="128" t="s">
-        <v>133</v>
       </c>
       <c r="AE26" s="128" t="s">
         <v>23</v>
@@ -57075,14 +57174,14 @@
       </c>
       <c r="L28" s="1"/>
       <c r="AA28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AF28" s="120" t="e">
         <f>SUM(AF30:AF150)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AJ28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AO28" s="120" t="e">
         <f>SUM(AO30:AO163)</f>
@@ -57093,7 +57192,7 @@
       <c r="AR28" s="1"/>
       <c r="AS28" s="1"/>
       <c r="AT28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AU28" s="1"/>
       <c r="AV28" s="1"/>
@@ -57371,7 +57470,7 @@
       </c>
       <c r="L32" s="1"/>
       <c r="M32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AA32" s="1">
         <f t="shared" ref="AA32:AA95" si="17">1+AA31</f>
@@ -60437,7 +60536,7 @@
       </c>
       <c r="J60" s="18"/>
       <c r="K60" s="14">
-        <v>11.99</v>
+        <v>12.99</v>
       </c>
       <c r="L60" s="1"/>
       <c r="AA60" s="1">
@@ -60545,7 +60644,7 @@
       </c>
       <c r="J61" s="21"/>
       <c r="K61" s="16">
-        <v>3.99</v>
+        <v>4.49</v>
       </c>
       <c r="L61" s="1"/>
       <c r="AA61" s="1">
@@ -60752,14 +60851,14 @@
     </row>
     <row r="63" spans="8:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H63" s="24" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I63" s="24"/>
       <c r="J63" s="24"/>
       <c r="K63" s="24"/>
       <c r="L63" s="24"/>
       <c r="N63" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="AA63" s="1">
         <f t="shared" si="17"/>
@@ -70733,7 +70832,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -70766,7 +70865,7 @@
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="71" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C2" s="70"/>
       <c r="D2" s="70"/>
@@ -70785,7 +70884,7 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="220" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F4" s="67"/>
       <c r="G4" s="67"/>
@@ -70826,7 +70925,7 @@
       </c>
       <c r="G6" s="191"/>
       <c r="H6" s="192" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I6" s="82"/>
       <c r="J6" s="82"/>
@@ -70852,7 +70951,7 @@
       <c r="F7" s="123"/>
       <c r="G7" s="92"/>
       <c r="H7" s="93" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I7" s="82"/>
       <c r="J7" s="82"/>
@@ -70878,7 +70977,7 @@
       <c r="F8" s="92"/>
       <c r="G8" s="93"/>
       <c r="H8" s="93" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I8" s="82"/>
       <c r="J8" s="82"/>
@@ -70904,7 +71003,7 @@
       <c r="F9" s="92"/>
       <c r="G9" s="93"/>
       <c r="H9" s="93" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I9" s="82"/>
       <c r="J9" s="82"/>
@@ -70930,7 +71029,7 @@
       <c r="F10" s="94"/>
       <c r="G10" s="93"/>
       <c r="H10" s="93" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I10" s="82"/>
       <c r="J10" s="82"/>
@@ -70955,7 +71054,7 @@
       <c r="F11" s="94"/>
       <c r="G11" s="93"/>
       <c r="H11" s="93" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I11" s="82"/>
       <c r="J11" s="82"/>
@@ -70974,14 +71073,14 @@
       </c>
       <c r="C12" s="82"/>
       <c r="D12" s="224">
-        <f>Kalkulationstool!D12</f>
+        <f>Kalkulationstool!D13</f>
         <v>0</v>
       </c>
       <c r="E12" s="86"/>
       <c r="F12" s="94"/>
       <c r="G12" s="93"/>
       <c r="H12" s="93" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I12" s="82"/>
       <c r="J12" s="82"/>
@@ -71000,14 +71099,14 @@
       </c>
       <c r="C13" s="82"/>
       <c r="D13" s="223" t="str">
-        <f>Kalkulationstool!D13</f>
+        <f>Kalkulationstool!D14</f>
         <v>-</v>
       </c>
       <c r="E13" s="85"/>
       <c r="F13" s="92"/>
       <c r="G13" s="93"/>
       <c r="H13" s="93" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I13" s="82"/>
       <c r="J13" s="82"/>
@@ -71026,14 +71125,14 @@
       </c>
       <c r="C14" s="82"/>
       <c r="D14" s="225">
-        <f>Kalkulationstool!D14</f>
+        <f>Kalkulationstool!D15</f>
         <v>0</v>
       </c>
       <c r="E14" s="85"/>
       <c r="F14" s="92"/>
       <c r="G14" s="93"/>
       <c r="H14" s="93" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I14" s="82"/>
       <c r="J14" s="82"/>
@@ -71065,11 +71164,11 @@
       <c r="C19" s="82"/>
       <c r="D19" s="122">
         <f ca="1">NOW()</f>
-        <v>45125.744189004632</v>
+        <v>45182.664424074072</v>
       </c>
       <c r="E19" s="82"/>
       <c r="F19" s="82" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G19" s="82"/>
       <c r="H19" s="82"/>
@@ -71086,7 +71185,7 @@
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="82" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" s="82"/>
       <c r="D20" s="184" t="e">
@@ -71095,7 +71194,7 @@
       </c>
       <c r="E20" s="87"/>
       <c r="F20" s="100" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G20" s="82"/>
       <c r="H20" s="82"/>
@@ -71112,7 +71211,7 @@
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" s="82"/>
       <c r="D21" s="185" t="e">
@@ -71180,13 +71279,13 @@
       <c r="B24" s="82"/>
       <c r="C24" s="82"/>
       <c r="D24" s="261" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E24" s="262"/>
       <c r="F24" s="82"/>
       <c r="G24" s="82"/>
       <c r="H24" s="181" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I24" s="82"/>
       <c r="J24" s="82"/>
@@ -71235,7 +71334,7 @@
         <v/>
       </c>
       <c r="I26" s="91" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J26" s="82"/>
       <c r="K26" s="82"/>
@@ -71377,13 +71476,13 @@
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="71" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C2" s="70"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="220" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C3" s="70"/>
     </row>
@@ -71395,14 +71494,14 @@
         <v>52</v>
       </c>
       <c r="D4" s="195" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E4" s="97"/>
       <c r="F4" s="98"/>
     </row>
     <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="100" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C5" s="164" t="e">
         <f>MIN(Wertbeitrag!C5,D5)</f>
@@ -71414,12 +71513,12 @@
       </c>
       <c r="E5" s="92"/>
       <c r="F5" s="93" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="150" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C6" s="164" t="e">
         <f>IF(C5&gt;0,ROUND(NOMINAL(C5,12),4),"")</f>
@@ -71428,7 +71527,7 @@
       <c r="D6" s="151"/>
       <c r="E6" s="152"/>
       <c r="F6" s="93" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -71440,7 +71539,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="81" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C8" s="84"/>
       <c r="D8" s="193" t="s">
@@ -71451,35 +71550,35 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="100" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C9" s="163"/>
       <c r="D9" s="151"/>
       <c r="E9" s="93"/>
       <c r="F9" s="93" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="100" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C10" s="163"/>
       <c r="D10" s="146"/>
       <c r="E10" s="92"/>
       <c r="F10" s="93" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="100" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C11" s="163"/>
       <c r="D11" s="92"/>
       <c r="E11" s="92"/>
       <c r="F11" s="93" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -71491,7 +71590,7 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="155" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C13" s="189" t="str">
         <f>IF(ISNUMBER('Bg Produktkalk I_Kredit2'!B15),'Bg Produktkalk I_Kredit2'!B15,"")</f>
@@ -71503,7 +71602,7 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="155" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C14" s="190" t="str">
         <f>IF(ISNUMBER('Bg WB vereinb_Kredit2'!B15),'Bg WB vereinb_Kredit2'!B15,"")</f>
@@ -71533,7 +71632,7 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="160" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C17" s="154"/>
       <c r="D17" s="154"/>
@@ -71542,7 +71641,7 @@
     </row>
     <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D18" s="154"/>
       <c r="E18" s="154"/>
@@ -71550,7 +71649,7 @@
     </row>
     <row r="19" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D19" s="154"/>
       <c r="E19" s="154"/>
@@ -71558,7 +71657,7 @@
     </row>
     <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C20" s="154"/>
       <c r="D20" s="154"/>
@@ -71567,12 +71666,12 @@
     </row>
     <row r="21" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="147" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>